<commit_message>
completed one nsa request
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="458" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10EF7322-60D3-4B5E-B385-58011B08CD6D}"/>
+  <xr:revisionPtr revIDLastSave="464" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D1D4D72-6677-4945-B1C7-4684880E45A1}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8880" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
+    <workbookView xWindow="31515" yWindow="2700" windowWidth="17250" windowHeight="8865" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="OoredooMasterFile" sheetId="2" r:id="rId1"/>
@@ -2559,10 +2559,11 @@
     <t>MMS Officer</t>
   </si>
   <si>
-    <t>R-1</t>
-  </si>
-  <si>
-    <t>30-Jan-2023 @11:11 - Ooredoo Sim Requested with Plan C; Approved by HR Manager and DGM - Dan</t>
+    <t>50323690</t>
+  </si>
+  <si>
+    <t>30-Jan-2023 @11:11 - Ooredoo Sim Requested with Plan C; Approved by HR Manager and DGM - Dan
+01-Feb-2023 @10:01 - Request was Completed; Service Number is 50323690 with Plan C; Email Reference - SR: 12551064 SSR 12554312</t>
   </si>
 </sst>
 </file>
@@ -2708,7 +2709,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2784,12 +2785,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2940,7 +2935,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3294,10 +3289,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="14" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -15728,7 +15720,7 @@
       <c r="V323"/>
       <c r="W323"/>
     </row>
-    <row r="324" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A324" s="114">
         <v>44956</v>
       </c>
@@ -15738,7 +15730,9 @@
       <c r="C324" s="115" t="s">
         <v>76</v>
       </c>
-      <c r="D324" s="125"/>
+      <c r="D324" s="125" t="s">
+        <v>824</v>
+      </c>
       <c r="E324" s="115" t="s">
         <v>156</v>
       </c>
@@ -15760,8 +15754,8 @@
       <c r="K324" s="117" t="s">
         <v>589</v>
       </c>
-      <c r="L324" s="126" t="s">
-        <v>824</v>
+      <c r="L324" s="119">
+        <v>44958</v>
       </c>
       <c r="M324" s="120" t="s">
         <v>825</v>

</xml_diff>

<commit_message>
ooredoo event: activated 45 new sim cards
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="667" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C566F4B-AF42-4F1D-8DB9-5CA3ADED7B1E}"/>
+  <xr:revisionPtr revIDLastSave="1120" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A30C687-42B5-40A3-BEE0-FDB1FE413E3A}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1969" uniqueCount="853">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2239" uniqueCount="958">
   <si>
     <t>ICC ID</t>
   </si>
@@ -2652,6 +2652,321 @@
   <si>
     <t>RESIGNED
 05-Feb-2023 @11:38 - Cancellation of this Ooredoo Account and Service Number (Resigned) - Dan</t>
+  </si>
+  <si>
+    <t>8997401002188647416</t>
+  </si>
+  <si>
+    <t>R-13</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:35 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220200976</t>
+  </si>
+  <si>
+    <t>R-14</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:37 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220200984</t>
+  </si>
+  <si>
+    <t>R-15</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:38 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220200992</t>
+  </si>
+  <si>
+    <t>R-16</t>
+  </si>
+  <si>
+    <t>8997401002220201099</t>
+  </si>
+  <si>
+    <t>R-17</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:41 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201081</t>
+  </si>
+  <si>
+    <t>R-18</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:42 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201065</t>
+  </si>
+  <si>
+    <t>R-19</t>
+  </si>
+  <si>
+    <t>8997401002220201008</t>
+  </si>
+  <si>
+    <t>R-20</t>
+  </si>
+  <si>
+    <t>8997401002220201073</t>
+  </si>
+  <si>
+    <t>R-21</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:45 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201024</t>
+  </si>
+  <si>
+    <t>R-22</t>
+  </si>
+  <si>
+    <t>8997401002220201032</t>
+  </si>
+  <si>
+    <t>R-23</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:46 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201040</t>
+  </si>
+  <si>
+    <t>R-24</t>
+  </si>
+  <si>
+    <t>8997401002220201057</t>
+  </si>
+  <si>
+    <t>R-25</t>
+  </si>
+  <si>
+    <t>8997401002220201107</t>
+  </si>
+  <si>
+    <t>R-26</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:47 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201115</t>
+  </si>
+  <si>
+    <t>R-27</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:48 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201123</t>
+  </si>
+  <si>
+    <t>R-28</t>
+  </si>
+  <si>
+    <t>8997401002220201131</t>
+  </si>
+  <si>
+    <t>R-29</t>
+  </si>
+  <si>
+    <t>8997401002220201149</t>
+  </si>
+  <si>
+    <t>R-30</t>
+  </si>
+  <si>
+    <t>8997401002220201156</t>
+  </si>
+  <si>
+    <t>R-31</t>
+  </si>
+  <si>
+    <t>8997401002220201164</t>
+  </si>
+  <si>
+    <t>R-32</t>
+  </si>
+  <si>
+    <t>8997401002220201172</t>
+  </si>
+  <si>
+    <t>R-33</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:49 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201180</t>
+  </si>
+  <si>
+    <t>R-34</t>
+  </si>
+  <si>
+    <t>8997401002220201198</t>
+  </si>
+  <si>
+    <t>R-35</t>
+  </si>
+  <si>
+    <t>8997401002220201206</t>
+  </si>
+  <si>
+    <t>R-36</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:50 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201214</t>
+  </si>
+  <si>
+    <t>R-37</t>
+  </si>
+  <si>
+    <t>8997401002220201222</t>
+  </si>
+  <si>
+    <t>R-38</t>
+  </si>
+  <si>
+    <t>8997401002220201230</t>
+  </si>
+  <si>
+    <t>R-39</t>
+  </si>
+  <si>
+    <t>8997401002220201248</t>
+  </si>
+  <si>
+    <t>R-40</t>
+  </si>
+  <si>
+    <t>8997401002220201255</t>
+  </si>
+  <si>
+    <t>R-41</t>
+  </si>
+  <si>
+    <t>8997401002220201263</t>
+  </si>
+  <si>
+    <t>R-42</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:51 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201271</t>
+  </si>
+  <si>
+    <t>R-43</t>
+  </si>
+  <si>
+    <t>8997401002220201289</t>
+  </si>
+  <si>
+    <t>R-44</t>
+  </si>
+  <si>
+    <t>8997401002220201297</t>
+  </si>
+  <si>
+    <t>R-45</t>
+  </si>
+  <si>
+    <t>8997401002220201305</t>
+  </si>
+  <si>
+    <t>R-46</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:52 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201313</t>
+  </si>
+  <si>
+    <t>R-47</t>
+  </si>
+  <si>
+    <t>8997401002220201321</t>
+  </si>
+  <si>
+    <t>R-48</t>
+  </si>
+  <si>
+    <t>8997401002220201339</t>
+  </si>
+  <si>
+    <t>R-49</t>
+  </si>
+  <si>
+    <t>8997401002220201347</t>
+  </si>
+  <si>
+    <t>R-50</t>
+  </si>
+  <si>
+    <t>8997401002220201354</t>
+  </si>
+  <si>
+    <t>R-51</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:53 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201362</t>
+  </si>
+  <si>
+    <t>R-52</t>
+  </si>
+  <si>
+    <t>8997401002220201370</t>
+  </si>
+  <si>
+    <t>R-53</t>
+  </si>
+  <si>
+    <t>8997401002220201388</t>
+  </si>
+  <si>
+    <t>R-54</t>
+  </si>
+  <si>
+    <t>8997401002220201396</t>
+  </si>
+  <si>
+    <t>R-55</t>
+  </si>
+  <si>
+    <t>8997401002220201404</t>
+  </si>
+  <si>
+    <t>R-56</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:54 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201420</t>
+  </si>
+  <si>
+    <t>R-57</t>
   </si>
 </sst>
 </file>
@@ -3021,7 +3336,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3399,13 +3714,16 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="14" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4413,8 +4731,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}" name="OoredooActiveUsers" displayName="OoredooActiveUsers" ref="A2:M324" headerRowDxfId="17" totalsRowDxfId="14" headerRowBorderDxfId="16" tableBorderDxfId="15">
-  <autoFilter ref="A2:M324" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}" name="OoredooActiveUsers" displayName="OoredooActiveUsers" ref="A2:M369" headerRowDxfId="17" totalsRowDxfId="14" headerRowBorderDxfId="16" tableBorderDxfId="15">
+  <autoFilter ref="A2:M369" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:M324">
     <sortCondition ref="A2:A323"/>
   </sortState>
@@ -4745,13 +5063,13 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:W324"/>
+  <dimension ref="A1:W369"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E308" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E343" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A325" sqref="A325"/>
+      <selection pane="bottomRight" activeCell="A370" sqref="A370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15909,12 +16227,1227 @@
       <c r="J324" s="134" t="s">
         <v>851</v>
       </c>
-      <c r="K324" s="135"/>
+      <c r="K324" s="16"/>
       <c r="L324" s="130" t="s">
         <v>849</v>
       </c>
       <c r="M324" s="129" t="s">
         <v>852</v>
+      </c>
+    </row>
+    <row r="325" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A325" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B325" s="109" t="s">
+        <v>853</v>
+      </c>
+      <c r="C325" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D325" s="135"/>
+      <c r="E325" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F325" s="110">
+        <v>90</v>
+      </c>
+      <c r="G325" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L325" s="136" t="s">
+        <v>854</v>
+      </c>
+      <c r="M325" s="114" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="326" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A326" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B326" s="109" t="s">
+        <v>856</v>
+      </c>
+      <c r="C326" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D326" s="135"/>
+      <c r="E326" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F326" s="110">
+        <v>90</v>
+      </c>
+      <c r="G326" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L326" s="136" t="s">
+        <v>857</v>
+      </c>
+      <c r="M326" s="114" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="327" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A327" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B327" s="109" t="s">
+        <v>859</v>
+      </c>
+      <c r="C327" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D327" s="135"/>
+      <c r="E327" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F327" s="110">
+        <v>90</v>
+      </c>
+      <c r="G327" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L327" s="136" t="s">
+        <v>860</v>
+      </c>
+      <c r="M327" s="114" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="328" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A328" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B328" s="109" t="s">
+        <v>862</v>
+      </c>
+      <c r="C328" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D328" s="135"/>
+      <c r="E328" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F328" s="110">
+        <v>90</v>
+      </c>
+      <c r="G328" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L328" s="136" t="s">
+        <v>863</v>
+      </c>
+      <c r="M328" s="114" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="329" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A329" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B329" s="109" t="s">
+        <v>864</v>
+      </c>
+      <c r="C329" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D329" s="135"/>
+      <c r="E329" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F329" s="110">
+        <v>90</v>
+      </c>
+      <c r="G329" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L329" s="136" t="s">
+        <v>865</v>
+      </c>
+      <c r="M329" s="114" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="330" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A330" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B330" s="109" t="s">
+        <v>867</v>
+      </c>
+      <c r="C330" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D330" s="135"/>
+      <c r="E330" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F330" s="110">
+        <v>90</v>
+      </c>
+      <c r="G330" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L330" s="136" t="s">
+        <v>868</v>
+      </c>
+      <c r="M330" s="114" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="331" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A331" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B331" s="109" t="s">
+        <v>870</v>
+      </c>
+      <c r="C331" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D331" s="135"/>
+      <c r="E331" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F331" s="110">
+        <v>90</v>
+      </c>
+      <c r="G331" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L331" s="136" t="s">
+        <v>871</v>
+      </c>
+      <c r="M331" s="114" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="332" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A332" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B332" s="109" t="s">
+        <v>872</v>
+      </c>
+      <c r="C332" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D332" s="135"/>
+      <c r="E332" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F332" s="110">
+        <v>90</v>
+      </c>
+      <c r="G332" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L332" s="136" t="s">
+        <v>873</v>
+      </c>
+      <c r="M332" s="114" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="333" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A333" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B333" s="109" t="s">
+        <v>874</v>
+      </c>
+      <c r="C333" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D333" s="135"/>
+      <c r="E333" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F333" s="110">
+        <v>90</v>
+      </c>
+      <c r="G333" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L333" s="136" t="s">
+        <v>875</v>
+      </c>
+      <c r="M333" s="114" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="334" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A334" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B334" s="109" t="s">
+        <v>877</v>
+      </c>
+      <c r="C334" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D334" s="135"/>
+      <c r="E334" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F334" s="110">
+        <v>90</v>
+      </c>
+      <c r="G334" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L334" s="136" t="s">
+        <v>878</v>
+      </c>
+      <c r="M334" s="114" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="335" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A335" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B335" s="109" t="s">
+        <v>879</v>
+      </c>
+      <c r="C335" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D335" s="135"/>
+      <c r="E335" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F335" s="110">
+        <v>90</v>
+      </c>
+      <c r="G335" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L335" s="136" t="s">
+        <v>880</v>
+      </c>
+      <c r="M335" s="114" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="336" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A336" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B336" s="109" t="s">
+        <v>882</v>
+      </c>
+      <c r="C336" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D336" s="135"/>
+      <c r="E336" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F336" s="110">
+        <v>90</v>
+      </c>
+      <c r="G336" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L336" s="136" t="s">
+        <v>883</v>
+      </c>
+      <c r="M336" s="114" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="337" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A337" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B337" s="109" t="s">
+        <v>884</v>
+      </c>
+      <c r="C337" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D337" s="135"/>
+      <c r="E337" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F337" s="110">
+        <v>90</v>
+      </c>
+      <c r="G337" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L337" s="136" t="s">
+        <v>885</v>
+      </c>
+      <c r="M337" s="114" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="338" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A338" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B338" s="109" t="s">
+        <v>886</v>
+      </c>
+      <c r="C338" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D338" s="135"/>
+      <c r="E338" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F338" s="110">
+        <v>90</v>
+      </c>
+      <c r="G338" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L338" s="136" t="s">
+        <v>887</v>
+      </c>
+      <c r="M338" s="114" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="339" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A339" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B339" s="109" t="s">
+        <v>889</v>
+      </c>
+      <c r="C339" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D339" s="135"/>
+      <c r="E339" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F339" s="110">
+        <v>90</v>
+      </c>
+      <c r="G339" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L339" s="136" t="s">
+        <v>890</v>
+      </c>
+      <c r="M339" s="114" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="340" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A340" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B340" s="109" t="s">
+        <v>892</v>
+      </c>
+      <c r="C340" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D340" s="135"/>
+      <c r="E340" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F340" s="110">
+        <v>90</v>
+      </c>
+      <c r="G340" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L340" s="136" t="s">
+        <v>893</v>
+      </c>
+      <c r="M340" s="114" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="341" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A341" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B341" s="109" t="s">
+        <v>894</v>
+      </c>
+      <c r="C341" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D341" s="135"/>
+      <c r="E341" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F341" s="110">
+        <v>90</v>
+      </c>
+      <c r="G341" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L341" s="136" t="s">
+        <v>895</v>
+      </c>
+      <c r="M341" s="114" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="342" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A342" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B342" s="109" t="s">
+        <v>896</v>
+      </c>
+      <c r="C342" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D342" s="135"/>
+      <c r="E342" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F342" s="110">
+        <v>90</v>
+      </c>
+      <c r="G342" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L342" s="136" t="s">
+        <v>897</v>
+      </c>
+      <c r="M342" s="114" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="343" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A343" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B343" s="109" t="s">
+        <v>898</v>
+      </c>
+      <c r="C343" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D343" s="135"/>
+      <c r="E343" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F343" s="110">
+        <v>90</v>
+      </c>
+      <c r="G343" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L343" s="136" t="s">
+        <v>899</v>
+      </c>
+      <c r="M343" s="114" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="344" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A344" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B344" s="109" t="s">
+        <v>900</v>
+      </c>
+      <c r="C344" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D344" s="135"/>
+      <c r="E344" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F344" s="110">
+        <v>90</v>
+      </c>
+      <c r="G344" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L344" s="136" t="s">
+        <v>901</v>
+      </c>
+      <c r="M344" s="114" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="345" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A345" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B345" s="109" t="s">
+        <v>902</v>
+      </c>
+      <c r="C345" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D345" s="135"/>
+      <c r="E345" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F345" s="110">
+        <v>90</v>
+      </c>
+      <c r="G345" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L345" s="136" t="s">
+        <v>903</v>
+      </c>
+      <c r="M345" s="114" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="346" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A346" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B346" s="109" t="s">
+        <v>905</v>
+      </c>
+      <c r="C346" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D346" s="135"/>
+      <c r="E346" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F346" s="110">
+        <v>90</v>
+      </c>
+      <c r="G346" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L346" s="136" t="s">
+        <v>906</v>
+      </c>
+      <c r="M346" s="114" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="347" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A347" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B347" s="109" t="s">
+        <v>907</v>
+      </c>
+      <c r="C347" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D347" s="135"/>
+      <c r="E347" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F347" s="110">
+        <v>90</v>
+      </c>
+      <c r="G347" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L347" s="136" t="s">
+        <v>908</v>
+      </c>
+      <c r="M347" s="114" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="348" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A348" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B348" s="109" t="s">
+        <v>909</v>
+      </c>
+      <c r="C348" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D348" s="135"/>
+      <c r="E348" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F348" s="110">
+        <v>90</v>
+      </c>
+      <c r="G348" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L348" s="136" t="s">
+        <v>910</v>
+      </c>
+      <c r="M348" s="114" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="349" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A349" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B349" s="109" t="s">
+        <v>912</v>
+      </c>
+      <c r="C349" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D349" s="135"/>
+      <c r="E349" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F349" s="110">
+        <v>90</v>
+      </c>
+      <c r="G349" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L349" s="136" t="s">
+        <v>913</v>
+      </c>
+      <c r="M349" s="114" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="350" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A350" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B350" s="109" t="s">
+        <v>914</v>
+      </c>
+      <c r="C350" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D350" s="135"/>
+      <c r="E350" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F350" s="110">
+        <v>90</v>
+      </c>
+      <c r="G350" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L350" s="136" t="s">
+        <v>915</v>
+      </c>
+      <c r="M350" s="114" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="351" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A351" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B351" s="109" t="s">
+        <v>916</v>
+      </c>
+      <c r="C351" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D351" s="135"/>
+      <c r="E351" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F351" s="110">
+        <v>90</v>
+      </c>
+      <c r="G351" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L351" s="136" t="s">
+        <v>917</v>
+      </c>
+      <c r="M351" s="114" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="352" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A352" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B352" s="109" t="s">
+        <v>918</v>
+      </c>
+      <c r="C352" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D352" s="135"/>
+      <c r="E352" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F352" s="110">
+        <v>90</v>
+      </c>
+      <c r="G352" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L352" s="136" t="s">
+        <v>919</v>
+      </c>
+      <c r="M352" s="114" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="353" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A353" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B353" s="109" t="s">
+        <v>920</v>
+      </c>
+      <c r="C353" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D353" s="135"/>
+      <c r="E353" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F353" s="110">
+        <v>90</v>
+      </c>
+      <c r="G353" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L353" s="136" t="s">
+        <v>921</v>
+      </c>
+      <c r="M353" s="114" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="354" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A354" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B354" s="109" t="s">
+        <v>922</v>
+      </c>
+      <c r="C354" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D354" s="135"/>
+      <c r="E354" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F354" s="110">
+        <v>90</v>
+      </c>
+      <c r="G354" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L354" s="136" t="s">
+        <v>923</v>
+      </c>
+      <c r="M354" s="114" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="355" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A355" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B355" s="109" t="s">
+        <v>925</v>
+      </c>
+      <c r="C355" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D355" s="135"/>
+      <c r="E355" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F355" s="110">
+        <v>90</v>
+      </c>
+      <c r="G355" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L355" s="136" t="s">
+        <v>926</v>
+      </c>
+      <c r="M355" s="114" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="356" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A356" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B356" s="109" t="s">
+        <v>927</v>
+      </c>
+      <c r="C356" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D356" s="135"/>
+      <c r="E356" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F356" s="110">
+        <v>90</v>
+      </c>
+      <c r="G356" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L356" s="136" t="s">
+        <v>928</v>
+      </c>
+      <c r="M356" s="114" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="357" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A357" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B357" s="109" t="s">
+        <v>929</v>
+      </c>
+      <c r="C357" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D357" s="135"/>
+      <c r="E357" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F357" s="110">
+        <v>90</v>
+      </c>
+      <c r="G357" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L357" s="136" t="s">
+        <v>930</v>
+      </c>
+      <c r="M357" s="114" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="358" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A358" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B358" s="109" t="s">
+        <v>931</v>
+      </c>
+      <c r="C358" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D358" s="135"/>
+      <c r="E358" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F358" s="110">
+        <v>90</v>
+      </c>
+      <c r="G358" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L358" s="136" t="s">
+        <v>932</v>
+      </c>
+      <c r="M358" s="114" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="359" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A359" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B359" s="109" t="s">
+        <v>934</v>
+      </c>
+      <c r="C359" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D359" s="135"/>
+      <c r="E359" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F359" s="110">
+        <v>90</v>
+      </c>
+      <c r="G359" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L359" s="136" t="s">
+        <v>935</v>
+      </c>
+      <c r="M359" s="114" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="360" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A360" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B360" s="109" t="s">
+        <v>936</v>
+      </c>
+      <c r="C360" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D360" s="135"/>
+      <c r="E360" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F360" s="110">
+        <v>90</v>
+      </c>
+      <c r="G360" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L360" s="136" t="s">
+        <v>937</v>
+      </c>
+      <c r="M360" s="114" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="361" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A361" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B361" s="109" t="s">
+        <v>938</v>
+      </c>
+      <c r="C361" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D361" s="135"/>
+      <c r="E361" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F361" s="110">
+        <v>90</v>
+      </c>
+      <c r="G361" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L361" s="136" t="s">
+        <v>939</v>
+      </c>
+      <c r="M361" s="114" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="362" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A362" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B362" s="109" t="s">
+        <v>940</v>
+      </c>
+      <c r="C362" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D362" s="135"/>
+      <c r="E362" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F362" s="110">
+        <v>90</v>
+      </c>
+      <c r="G362" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L362" s="136" t="s">
+        <v>941</v>
+      </c>
+      <c r="M362" s="114" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="363" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A363" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B363" s="109" t="s">
+        <v>942</v>
+      </c>
+      <c r="C363" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D363" s="135"/>
+      <c r="E363" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F363" s="110">
+        <v>90</v>
+      </c>
+      <c r="G363" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L363" s="136" t="s">
+        <v>943</v>
+      </c>
+      <c r="M363" s="114" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="364" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A364" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B364" s="109" t="s">
+        <v>945</v>
+      </c>
+      <c r="C364" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D364" s="135"/>
+      <c r="E364" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F364" s="110">
+        <v>90</v>
+      </c>
+      <c r="G364" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L364" s="136" t="s">
+        <v>946</v>
+      </c>
+      <c r="M364" s="114" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="365" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A365" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B365" s="109" t="s">
+        <v>947</v>
+      </c>
+      <c r="C365" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D365" s="135"/>
+      <c r="E365" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F365" s="110">
+        <v>90</v>
+      </c>
+      <c r="G365" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L365" s="136" t="s">
+        <v>948</v>
+      </c>
+      <c r="M365" s="114" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="366" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A366" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B366" s="109" t="s">
+        <v>949</v>
+      </c>
+      <c r="C366" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D366" s="135"/>
+      <c r="E366" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F366" s="110">
+        <v>90</v>
+      </c>
+      <c r="G366" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L366" s="136" t="s">
+        <v>950</v>
+      </c>
+      <c r="M366" s="114" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="367" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A367" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B367" s="109" t="s">
+        <v>951</v>
+      </c>
+      <c r="C367" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D367" s="135"/>
+      <c r="E367" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F367" s="110">
+        <v>90</v>
+      </c>
+      <c r="G367" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L367" s="136" t="s">
+        <v>952</v>
+      </c>
+      <c r="M367" s="114" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="368" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A368" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B368" s="109" t="s">
+        <v>953</v>
+      </c>
+      <c r="C368" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D368" s="135"/>
+      <c r="E368" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F368" s="110">
+        <v>90</v>
+      </c>
+      <c r="G368" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L368" s="136" t="s">
+        <v>954</v>
+      </c>
+      <c r="M368" s="114" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="369" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A369" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B369" s="109" t="s">
+        <v>956</v>
+      </c>
+      <c r="C369" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D369" s="135"/>
+      <c r="E369" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F369" s="110">
+        <v>90</v>
+      </c>
+      <c r="G369" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="L369" s="136" t="s">
+        <v>957</v>
+      </c>
+      <c r="M369" s="114" t="s">
+        <v>955</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ooredoo event: completed 11 + 1 pending requests
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1120" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A30C687-42B5-40A3-BEE0-FDB1FE413E3A}"/>
+  <xr:revisionPtr revIDLastSave="1177" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEF7A6D4-4C16-4DEC-9E21-5C603FF4A18F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="OoredooMasterFile" sheetId="2" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2239" uniqueCount="958">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2227" uniqueCount="946">
   <si>
     <t>ICC ID</t>
   </si>
@@ -2539,9 +2539,6 @@
 01-Feb-2023 @10:01 - Request was Completed; Service Number is 50323690 with Plan C; Email Reference - SR: 12551064 SSR 12554312</t>
   </si>
   <si>
-    <t>R-2</t>
-  </si>
-  <si>
     <t>Qatar University Station</t>
   </si>
   <si>
@@ -2551,422 +2548,401 @@
     <t>Civil SME</t>
   </si>
   <si>
-    <t>R-1</t>
-  </si>
-  <si>
     <t>MEP TECHNICAL SUPPORT OFFICER</t>
   </si>
   <si>
-    <t>R-3</t>
-  </si>
-  <si>
     <t>ACIFM Driver</t>
   </si>
   <si>
-    <t>R-4</t>
-  </si>
-  <si>
-    <t>R-5</t>
-  </si>
-  <si>
-    <t>R-6</t>
-  </si>
-  <si>
-    <t>R-7</t>
-  </si>
-  <si>
     <t>Bin Mahmoud Station</t>
   </si>
   <si>
-    <t>R-8</t>
-  </si>
-  <si>
-    <t>02-Feb-2023 @11:23 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS</t>
-  </si>
-  <si>
-    <t>02-Feb-2023 @11:38 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS</t>
-  </si>
-  <si>
-    <t>02-Feb-2023 @11:36 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS</t>
-  </si>
-  <si>
-    <t>02-Feb-2023 @11:30 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS</t>
-  </si>
-  <si>
-    <t>02-Feb-2023 @11:28 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS</t>
-  </si>
-  <si>
-    <t>Upgraded from Plan A to Plan D at December 12, 2022
-02-Feb-2023 @11:37 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS</t>
-  </si>
-  <si>
-    <t>Upgraded from Plan D to Plan F at July 18, 2022; Downgraded back from Plan F to Plan D on October 20, 2022 due to misinformation and misleading details
-02-Feb-2023 @11:37 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS</t>
-  </si>
-  <si>
-    <t>Previous plan A/Aamali 65
-02-Feb-2023 @11:34 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS</t>
-  </si>
-  <si>
     <t>Head Office</t>
   </si>
   <si>
     <t>ADMIN ASSISTANT / FOOD COORDINATOR</t>
   </si>
   <si>
-    <t>R-9</t>
-  </si>
-  <si>
-    <t>Upgraded from Plan C to Plan D at November 15, 2022
-02-Feb-2023 @11:47 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS</t>
-  </si>
-  <si>
     <t>ADMIN ASSISTANT - SOFT SERVICES</t>
   </si>
   <si>
-    <t>R-10</t>
+    <t>M1A</t>
+  </si>
+  <si>
+    <t>Cancelled (30138599)</t>
+  </si>
+  <si>
+    <t>Mechanical Engineer</t>
+  </si>
+  <si>
+    <t>8997401002188647416</t>
+  </si>
+  <si>
+    <t>R-13</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:35 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220200976</t>
+  </si>
+  <si>
+    <t>R-14</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:37 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220200984</t>
+  </si>
+  <si>
+    <t>R-15</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:38 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220200992</t>
+  </si>
+  <si>
+    <t>R-16</t>
+  </si>
+  <si>
+    <t>8997401002220201099</t>
+  </si>
+  <si>
+    <t>R-17</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:41 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201081</t>
+  </si>
+  <si>
+    <t>R-18</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:42 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201065</t>
+  </si>
+  <si>
+    <t>R-19</t>
+  </si>
+  <si>
+    <t>8997401002220201008</t>
+  </si>
+  <si>
+    <t>R-20</t>
+  </si>
+  <si>
+    <t>8997401002220201073</t>
+  </si>
+  <si>
+    <t>R-21</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:45 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201024</t>
+  </si>
+  <si>
+    <t>R-22</t>
+  </si>
+  <si>
+    <t>8997401002220201032</t>
+  </si>
+  <si>
+    <t>R-23</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:46 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201040</t>
+  </si>
+  <si>
+    <t>R-24</t>
+  </si>
+  <si>
+    <t>8997401002220201057</t>
+  </si>
+  <si>
+    <t>R-25</t>
+  </si>
+  <si>
+    <t>8997401002220201107</t>
+  </si>
+  <si>
+    <t>R-26</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:47 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201115</t>
+  </si>
+  <si>
+    <t>R-27</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:48 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201123</t>
+  </si>
+  <si>
+    <t>R-28</t>
+  </si>
+  <si>
+    <t>8997401002220201131</t>
+  </si>
+  <si>
+    <t>R-29</t>
+  </si>
+  <si>
+    <t>8997401002220201149</t>
+  </si>
+  <si>
+    <t>R-30</t>
+  </si>
+  <si>
+    <t>8997401002220201156</t>
+  </si>
+  <si>
+    <t>R-31</t>
+  </si>
+  <si>
+    <t>8997401002220201164</t>
+  </si>
+  <si>
+    <t>R-32</t>
+  </si>
+  <si>
+    <t>8997401002220201172</t>
+  </si>
+  <si>
+    <t>R-33</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:49 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201180</t>
+  </si>
+  <si>
+    <t>R-34</t>
+  </si>
+  <si>
+    <t>8997401002220201198</t>
+  </si>
+  <si>
+    <t>R-35</t>
+  </si>
+  <si>
+    <t>8997401002220201206</t>
+  </si>
+  <si>
+    <t>R-36</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:50 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201214</t>
+  </si>
+  <si>
+    <t>R-37</t>
+  </si>
+  <si>
+    <t>8997401002220201222</t>
+  </si>
+  <si>
+    <t>R-38</t>
+  </si>
+  <si>
+    <t>8997401002220201230</t>
+  </si>
+  <si>
+    <t>R-39</t>
+  </si>
+  <si>
+    <t>8997401002220201248</t>
+  </si>
+  <si>
+    <t>R-40</t>
+  </si>
+  <si>
+    <t>8997401002220201255</t>
+  </si>
+  <si>
+    <t>R-41</t>
+  </si>
+  <si>
+    <t>8997401002220201263</t>
+  </si>
+  <si>
+    <t>R-42</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:51 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201271</t>
+  </si>
+  <si>
+    <t>R-43</t>
+  </si>
+  <si>
+    <t>8997401002220201289</t>
+  </si>
+  <si>
+    <t>R-44</t>
+  </si>
+  <si>
+    <t>8997401002220201297</t>
+  </si>
+  <si>
+    <t>R-45</t>
+  </si>
+  <si>
+    <t>8997401002220201305</t>
+  </si>
+  <si>
+    <t>R-46</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:52 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201313</t>
+  </si>
+  <si>
+    <t>R-47</t>
+  </si>
+  <si>
+    <t>8997401002220201321</t>
+  </si>
+  <si>
+    <t>R-48</t>
+  </si>
+  <si>
+    <t>8997401002220201339</t>
+  </si>
+  <si>
+    <t>R-49</t>
+  </si>
+  <si>
+    <t>8997401002220201347</t>
+  </si>
+  <si>
+    <t>R-50</t>
+  </si>
+  <si>
+    <t>8997401002220201354</t>
+  </si>
+  <si>
+    <t>R-51</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:53 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201362</t>
+  </si>
+  <si>
+    <t>R-52</t>
+  </si>
+  <si>
+    <t>8997401002220201370</t>
+  </si>
+  <si>
+    <t>R-53</t>
+  </si>
+  <si>
+    <t>8997401002220201388</t>
+  </si>
+  <si>
+    <t>R-54</t>
+  </si>
+  <si>
+    <t>8997401002220201396</t>
+  </si>
+  <si>
+    <t>R-55</t>
+  </si>
+  <si>
+    <t>8997401002220201404</t>
+  </si>
+  <si>
+    <t>R-56</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:54 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
+  </si>
+  <si>
+    <t>8997401002220201420</t>
+  </si>
+  <si>
+    <t>R-57</t>
+  </si>
+  <si>
+    <t>PRF # 3197
+02-Feb-2023 @11:51 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS
+08-Feb-2023 @11:09 - Request was Completed with Plan D</t>
   </si>
   <si>
     <t>Upgraded from Plan A to Plan D at November 15, 2022
-02-Feb-2023 @11:49 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS</t>
-  </si>
-  <si>
-    <t>R-11</t>
-  </si>
-  <si>
-    <t>PRF # 3197
-02-Feb-2023 @11:51 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS</t>
-  </si>
-  <si>
-    <t>M1A</t>
-  </si>
-  <si>
-    <t>R-12</t>
-  </si>
-  <si>
-    <t>Cancelled (30138599)</t>
-  </si>
-  <si>
-    <t>Mechanical Engineer</t>
+02-Feb-2023 @11:49 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS
+08-Feb-2023 @11:12 - Request was Completed with Plan D</t>
+  </si>
+  <si>
+    <t>02-Feb-2023 @11:28 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS
+08-Feb-2023 @11:16 - Request was Completed with Plan F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02-Feb-2023 @11:23 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS
+08-Feb-2023 @11:28 - Request was Completed with Plan D; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">02-Feb-2023 @11:30 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS
+08-Feb-2023 @11:30 - Request was Completed with Plan F; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Previous plan A/Aamali 65
+02-Feb-2023 @11:34 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS
+08-Feb-2023 @11:30 - Request was Completed with Plan B; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">02-Feb-2023 @11:36 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS
+08-Feb-2023 @11:30 - Request was Completed with Plan D; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upgraded from Plan D to Plan F at July 18, 2022; Downgraded back from Plan F to Plan D on October 20, 2022 due to misinformation and misleading details
+02-Feb-2023 @11:37 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS
+08-Feb-2023 @11:30 - Request was Completed with Plan D; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upgraded from Plan A to Plan D at December 12, 2022
+02-Feb-2023 @11:37 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS
+08-Feb-2023 @11:30 - Request was Completed with Plan D; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">02-Feb-2023 @11:38 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS
+08-Feb-2023 @11:31 - Request was Completed with Plan D; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upgraded from Plan C to Plan D at November 15, 2022
+02-Feb-2023 @11:47 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS
+08-Feb-2023 @11:31 - Request was Completed with Plan D; </t>
   </si>
   <si>
     <t>RESIGNED
-05-Feb-2023 @11:38 - Cancellation of this Ooredoo Account and Service Number (Resigned) - Dan</t>
-  </si>
-  <si>
-    <t>8997401002188647416</t>
-  </si>
-  <si>
-    <t>R-13</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:35 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
-    <t>8997401002220200976</t>
-  </si>
-  <si>
-    <t>R-14</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:37 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
-    <t>8997401002220200984</t>
-  </si>
-  <si>
-    <t>R-15</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:38 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
-    <t>8997401002220200992</t>
-  </si>
-  <si>
-    <t>R-16</t>
-  </si>
-  <si>
-    <t>8997401002220201099</t>
-  </si>
-  <si>
-    <t>R-17</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:41 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
-    <t>8997401002220201081</t>
-  </si>
-  <si>
-    <t>R-18</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:42 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
-    <t>8997401002220201065</t>
-  </si>
-  <si>
-    <t>R-19</t>
-  </si>
-  <si>
-    <t>8997401002220201008</t>
-  </si>
-  <si>
-    <t>R-20</t>
-  </si>
-  <si>
-    <t>8997401002220201073</t>
-  </si>
-  <si>
-    <t>R-21</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:45 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
-    <t>8997401002220201024</t>
-  </si>
-  <si>
-    <t>R-22</t>
-  </si>
-  <si>
-    <t>8997401002220201032</t>
-  </si>
-  <si>
-    <t>R-23</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:46 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
-    <t>8997401002220201040</t>
-  </si>
-  <si>
-    <t>R-24</t>
-  </si>
-  <si>
-    <t>8997401002220201057</t>
-  </si>
-  <si>
-    <t>R-25</t>
-  </si>
-  <si>
-    <t>8997401002220201107</t>
-  </si>
-  <si>
-    <t>R-26</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:47 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
-    <t>8997401002220201115</t>
-  </si>
-  <si>
-    <t>R-27</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:48 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
-    <t>8997401002220201123</t>
-  </si>
-  <si>
-    <t>R-28</t>
-  </si>
-  <si>
-    <t>8997401002220201131</t>
-  </si>
-  <si>
-    <t>R-29</t>
-  </si>
-  <si>
-    <t>8997401002220201149</t>
-  </si>
-  <si>
-    <t>R-30</t>
-  </si>
-  <si>
-    <t>8997401002220201156</t>
-  </si>
-  <si>
-    <t>R-31</t>
-  </si>
-  <si>
-    <t>8997401002220201164</t>
-  </si>
-  <si>
-    <t>R-32</t>
-  </si>
-  <si>
-    <t>8997401002220201172</t>
-  </si>
-  <si>
-    <t>R-33</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:49 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
-    <t>8997401002220201180</t>
-  </si>
-  <si>
-    <t>R-34</t>
-  </si>
-  <si>
-    <t>8997401002220201198</t>
-  </si>
-  <si>
-    <t>R-35</t>
-  </si>
-  <si>
-    <t>8997401002220201206</t>
-  </si>
-  <si>
-    <t>R-36</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:50 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
-    <t>8997401002220201214</t>
-  </si>
-  <si>
-    <t>R-37</t>
-  </si>
-  <si>
-    <t>8997401002220201222</t>
-  </si>
-  <si>
-    <t>R-38</t>
-  </si>
-  <si>
-    <t>8997401002220201230</t>
-  </si>
-  <si>
-    <t>R-39</t>
-  </si>
-  <si>
-    <t>8997401002220201248</t>
-  </si>
-  <si>
-    <t>R-40</t>
-  </si>
-  <si>
-    <t>8997401002220201255</t>
-  </si>
-  <si>
-    <t>R-41</t>
-  </si>
-  <si>
-    <t>8997401002220201263</t>
-  </si>
-  <si>
-    <t>R-42</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:51 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
-    <t>8997401002220201271</t>
-  </si>
-  <si>
-    <t>R-43</t>
-  </si>
-  <si>
-    <t>8997401002220201289</t>
-  </si>
-  <si>
-    <t>R-44</t>
-  </si>
-  <si>
-    <t>8997401002220201297</t>
-  </si>
-  <si>
-    <t>R-45</t>
-  </si>
-  <si>
-    <t>8997401002220201305</t>
-  </si>
-  <si>
-    <t>R-46</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:52 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
-    <t>8997401002220201313</t>
-  </si>
-  <si>
-    <t>R-47</t>
-  </si>
-  <si>
-    <t>8997401002220201321</t>
-  </si>
-  <si>
-    <t>R-48</t>
-  </si>
-  <si>
-    <t>8997401002220201339</t>
-  </si>
-  <si>
-    <t>R-49</t>
-  </si>
-  <si>
-    <t>8997401002220201347</t>
-  </si>
-  <si>
-    <t>R-50</t>
-  </si>
-  <si>
-    <t>8997401002220201354</t>
-  </si>
-  <si>
-    <t>R-51</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:53 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
-    <t>8997401002220201362</t>
-  </si>
-  <si>
-    <t>R-52</t>
-  </si>
-  <si>
-    <t>8997401002220201370</t>
-  </si>
-  <si>
-    <t>R-53</t>
-  </si>
-  <si>
-    <t>8997401002220201388</t>
-  </si>
-  <si>
-    <t>R-54</t>
-  </si>
-  <si>
-    <t>8997401002220201396</t>
-  </si>
-  <si>
-    <t>R-55</t>
-  </si>
-  <si>
-    <t>8997401002220201404</t>
-  </si>
-  <si>
-    <t>R-56</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:54 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
-    <t>8997401002220201420</t>
-  </si>
-  <si>
-    <t>R-57</t>
+05-Feb-2023 @11:38 - Cancellation of this Ooredoo Account and Service Number (Resigned) - Dan
+08-Feb-2023 @11:35 - Request was Completed with Plan G; Successfully Cancelled</t>
   </si>
 </sst>
 </file>
@@ -3336,7 +3312,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3672,9 +3648,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3693,9 +3666,6 @@
     <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3704,9 +3674,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="14" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5066,10 +5033,10 @@
   <dimension ref="A1:W369"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E343" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="J352" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A370" sqref="A370"/>
+      <selection pane="bottomRight" activeCell="L370" sqref="L370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15659,43 +15626,43 @@
       <c r="W311" s="7"/>
     </row>
     <row r="312" spans="1:23" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A312" s="120">
+      <c r="A312" s="119">
         <v>44956</v>
       </c>
-      <c r="B312" s="121" t="s">
+      <c r="B312" s="120" t="s">
         <v>810</v>
       </c>
-      <c r="C312" s="121" t="s">
+      <c r="C312" s="120" t="s">
         <v>76</v>
       </c>
       <c r="D312" s="69" t="s">
         <v>815</v>
       </c>
-      <c r="E312" s="121" t="s">
+      <c r="E312" s="120" t="s">
         <v>155</v>
       </c>
-      <c r="F312" s="122">
+      <c r="F312" s="121">
         <v>90</v>
       </c>
-      <c r="G312" s="123" t="s">
+      <c r="G312" s="122" t="s">
         <v>811</v>
       </c>
-      <c r="H312" s="124" t="s">
+      <c r="H312" s="123" t="s">
         <v>812</v>
       </c>
-      <c r="I312" s="123" t="s">
+      <c r="I312" s="122" t="s">
         <v>813</v>
       </c>
-      <c r="J312" s="123" t="s">
+      <c r="J312" s="122" t="s">
         <v>814</v>
       </c>
-      <c r="K312" s="123" t="s">
+      <c r="K312" s="122" t="s">
         <v>585</v>
       </c>
-      <c r="L312" s="125">
+      <c r="L312" s="124">
         <v>44958</v>
       </c>
-      <c r="M312" s="127" t="s">
+      <c r="M312" s="125" t="s">
         <v>816</v>
       </c>
       <c r="N312"/>
@@ -15709,7 +15676,7 @@
       <c r="V312"/>
       <c r="W312"/>
     </row>
-    <row r="313" spans="1:23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A313" s="15">
         <v>44959</v>
       </c>
@@ -15743,14 +15710,14 @@
       <c r="K313" s="16" t="s">
         <v>602</v>
       </c>
-      <c r="L313" s="119" t="s">
-        <v>846</v>
+      <c r="L313" s="48">
+        <v>44965</v>
       </c>
       <c r="M313" s="99" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="314" spans="1:23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="314" spans="1:23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A314" s="38">
         <v>44959</v>
       </c>
@@ -15770,7 +15737,7 @@
         <v>110.5</v>
       </c>
       <c r="G314" s="39" t="s">
-        <v>839</v>
+        <v>823</v>
       </c>
       <c r="H314" s="45" t="s">
         <v>775</v>
@@ -15779,17 +15746,17 @@
         <v>370</v>
       </c>
       <c r="J314" s="39" t="s">
-        <v>840</v>
+        <v>824</v>
       </c>
       <c r="K314" s="16"/>
-      <c r="L314" s="119" t="s">
-        <v>841</v>
+      <c r="L314" s="48">
+        <v>44965</v>
       </c>
       <c r="M314" s="106" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="315" spans="1:23" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="315" spans="1:23" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A315" s="38">
         <v>44959</v>
       </c>
@@ -15809,7 +15776,7 @@
         <v>110.5</v>
       </c>
       <c r="G315" s="39" t="s">
-        <v>839</v>
+        <v>823</v>
       </c>
       <c r="H315" s="45" t="s">
         <v>149</v>
@@ -15818,14 +15785,14 @@
         <v>150</v>
       </c>
       <c r="J315" s="39" t="s">
-        <v>843</v>
+        <v>825</v>
       </c>
       <c r="K315" s="16"/>
-      <c r="L315" s="119" t="s">
-        <v>844</v>
+      <c r="L315" s="48">
+        <v>44965</v>
       </c>
       <c r="M315" s="106" t="s">
-        <v>845</v>
+        <v>935</v>
       </c>
       <c r="N315"/>
       <c r="O315"/>
@@ -15838,7 +15805,7 @@
       <c r="V315"/>
       <c r="W315"/>
     </row>
-    <row r="316" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:23" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A316" s="15">
         <v>44959</v>
       </c>
@@ -15858,21 +15825,21 @@
         <v>110.5</v>
       </c>
       <c r="G316" s="16" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H316" s="17" t="s">
         <v>88</v>
       </c>
       <c r="I316" s="16" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="J316" s="16"/>
       <c r="K316" s="16"/>
-      <c r="L316" s="119" t="s">
-        <v>817</v>
+      <c r="L316" s="48">
+        <v>44965</v>
       </c>
       <c r="M316" s="99" t="s">
-        <v>831</v>
+        <v>937</v>
       </c>
       <c r="N316"/>
       <c r="O316"/>
@@ -15885,7 +15852,7 @@
       <c r="V316"/>
       <c r="W316"/>
     </row>
-    <row r="317" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:23" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A317" s="15">
         <v>44959</v>
       </c>
@@ -15914,14 +15881,14 @@
         <v>203</v>
       </c>
       <c r="J317" s="16" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="K317" s="16"/>
-      <c r="L317" s="119" t="s">
-        <v>825</v>
+      <c r="L317" s="48">
+        <v>44965</v>
       </c>
       <c r="M317" s="99" t="s">
-        <v>838</v>
+        <v>939</v>
       </c>
       <c r="N317"/>
       <c r="O317"/>
@@ -15934,7 +15901,7 @@
       <c r="V317"/>
       <c r="W317"/>
     </row>
-    <row r="318" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:23" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A318" s="15">
         <v>44959</v>
       </c>
@@ -15960,15 +15927,15 @@
         <v>88</v>
       </c>
       <c r="I318" s="16" t="s">
-        <v>829</v>
+        <v>822</v>
       </c>
       <c r="J318" s="16"/>
       <c r="K318" s="16"/>
-      <c r="L318" s="119" t="s">
-        <v>830</v>
+      <c r="L318" s="48">
+        <v>44965</v>
       </c>
       <c r="M318" s="99" t="s">
-        <v>832</v>
+        <v>943</v>
       </c>
       <c r="N318"/>
       <c r="O318"/>
@@ -15981,7 +15948,7 @@
       <c r="V318"/>
       <c r="W318"/>
     </row>
-    <row r="319" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:23" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A319" s="15">
         <v>44959</v>
       </c>
@@ -16011,11 +15978,11 @@
       </c>
       <c r="J319" s="16"/>
       <c r="K319" s="16"/>
-      <c r="L319" s="119" t="s">
-        <v>826</v>
+      <c r="L319" s="48">
+        <v>44965</v>
       </c>
       <c r="M319" s="99" t="s">
-        <v>833</v>
+        <v>940</v>
       </c>
       <c r="N319"/>
       <c r="O319"/>
@@ -16028,7 +15995,7 @@
       <c r="V319"/>
       <c r="W319"/>
     </row>
-    <row r="320" spans="1:23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A320" s="15">
         <v>44959</v>
       </c>
@@ -16057,19 +16024,19 @@
         <v>532</v>
       </c>
       <c r="J320" s="16" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="K320" s="16" t="s">
-        <v>848</v>
-      </c>
-      <c r="L320" s="119" t="s">
-        <v>823</v>
+        <v>826</v>
+      </c>
+      <c r="L320" s="48">
+        <v>44965</v>
       </c>
       <c r="M320" s="99" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="321" spans="1:23" customFormat="1" x14ac:dyDescent="0.3">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="321" spans="1:23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A321" s="15">
         <v>44959</v>
       </c>
@@ -16098,19 +16065,19 @@
         <v>538</v>
       </c>
       <c r="J321" s="16" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="K321" s="16" t="s">
-        <v>848</v>
-      </c>
-      <c r="L321" s="119" t="s">
-        <v>821</v>
+        <v>826</v>
+      </c>
+      <c r="L321" s="48">
+        <v>44965</v>
       </c>
       <c r="M321" s="99" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="322" spans="1:23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="322" spans="1:23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A322" s="42">
         <v>44959</v>
       </c>
@@ -16140,14 +16107,14 @@
       </c>
       <c r="J322" s="43"/>
       <c r="K322" s="16"/>
-      <c r="L322" s="119" t="s">
-        <v>827</v>
+      <c r="L322" s="48">
+        <v>44965</v>
       </c>
       <c r="M322" s="107" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="323" spans="1:23" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="323" spans="1:23" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A323" s="46">
         <v>44959</v>
       </c>
@@ -16179,11 +16146,11 @@
         <v>88</v>
       </c>
       <c r="K323" s="16"/>
-      <c r="L323" s="126" t="s">
-        <v>828</v>
+      <c r="L323" s="46">
+        <v>44965</v>
       </c>
       <c r="M323" s="99" t="s">
-        <v>836</v>
+        <v>942</v>
       </c>
       <c r="N323"/>
       <c r="O323"/>
@@ -16196,43 +16163,43 @@
       <c r="V323"/>
       <c r="W323"/>
     </row>
-    <row r="324" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A324" s="128">
+    <row r="324" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A324" s="126">
         <v>44962</v>
       </c>
-      <c r="B324" s="131" t="s">
+      <c r="B324" s="128" t="s">
         <v>75</v>
       </c>
-      <c r="C324" s="131" t="s">
-        <v>76</v>
-      </c>
-      <c r="D324" s="133" t="s">
-        <v>850</v>
-      </c>
-      <c r="E324" s="131" t="s">
+      <c r="C324" s="128" t="s">
+        <v>76</v>
+      </c>
+      <c r="D324" s="130" t="s">
+        <v>827</v>
+      </c>
+      <c r="E324" s="128" t="s">
         <v>77</v>
       </c>
-      <c r="F324" s="132">
+      <c r="F324" s="129">
         <v>195</v>
       </c>
-      <c r="G324" s="134" t="s">
-        <v>839</v>
-      </c>
-      <c r="H324" s="133" t="s">
+      <c r="G324" s="131" t="s">
+        <v>823</v>
+      </c>
+      <c r="H324" s="130" t="s">
         <v>79</v>
       </c>
-      <c r="I324" s="134" t="s">
+      <c r="I324" s="131" t="s">
         <v>80</v>
       </c>
-      <c r="J324" s="134" t="s">
-        <v>851</v>
+      <c r="J324" s="131" t="s">
+        <v>828</v>
       </c>
       <c r="K324" s="16"/>
-      <c r="L324" s="130" t="s">
-        <v>849</v>
-      </c>
-      <c r="M324" s="129" t="s">
-        <v>852</v>
+      <c r="L324" s="113">
+        <v>44965</v>
+      </c>
+      <c r="M324" s="127" t="s">
+        <v>945</v>
       </c>
     </row>
     <row r="325" spans="1:23" x14ac:dyDescent="0.3">
@@ -16240,12 +16207,12 @@
         <v>44964</v>
       </c>
       <c r="B325" s="109" t="s">
-        <v>853</v>
+        <v>829</v>
       </c>
       <c r="C325" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D325" s="135"/>
+      <c r="D325" s="132"/>
       <c r="E325" s="109" t="s">
         <v>155</v>
       </c>
@@ -16255,11 +16222,11 @@
       <c r="G325" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L325" s="136" t="s">
-        <v>854</v>
+      <c r="L325" s="133" t="s">
+        <v>830</v>
       </c>
       <c r="M325" s="114" t="s">
-        <v>855</v>
+        <v>831</v>
       </c>
     </row>
     <row r="326" spans="1:23" x14ac:dyDescent="0.3">
@@ -16267,12 +16234,12 @@
         <v>44964</v>
       </c>
       <c r="B326" s="109" t="s">
-        <v>856</v>
+        <v>832</v>
       </c>
       <c r="C326" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D326" s="135"/>
+      <c r="D326" s="132"/>
       <c r="E326" s="109" t="s">
         <v>155</v>
       </c>
@@ -16282,11 +16249,11 @@
       <c r="G326" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L326" s="136" t="s">
-        <v>857</v>
+      <c r="L326" s="133" t="s">
+        <v>833</v>
       </c>
       <c r="M326" s="114" t="s">
-        <v>858</v>
+        <v>834</v>
       </c>
     </row>
     <row r="327" spans="1:23" x14ac:dyDescent="0.3">
@@ -16294,12 +16261,12 @@
         <v>44964</v>
       </c>
       <c r="B327" s="109" t="s">
-        <v>859</v>
+        <v>835</v>
       </c>
       <c r="C327" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D327" s="135"/>
+      <c r="D327" s="132"/>
       <c r="E327" s="109" t="s">
         <v>155</v>
       </c>
@@ -16309,11 +16276,11 @@
       <c r="G327" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L327" s="136" t="s">
-        <v>860</v>
+      <c r="L327" s="133" t="s">
+        <v>836</v>
       </c>
       <c r="M327" s="114" t="s">
-        <v>861</v>
+        <v>837</v>
       </c>
     </row>
     <row r="328" spans="1:23" x14ac:dyDescent="0.3">
@@ -16321,12 +16288,12 @@
         <v>44964</v>
       </c>
       <c r="B328" s="109" t="s">
-        <v>862</v>
+        <v>838</v>
       </c>
       <c r="C328" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D328" s="135"/>
+      <c r="D328" s="132"/>
       <c r="E328" s="109" t="s">
         <v>155</v>
       </c>
@@ -16336,11 +16303,11 @@
       <c r="G328" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L328" s="136" t="s">
-        <v>863</v>
+      <c r="L328" s="133" t="s">
+        <v>839</v>
       </c>
       <c r="M328" s="114" t="s">
-        <v>861</v>
+        <v>837</v>
       </c>
     </row>
     <row r="329" spans="1:23" x14ac:dyDescent="0.3">
@@ -16348,12 +16315,12 @@
         <v>44964</v>
       </c>
       <c r="B329" s="109" t="s">
-        <v>864</v>
+        <v>840</v>
       </c>
       <c r="C329" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D329" s="135"/>
+      <c r="D329" s="132"/>
       <c r="E329" s="109" t="s">
         <v>155</v>
       </c>
@@ -16363,11 +16330,11 @@
       <c r="G329" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L329" s="136" t="s">
-        <v>865</v>
+      <c r="L329" s="133" t="s">
+        <v>841</v>
       </c>
       <c r="M329" s="114" t="s">
-        <v>866</v>
+        <v>842</v>
       </c>
     </row>
     <row r="330" spans="1:23" x14ac:dyDescent="0.3">
@@ -16375,12 +16342,12 @@
         <v>44964</v>
       </c>
       <c r="B330" s="109" t="s">
-        <v>867</v>
+        <v>843</v>
       </c>
       <c r="C330" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D330" s="135"/>
+      <c r="D330" s="132"/>
       <c r="E330" s="109" t="s">
         <v>155</v>
       </c>
@@ -16390,11 +16357,11 @@
       <c r="G330" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L330" s="136" t="s">
-        <v>868</v>
+      <c r="L330" s="133" t="s">
+        <v>844</v>
       </c>
       <c r="M330" s="114" t="s">
-        <v>869</v>
+        <v>845</v>
       </c>
     </row>
     <row r="331" spans="1:23" x14ac:dyDescent="0.3">
@@ -16402,12 +16369,12 @@
         <v>44964</v>
       </c>
       <c r="B331" s="109" t="s">
-        <v>870</v>
+        <v>846</v>
       </c>
       <c r="C331" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D331" s="135"/>
+      <c r="D331" s="132"/>
       <c r="E331" s="109" t="s">
         <v>155</v>
       </c>
@@ -16417,11 +16384,11 @@
       <c r="G331" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L331" s="136" t="s">
-        <v>871</v>
+      <c r="L331" s="133" t="s">
+        <v>847</v>
       </c>
       <c r="M331" s="114" t="s">
-        <v>869</v>
+        <v>845</v>
       </c>
     </row>
     <row r="332" spans="1:23" x14ac:dyDescent="0.3">
@@ -16429,12 +16396,12 @@
         <v>44964</v>
       </c>
       <c r="B332" s="109" t="s">
-        <v>872</v>
+        <v>848</v>
       </c>
       <c r="C332" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D332" s="135"/>
+      <c r="D332" s="132"/>
       <c r="E332" s="109" t="s">
         <v>155</v>
       </c>
@@ -16444,11 +16411,11 @@
       <c r="G332" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L332" s="136" t="s">
-        <v>873</v>
+      <c r="L332" s="133" t="s">
+        <v>849</v>
       </c>
       <c r="M332" s="114" t="s">
-        <v>869</v>
+        <v>845</v>
       </c>
     </row>
     <row r="333" spans="1:23" x14ac:dyDescent="0.3">
@@ -16456,12 +16423,12 @@
         <v>44964</v>
       </c>
       <c r="B333" s="109" t="s">
-        <v>874</v>
+        <v>850</v>
       </c>
       <c r="C333" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D333" s="135"/>
+      <c r="D333" s="132"/>
       <c r="E333" s="109" t="s">
         <v>155</v>
       </c>
@@ -16471,11 +16438,11 @@
       <c r="G333" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L333" s="136" t="s">
-        <v>875</v>
+      <c r="L333" s="133" t="s">
+        <v>851</v>
       </c>
       <c r="M333" s="114" t="s">
-        <v>876</v>
+        <v>852</v>
       </c>
     </row>
     <row r="334" spans="1:23" x14ac:dyDescent="0.3">
@@ -16483,12 +16450,12 @@
         <v>44964</v>
       </c>
       <c r="B334" s="109" t="s">
-        <v>877</v>
+        <v>853</v>
       </c>
       <c r="C334" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D334" s="135"/>
+      <c r="D334" s="132"/>
       <c r="E334" s="109" t="s">
         <v>155</v>
       </c>
@@ -16498,11 +16465,11 @@
       <c r="G334" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L334" s="136" t="s">
-        <v>878</v>
+      <c r="L334" s="133" t="s">
+        <v>854</v>
       </c>
       <c r="M334" s="114" t="s">
-        <v>876</v>
+        <v>852</v>
       </c>
     </row>
     <row r="335" spans="1:23" x14ac:dyDescent="0.3">
@@ -16510,12 +16477,12 @@
         <v>44964</v>
       </c>
       <c r="B335" s="109" t="s">
-        <v>879</v>
+        <v>855</v>
       </c>
       <c r="C335" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D335" s="135"/>
+      <c r="D335" s="132"/>
       <c r="E335" s="109" t="s">
         <v>155</v>
       </c>
@@ -16525,11 +16492,11 @@
       <c r="G335" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L335" s="136" t="s">
-        <v>880</v>
+      <c r="L335" s="133" t="s">
+        <v>856</v>
       </c>
       <c r="M335" s="114" t="s">
-        <v>881</v>
+        <v>857</v>
       </c>
     </row>
     <row r="336" spans="1:23" x14ac:dyDescent="0.3">
@@ -16537,12 +16504,12 @@
         <v>44964</v>
       </c>
       <c r="B336" s="109" t="s">
-        <v>882</v>
+        <v>858</v>
       </c>
       <c r="C336" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D336" s="135"/>
+      <c r="D336" s="132"/>
       <c r="E336" s="109" t="s">
         <v>155</v>
       </c>
@@ -16552,11 +16519,11 @@
       <c r="G336" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L336" s="136" t="s">
-        <v>883</v>
+      <c r="L336" s="133" t="s">
+        <v>859</v>
       </c>
       <c r="M336" s="114" t="s">
-        <v>881</v>
+        <v>857</v>
       </c>
     </row>
     <row r="337" spans="1:13" x14ac:dyDescent="0.3">
@@ -16564,12 +16531,12 @@
         <v>44964</v>
       </c>
       <c r="B337" s="109" t="s">
-        <v>884</v>
+        <v>860</v>
       </c>
       <c r="C337" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D337" s="135"/>
+      <c r="D337" s="132"/>
       <c r="E337" s="109" t="s">
         <v>155</v>
       </c>
@@ -16579,11 +16546,11 @@
       <c r="G337" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L337" s="136" t="s">
-        <v>885</v>
+      <c r="L337" s="133" t="s">
+        <v>861</v>
       </c>
       <c r="M337" s="114" t="s">
-        <v>881</v>
+        <v>857</v>
       </c>
     </row>
     <row r="338" spans="1:13" x14ac:dyDescent="0.3">
@@ -16591,12 +16558,12 @@
         <v>44964</v>
       </c>
       <c r="B338" s="109" t="s">
-        <v>886</v>
+        <v>862</v>
       </c>
       <c r="C338" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D338" s="135"/>
+      <c r="D338" s="132"/>
       <c r="E338" s="109" t="s">
         <v>155</v>
       </c>
@@ -16606,11 +16573,11 @@
       <c r="G338" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L338" s="136" t="s">
-        <v>887</v>
+      <c r="L338" s="133" t="s">
+        <v>863</v>
       </c>
       <c r="M338" s="114" t="s">
-        <v>888</v>
+        <v>864</v>
       </c>
     </row>
     <row r="339" spans="1:13" x14ac:dyDescent="0.3">
@@ -16618,12 +16585,12 @@
         <v>44964</v>
       </c>
       <c r="B339" s="109" t="s">
-        <v>889</v>
+        <v>865</v>
       </c>
       <c r="C339" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D339" s="135"/>
+      <c r="D339" s="132"/>
       <c r="E339" s="109" t="s">
         <v>155</v>
       </c>
@@ -16633,11 +16600,11 @@
       <c r="G339" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L339" s="136" t="s">
-        <v>890</v>
+      <c r="L339" s="133" t="s">
+        <v>866</v>
       </c>
       <c r="M339" s="114" t="s">
-        <v>891</v>
+        <v>867</v>
       </c>
     </row>
     <row r="340" spans="1:13" x14ac:dyDescent="0.3">
@@ -16645,12 +16612,12 @@
         <v>44964</v>
       </c>
       <c r="B340" s="109" t="s">
-        <v>892</v>
+        <v>868</v>
       </c>
       <c r="C340" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D340" s="135"/>
+      <c r="D340" s="132"/>
       <c r="E340" s="109" t="s">
         <v>155</v>
       </c>
@@ -16660,11 +16627,11 @@
       <c r="G340" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L340" s="136" t="s">
-        <v>893</v>
+      <c r="L340" s="133" t="s">
+        <v>869</v>
       </c>
       <c r="M340" s="114" t="s">
-        <v>891</v>
+        <v>867</v>
       </c>
     </row>
     <row r="341" spans="1:13" x14ac:dyDescent="0.3">
@@ -16672,12 +16639,12 @@
         <v>44964</v>
       </c>
       <c r="B341" s="109" t="s">
-        <v>894</v>
+        <v>870</v>
       </c>
       <c r="C341" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D341" s="135"/>
+      <c r="D341" s="132"/>
       <c r="E341" s="109" t="s">
         <v>155</v>
       </c>
@@ -16687,11 +16654,11 @@
       <c r="G341" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L341" s="136" t="s">
-        <v>895</v>
+      <c r="L341" s="133" t="s">
+        <v>871</v>
       </c>
       <c r="M341" s="114" t="s">
-        <v>891</v>
+        <v>867</v>
       </c>
     </row>
     <row r="342" spans="1:13" x14ac:dyDescent="0.3">
@@ -16699,12 +16666,12 @@
         <v>44964</v>
       </c>
       <c r="B342" s="109" t="s">
-        <v>896</v>
+        <v>872</v>
       </c>
       <c r="C342" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D342" s="135"/>
+      <c r="D342" s="132"/>
       <c r="E342" s="109" t="s">
         <v>155</v>
       </c>
@@ -16714,11 +16681,11 @@
       <c r="G342" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L342" s="136" t="s">
-        <v>897</v>
+      <c r="L342" s="133" t="s">
+        <v>873</v>
       </c>
       <c r="M342" s="114" t="s">
-        <v>891</v>
+        <v>867</v>
       </c>
     </row>
     <row r="343" spans="1:13" x14ac:dyDescent="0.3">
@@ -16726,12 +16693,12 @@
         <v>44964</v>
       </c>
       <c r="B343" s="109" t="s">
-        <v>898</v>
+        <v>874</v>
       </c>
       <c r="C343" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D343" s="135"/>
+      <c r="D343" s="132"/>
       <c r="E343" s="109" t="s">
         <v>155</v>
       </c>
@@ -16741,11 +16708,11 @@
       <c r="G343" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L343" s="136" t="s">
-        <v>899</v>
+      <c r="L343" s="133" t="s">
+        <v>875</v>
       </c>
       <c r="M343" s="114" t="s">
-        <v>891</v>
+        <v>867</v>
       </c>
     </row>
     <row r="344" spans="1:13" x14ac:dyDescent="0.3">
@@ -16753,12 +16720,12 @@
         <v>44964</v>
       </c>
       <c r="B344" s="109" t="s">
-        <v>900</v>
+        <v>876</v>
       </c>
       <c r="C344" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D344" s="135"/>
+      <c r="D344" s="132"/>
       <c r="E344" s="109" t="s">
         <v>155</v>
       </c>
@@ -16768,11 +16735,11 @@
       <c r="G344" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L344" s="136" t="s">
-        <v>901</v>
+      <c r="L344" s="133" t="s">
+        <v>877</v>
       </c>
       <c r="M344" s="114" t="s">
-        <v>891</v>
+        <v>867</v>
       </c>
     </row>
     <row r="345" spans="1:13" x14ac:dyDescent="0.3">
@@ -16780,12 +16747,12 @@
         <v>44964</v>
       </c>
       <c r="B345" s="109" t="s">
-        <v>902</v>
+        <v>878</v>
       </c>
       <c r="C345" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D345" s="135"/>
+      <c r="D345" s="132"/>
       <c r="E345" s="109" t="s">
         <v>155</v>
       </c>
@@ -16795,11 +16762,11 @@
       <c r="G345" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L345" s="136" t="s">
-        <v>903</v>
+      <c r="L345" s="133" t="s">
+        <v>879</v>
       </c>
       <c r="M345" s="114" t="s">
-        <v>904</v>
+        <v>880</v>
       </c>
     </row>
     <row r="346" spans="1:13" x14ac:dyDescent="0.3">
@@ -16807,12 +16774,12 @@
         <v>44964</v>
       </c>
       <c r="B346" s="109" t="s">
-        <v>905</v>
+        <v>881</v>
       </c>
       <c r="C346" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D346" s="135"/>
+      <c r="D346" s="132"/>
       <c r="E346" s="109" t="s">
         <v>155</v>
       </c>
@@ -16822,11 +16789,11 @@
       <c r="G346" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L346" s="136" t="s">
-        <v>906</v>
+      <c r="L346" s="133" t="s">
+        <v>882</v>
       </c>
       <c r="M346" s="114" t="s">
-        <v>904</v>
+        <v>880</v>
       </c>
     </row>
     <row r="347" spans="1:13" x14ac:dyDescent="0.3">
@@ -16834,12 +16801,12 @@
         <v>44964</v>
       </c>
       <c r="B347" s="109" t="s">
-        <v>907</v>
+        <v>883</v>
       </c>
       <c r="C347" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D347" s="135"/>
+      <c r="D347" s="132"/>
       <c r="E347" s="109" t="s">
         <v>155</v>
       </c>
@@ -16849,11 +16816,11 @@
       <c r="G347" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L347" s="136" t="s">
-        <v>908</v>
+      <c r="L347" s="133" t="s">
+        <v>884</v>
       </c>
       <c r="M347" s="114" t="s">
-        <v>904</v>
+        <v>880</v>
       </c>
     </row>
     <row r="348" spans="1:13" x14ac:dyDescent="0.3">
@@ -16861,12 +16828,12 @@
         <v>44964</v>
       </c>
       <c r="B348" s="109" t="s">
-        <v>909</v>
+        <v>885</v>
       </c>
       <c r="C348" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D348" s="135"/>
+      <c r="D348" s="132"/>
       <c r="E348" s="109" t="s">
         <v>155</v>
       </c>
@@ -16876,11 +16843,11 @@
       <c r="G348" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L348" s="136" t="s">
-        <v>910</v>
+      <c r="L348" s="133" t="s">
+        <v>886</v>
       </c>
       <c r="M348" s="114" t="s">
-        <v>911</v>
+        <v>887</v>
       </c>
     </row>
     <row r="349" spans="1:13" x14ac:dyDescent="0.3">
@@ -16888,12 +16855,12 @@
         <v>44964</v>
       </c>
       <c r="B349" s="109" t="s">
-        <v>912</v>
+        <v>888</v>
       </c>
       <c r="C349" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D349" s="135"/>
+      <c r="D349" s="132"/>
       <c r="E349" s="109" t="s">
         <v>155</v>
       </c>
@@ -16903,11 +16870,11 @@
       <c r="G349" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L349" s="136" t="s">
-        <v>913</v>
+      <c r="L349" s="133" t="s">
+        <v>889</v>
       </c>
       <c r="M349" s="114" t="s">
-        <v>911</v>
+        <v>887</v>
       </c>
     </row>
     <row r="350" spans="1:13" x14ac:dyDescent="0.3">
@@ -16915,12 +16882,12 @@
         <v>44964</v>
       </c>
       <c r="B350" s="109" t="s">
-        <v>914</v>
+        <v>890</v>
       </c>
       <c r="C350" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D350" s="135"/>
+      <c r="D350" s="132"/>
       <c r="E350" s="109" t="s">
         <v>155</v>
       </c>
@@ -16930,11 +16897,11 @@
       <c r="G350" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L350" s="136" t="s">
-        <v>915</v>
+      <c r="L350" s="133" t="s">
+        <v>891</v>
       </c>
       <c r="M350" s="114" t="s">
-        <v>911</v>
+        <v>887</v>
       </c>
     </row>
     <row r="351" spans="1:13" x14ac:dyDescent="0.3">
@@ -16942,12 +16909,12 @@
         <v>44964</v>
       </c>
       <c r="B351" s="109" t="s">
-        <v>916</v>
+        <v>892</v>
       </c>
       <c r="C351" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D351" s="135"/>
+      <c r="D351" s="132"/>
       <c r="E351" s="109" t="s">
         <v>155</v>
       </c>
@@ -16957,11 +16924,11 @@
       <c r="G351" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L351" s="136" t="s">
-        <v>917</v>
+      <c r="L351" s="133" t="s">
+        <v>893</v>
       </c>
       <c r="M351" s="114" t="s">
-        <v>911</v>
+        <v>887</v>
       </c>
     </row>
     <row r="352" spans="1:13" x14ac:dyDescent="0.3">
@@ -16969,12 +16936,12 @@
         <v>44964</v>
       </c>
       <c r="B352" s="109" t="s">
-        <v>918</v>
+        <v>894</v>
       </c>
       <c r="C352" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D352" s="135"/>
+      <c r="D352" s="132"/>
       <c r="E352" s="109" t="s">
         <v>155</v>
       </c>
@@ -16984,11 +16951,11 @@
       <c r="G352" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L352" s="136" t="s">
-        <v>919</v>
+      <c r="L352" s="133" t="s">
+        <v>895</v>
       </c>
       <c r="M352" s="114" t="s">
-        <v>911</v>
+        <v>887</v>
       </c>
     </row>
     <row r="353" spans="1:13" x14ac:dyDescent="0.3">
@@ -16996,12 +16963,12 @@
         <v>44964</v>
       </c>
       <c r="B353" s="109" t="s">
-        <v>920</v>
+        <v>896</v>
       </c>
       <c r="C353" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D353" s="135"/>
+      <c r="D353" s="132"/>
       <c r="E353" s="109" t="s">
         <v>155</v>
       </c>
@@ -17011,11 +16978,11 @@
       <c r="G353" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L353" s="136" t="s">
-        <v>921</v>
+      <c r="L353" s="133" t="s">
+        <v>897</v>
       </c>
       <c r="M353" s="114" t="s">
-        <v>911</v>
+        <v>887</v>
       </c>
     </row>
     <row r="354" spans="1:13" x14ac:dyDescent="0.3">
@@ -17023,12 +16990,12 @@
         <v>44964</v>
       </c>
       <c r="B354" s="109" t="s">
-        <v>922</v>
+        <v>898</v>
       </c>
       <c r="C354" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D354" s="135"/>
+      <c r="D354" s="132"/>
       <c r="E354" s="109" t="s">
         <v>155</v>
       </c>
@@ -17038,11 +17005,11 @@
       <c r="G354" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L354" s="136" t="s">
-        <v>923</v>
+      <c r="L354" s="133" t="s">
+        <v>899</v>
       </c>
       <c r="M354" s="114" t="s">
-        <v>924</v>
+        <v>900</v>
       </c>
     </row>
     <row r="355" spans="1:13" x14ac:dyDescent="0.3">
@@ -17050,12 +17017,12 @@
         <v>44964</v>
       </c>
       <c r="B355" s="109" t="s">
-        <v>925</v>
+        <v>901</v>
       </c>
       <c r="C355" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D355" s="135"/>
+      <c r="D355" s="132"/>
       <c r="E355" s="109" t="s">
         <v>155</v>
       </c>
@@ -17065,11 +17032,11 @@
       <c r="G355" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L355" s="136" t="s">
-        <v>926</v>
+      <c r="L355" s="133" t="s">
+        <v>902</v>
       </c>
       <c r="M355" s="114" t="s">
-        <v>924</v>
+        <v>900</v>
       </c>
     </row>
     <row r="356" spans="1:13" x14ac:dyDescent="0.3">
@@ -17077,12 +17044,12 @@
         <v>44964</v>
       </c>
       <c r="B356" s="109" t="s">
-        <v>927</v>
+        <v>903</v>
       </c>
       <c r="C356" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D356" s="135"/>
+      <c r="D356" s="132"/>
       <c r="E356" s="109" t="s">
         <v>155</v>
       </c>
@@ -17092,11 +17059,11 @@
       <c r="G356" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L356" s="136" t="s">
-        <v>928</v>
+      <c r="L356" s="133" t="s">
+        <v>904</v>
       </c>
       <c r="M356" s="114" t="s">
-        <v>924</v>
+        <v>900</v>
       </c>
     </row>
     <row r="357" spans="1:13" x14ac:dyDescent="0.3">
@@ -17104,12 +17071,12 @@
         <v>44964</v>
       </c>
       <c r="B357" s="109" t="s">
-        <v>929</v>
+        <v>905</v>
       </c>
       <c r="C357" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D357" s="135"/>
+      <c r="D357" s="132"/>
       <c r="E357" s="109" t="s">
         <v>155</v>
       </c>
@@ -17119,11 +17086,11 @@
       <c r="G357" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L357" s="136" t="s">
-        <v>930</v>
+      <c r="L357" s="133" t="s">
+        <v>906</v>
       </c>
       <c r="M357" s="114" t="s">
-        <v>924</v>
+        <v>900</v>
       </c>
     </row>
     <row r="358" spans="1:13" x14ac:dyDescent="0.3">
@@ -17131,12 +17098,12 @@
         <v>44964</v>
       </c>
       <c r="B358" s="109" t="s">
-        <v>931</v>
+        <v>907</v>
       </c>
       <c r="C358" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D358" s="135"/>
+      <c r="D358" s="132"/>
       <c r="E358" s="109" t="s">
         <v>155</v>
       </c>
@@ -17146,11 +17113,11 @@
       <c r="G358" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L358" s="136" t="s">
-        <v>932</v>
+      <c r="L358" s="133" t="s">
+        <v>908</v>
       </c>
       <c r="M358" s="114" t="s">
-        <v>933</v>
+        <v>909</v>
       </c>
     </row>
     <row r="359" spans="1:13" x14ac:dyDescent="0.3">
@@ -17158,12 +17125,12 @@
         <v>44964</v>
       </c>
       <c r="B359" s="109" t="s">
-        <v>934</v>
+        <v>910</v>
       </c>
       <c r="C359" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D359" s="135"/>
+      <c r="D359" s="132"/>
       <c r="E359" s="109" t="s">
         <v>155</v>
       </c>
@@ -17173,11 +17140,11 @@
       <c r="G359" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L359" s="136" t="s">
-        <v>935</v>
+      <c r="L359" s="133" t="s">
+        <v>911</v>
       </c>
       <c r="M359" s="114" t="s">
-        <v>933</v>
+        <v>909</v>
       </c>
     </row>
     <row r="360" spans="1:13" x14ac:dyDescent="0.3">
@@ -17185,12 +17152,12 @@
         <v>44964</v>
       </c>
       <c r="B360" s="109" t="s">
-        <v>936</v>
+        <v>912</v>
       </c>
       <c r="C360" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D360" s="135"/>
+      <c r="D360" s="132"/>
       <c r="E360" s="109" t="s">
         <v>155</v>
       </c>
@@ -17200,11 +17167,11 @@
       <c r="G360" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L360" s="136" t="s">
-        <v>937</v>
+      <c r="L360" s="133" t="s">
+        <v>913</v>
       </c>
       <c r="M360" s="114" t="s">
-        <v>933</v>
+        <v>909</v>
       </c>
     </row>
     <row r="361" spans="1:13" x14ac:dyDescent="0.3">
@@ -17212,12 +17179,12 @@
         <v>44964</v>
       </c>
       <c r="B361" s="109" t="s">
-        <v>938</v>
+        <v>914</v>
       </c>
       <c r="C361" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D361" s="135"/>
+      <c r="D361" s="132"/>
       <c r="E361" s="109" t="s">
         <v>155</v>
       </c>
@@ -17227,11 +17194,11 @@
       <c r="G361" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L361" s="136" t="s">
-        <v>939</v>
+      <c r="L361" s="133" t="s">
+        <v>915</v>
       </c>
       <c r="M361" s="114" t="s">
-        <v>933</v>
+        <v>909</v>
       </c>
     </row>
     <row r="362" spans="1:13" x14ac:dyDescent="0.3">
@@ -17239,12 +17206,12 @@
         <v>44964</v>
       </c>
       <c r="B362" s="109" t="s">
-        <v>940</v>
+        <v>916</v>
       </c>
       <c r="C362" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D362" s="135"/>
+      <c r="D362" s="132"/>
       <c r="E362" s="109" t="s">
         <v>155</v>
       </c>
@@ -17254,11 +17221,11 @@
       <c r="G362" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L362" s="136" t="s">
-        <v>941</v>
+      <c r="L362" s="133" t="s">
+        <v>917</v>
       </c>
       <c r="M362" s="114" t="s">
-        <v>933</v>
+        <v>909</v>
       </c>
     </row>
     <row r="363" spans="1:13" x14ac:dyDescent="0.3">
@@ -17266,12 +17233,12 @@
         <v>44964</v>
       </c>
       <c r="B363" s="109" t="s">
-        <v>942</v>
+        <v>918</v>
       </c>
       <c r="C363" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D363" s="135"/>
+      <c r="D363" s="132"/>
       <c r="E363" s="109" t="s">
         <v>155</v>
       </c>
@@ -17281,11 +17248,11 @@
       <c r="G363" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L363" s="136" t="s">
-        <v>943</v>
+      <c r="L363" s="133" t="s">
+        <v>919</v>
       </c>
       <c r="M363" s="114" t="s">
-        <v>944</v>
+        <v>920</v>
       </c>
     </row>
     <row r="364" spans="1:13" x14ac:dyDescent="0.3">
@@ -17293,12 +17260,12 @@
         <v>44964</v>
       </c>
       <c r="B364" s="109" t="s">
-        <v>945</v>
+        <v>921</v>
       </c>
       <c r="C364" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D364" s="135"/>
+      <c r="D364" s="132"/>
       <c r="E364" s="109" t="s">
         <v>155</v>
       </c>
@@ -17308,11 +17275,11 @@
       <c r="G364" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L364" s="136" t="s">
-        <v>946</v>
+      <c r="L364" s="133" t="s">
+        <v>922</v>
       </c>
       <c r="M364" s="114" t="s">
-        <v>944</v>
+        <v>920</v>
       </c>
     </row>
     <row r="365" spans="1:13" x14ac:dyDescent="0.3">
@@ -17320,12 +17287,12 @@
         <v>44964</v>
       </c>
       <c r="B365" s="109" t="s">
-        <v>947</v>
+        <v>923</v>
       </c>
       <c r="C365" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D365" s="135"/>
+      <c r="D365" s="132"/>
       <c r="E365" s="109" t="s">
         <v>155</v>
       </c>
@@ -17335,11 +17302,11 @@
       <c r="G365" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L365" s="136" t="s">
-        <v>948</v>
+      <c r="L365" s="133" t="s">
+        <v>924</v>
       </c>
       <c r="M365" s="114" t="s">
-        <v>944</v>
+        <v>920</v>
       </c>
     </row>
     <row r="366" spans="1:13" x14ac:dyDescent="0.3">
@@ -17347,12 +17314,12 @@
         <v>44964</v>
       </c>
       <c r="B366" s="109" t="s">
-        <v>949</v>
+        <v>925</v>
       </c>
       <c r="C366" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D366" s="135"/>
+      <c r="D366" s="132"/>
       <c r="E366" s="109" t="s">
         <v>155</v>
       </c>
@@ -17362,11 +17329,11 @@
       <c r="G366" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L366" s="136" t="s">
-        <v>950</v>
+      <c r="L366" s="133" t="s">
+        <v>926</v>
       </c>
       <c r="M366" s="114" t="s">
-        <v>944</v>
+        <v>920</v>
       </c>
     </row>
     <row r="367" spans="1:13" x14ac:dyDescent="0.3">
@@ -17374,12 +17341,12 @@
         <v>44964</v>
       </c>
       <c r="B367" s="109" t="s">
-        <v>951</v>
+        <v>927</v>
       </c>
       <c r="C367" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D367" s="135"/>
+      <c r="D367" s="132"/>
       <c r="E367" s="109" t="s">
         <v>155</v>
       </c>
@@ -17389,11 +17356,11 @@
       <c r="G367" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L367" s="136" t="s">
-        <v>952</v>
+      <c r="L367" s="133" t="s">
+        <v>928</v>
       </c>
       <c r="M367" s="114" t="s">
-        <v>944</v>
+        <v>920</v>
       </c>
     </row>
     <row r="368" spans="1:13" x14ac:dyDescent="0.3">
@@ -17401,12 +17368,12 @@
         <v>44964</v>
       </c>
       <c r="B368" s="109" t="s">
-        <v>953</v>
+        <v>929</v>
       </c>
       <c r="C368" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D368" s="135"/>
+      <c r="D368" s="132"/>
       <c r="E368" s="109" t="s">
         <v>155</v>
       </c>
@@ -17416,11 +17383,11 @@
       <c r="G368" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L368" s="136" t="s">
-        <v>954</v>
+      <c r="L368" s="133" t="s">
+        <v>930</v>
       </c>
       <c r="M368" s="114" t="s">
-        <v>955</v>
+        <v>931</v>
       </c>
     </row>
     <row r="369" spans="1:13" x14ac:dyDescent="0.3">
@@ -17428,12 +17395,12 @@
         <v>44964</v>
       </c>
       <c r="B369" s="109" t="s">
-        <v>956</v>
+        <v>932</v>
       </c>
       <c r="C369" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D369" s="135"/>
+      <c r="D369" s="132"/>
       <c r="E369" s="109" t="s">
         <v>155</v>
       </c>
@@ -17443,11 +17410,11 @@
       <c r="G369" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L369" s="136" t="s">
-        <v>957</v>
+      <c r="L369" s="133" t="s">
+        <v>933</v>
       </c>
       <c r="M369" s="114" t="s">
-        <v>955</v>
+        <v>931</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ooredoo event: applied the details for 45 new sim
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1177" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEF7A6D4-4C16-4DEC-9E21-5C603FF4A18F}"/>
+  <xr:revisionPtr revIDLastSave="1190" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33C552F9-0481-4126-9BEB-C5050DCF8CA4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="OoredooMasterFile" sheetId="2" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2227" uniqueCount="946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2375" uniqueCount="1031">
   <si>
     <t>ICC ID</t>
   </si>
@@ -2943,6 +2943,261 @@
     <t>RESIGNED
 05-Feb-2023 @11:38 - Cancellation of this Ooredoo Account and Service Number (Resigned) - Dan
 08-Feb-2023 @11:35 - Request was Completed with Plan G; Successfully Cancelled</t>
+  </si>
+  <si>
+    <t>LAKSHAMAN CHAUHAN</t>
+  </si>
+  <si>
+    <t>SENIOR MECHANICAL TECHNICIAN</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>EDWARD KABUYE</t>
+  </si>
+  <si>
+    <t>ELECTRICAL TECHNICIAN</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>MOHAMMED ABDUL KADER MONSHI</t>
+  </si>
+  <si>
+    <t>MECHANICAL TECHNICIAN</t>
+  </si>
+  <si>
+    <t>MUHAMMAD MOHSIN HUSSAIN</t>
+  </si>
+  <si>
+    <t>SENIOR ELECTRICAL TECHNICIAN</t>
+  </si>
+  <si>
+    <t>FARHAN ULLAH</t>
+  </si>
+  <si>
+    <t>ASSISTANT ELECTRICAL TECHNICIAN</t>
+  </si>
+  <si>
+    <t>UZAIR KHAN ANWAR KHAN</t>
+  </si>
+  <si>
+    <t>SHOBASH KANDEL</t>
+  </si>
+  <si>
+    <t>MARGARITO BUSTAMANTE BARRIT</t>
+  </si>
+  <si>
+    <t>SENIOR HVAC TECHNICIAN</t>
+  </si>
+  <si>
+    <t>ASAD ABBASS</t>
+  </si>
+  <si>
+    <t>YUSUFU MUBIRU</t>
+  </si>
+  <si>
+    <t>FAIZAN HUSSAIN</t>
+  </si>
+  <si>
+    <t>SADDAM HUSSAIN MOHAMMAD SAGHIR</t>
+  </si>
+  <si>
+    <t>MUHAMMAD IMRAN</t>
+  </si>
+  <si>
+    <t>SRIRAM SINGAPRAVADIVELU</t>
+  </si>
+  <si>
+    <t>DENIS SEBUGWAWO KATAMBA</t>
+  </si>
+  <si>
+    <t>BEDAR AHMAD</t>
+  </si>
+  <si>
+    <t>MATTHEW TIKAWEN</t>
+  </si>
+  <si>
+    <t>REY JAY MANZALAY DANAO</t>
+  </si>
+  <si>
+    <t>WAJID QAMAR BHATTI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PATRICK AGYEI MENSAH </t>
+  </si>
+  <si>
+    <t>ALIMANSI ISABIRYE</t>
+  </si>
+  <si>
+    <t>ABDULRASHID BYARUGABA</t>
+  </si>
+  <si>
+    <t>MOHAMMAD NOOR ALAM</t>
+  </si>
+  <si>
+    <t>DAVID WILLIAM BASAJJASUBI KYEYUNE</t>
+  </si>
+  <si>
+    <t>ALEX DAVIDS KISEKKA</t>
+  </si>
+  <si>
+    <t>ASSISTANT MECHANICAL TECHNICIAN</t>
+  </si>
+  <si>
+    <t>MUHAMMAD IMRAN MUHAMMAD TAJ</t>
+  </si>
+  <si>
+    <t>SALAMATHULLAH</t>
+  </si>
+  <si>
+    <t>STEPHEN OFOSU</t>
+  </si>
+  <si>
+    <t>SADDAM HUSSAIN</t>
+  </si>
+  <si>
+    <t>ZEESHAN ADIL</t>
+  </si>
+  <si>
+    <t>JOSEPH NDIBILBE</t>
+  </si>
+  <si>
+    <t>CONRADO ANU OS MELENCION</t>
+  </si>
+  <si>
+    <t>ABDUL SABOOR RAWALPINDI</t>
+  </si>
+  <si>
+    <t>ISMA KASOLO</t>
+  </si>
+  <si>
+    <t>HVAC TECHNICIAN</t>
+  </si>
+  <si>
+    <t>ABDUL AZIZ</t>
+  </si>
+  <si>
+    <t>FLS ELECTRICAL TECHNICIAN</t>
+  </si>
+  <si>
+    <t>SK SAMIM</t>
+  </si>
+  <si>
+    <t>MD SHAHINUR ISLAM</t>
+  </si>
+  <si>
+    <t>000272 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>000723 - ELECTRICAL</t>
+  </si>
+  <si>
+    <t>000758 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>001815 - ELECTRICAL</t>
+  </si>
+  <si>
+    <t>001761 - ELECTRICAL</t>
+  </si>
+  <si>
+    <t>001764 - ELECTRICAL</t>
+  </si>
+  <si>
+    <t>001814 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>000755 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>001871 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>000712 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>001618 - ELECTRICAL</t>
+  </si>
+  <si>
+    <t>000237 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>001543 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>000532 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>000170 - ELECTRICAL</t>
+  </si>
+  <si>
+    <t>001544 - ELECTRICAL</t>
+  </si>
+  <si>
+    <t>000598 - ELECTRICAL</t>
+  </si>
+  <si>
+    <t>001533 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>000126 - ELECTRICAL</t>
+  </si>
+  <si>
+    <t>001404 - ELECTRICAL</t>
+  </si>
+  <si>
+    <t>000678 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>000333 - ELECTRICAL</t>
+  </si>
+  <si>
+    <t>000360 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>000149 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>000690 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>001749 - ELECTRICAL</t>
+  </si>
+  <si>
+    <t>001875 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>000764 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>001451 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>001547 - ELECTRICAL</t>
+  </si>
+  <si>
+    <t>001050 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>000754 - ELECTRICAL</t>
+  </si>
+  <si>
+    <t>001924 - ELECTRICAL</t>
+  </si>
+  <si>
+    <t>000677 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>001819 - ELECTRICAL</t>
+  </si>
+  <si>
+    <t>001038 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>001813 - MECHANICAL/HVAC</t>
   </si>
 </sst>
 </file>
@@ -3687,10 +3942,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="14" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="14" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5033,10 +5288,10 @@
   <dimension ref="A1:W369"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="J352" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E341" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L370" sqref="L370"/>
+      <selection pane="bottomRight" activeCell="D370" sqref="D370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5048,9 +5303,9 @@
     <col min="5" max="5" width="16.5546875" style="109" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="110" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.109375" style="111" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.88671875" style="112" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.77734375" style="111" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.88671875" style="111" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.33203125" style="112" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40" style="111" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.88671875" style="111" customWidth="1"/>
     <col min="11" max="11" width="10.33203125" style="111" customWidth="1"/>
     <col min="12" max="12" width="22.5546875" style="113" customWidth="1"/>
     <col min="13" max="13" width="139.88671875" style="114" bestFit="1" customWidth="1"/>
@@ -16212,7 +16467,9 @@
       <c r="C325" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D325" s="132"/>
+      <c r="D325" s="133">
+        <v>33574156</v>
+      </c>
       <c r="E325" s="109" t="s">
         <v>155</v>
       </c>
@@ -16222,7 +16479,19 @@
       <c r="G325" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L325" s="133" t="s">
+      <c r="H325" s="112" t="s">
+        <v>994</v>
+      </c>
+      <c r="I325" s="111" t="s">
+        <v>946</v>
+      </c>
+      <c r="J325" s="111" t="s">
+        <v>947</v>
+      </c>
+      <c r="K325" s="111" t="s">
+        <v>948</v>
+      </c>
+      <c r="L325" s="132" t="s">
         <v>830</v>
       </c>
       <c r="M325" s="114" t="s">
@@ -16239,7 +16508,9 @@
       <c r="C326" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D326" s="132"/>
+      <c r="D326" s="133">
+        <v>33603140</v>
+      </c>
       <c r="E326" s="109" t="s">
         <v>155</v>
       </c>
@@ -16249,7 +16520,19 @@
       <c r="G326" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L326" s="133" t="s">
+      <c r="H326" s="112" t="s">
+        <v>995</v>
+      </c>
+      <c r="I326" s="111" t="s">
+        <v>949</v>
+      </c>
+      <c r="J326" s="111" t="s">
+        <v>950</v>
+      </c>
+      <c r="K326" s="111" t="s">
+        <v>951</v>
+      </c>
+      <c r="L326" s="132" t="s">
         <v>833</v>
       </c>
       <c r="M326" s="114" t="s">
@@ -16266,7 +16549,9 @@
       <c r="C327" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D327" s="132"/>
+      <c r="D327" s="133">
+        <v>33585461</v>
+      </c>
       <c r="E327" s="109" t="s">
         <v>155</v>
       </c>
@@ -16276,7 +16561,19 @@
       <c r="G327" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L327" s="133" t="s">
+      <c r="H327" s="112" t="s">
+        <v>996</v>
+      </c>
+      <c r="I327" s="111" t="s">
+        <v>952</v>
+      </c>
+      <c r="J327" s="111" t="s">
+        <v>953</v>
+      </c>
+      <c r="K327" s="111" t="s">
+        <v>641</v>
+      </c>
+      <c r="L327" s="132" t="s">
         <v>836</v>
       </c>
       <c r="M327" s="114" t="s">
@@ -16293,7 +16590,9 @@
       <c r="C328" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D328" s="132"/>
+      <c r="D328" s="133">
+        <v>33576710</v>
+      </c>
       <c r="E328" s="109" t="s">
         <v>155</v>
       </c>
@@ -16303,7 +16602,19 @@
       <c r="G328" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L328" s="133" t="s">
+      <c r="H328" s="112" t="s">
+        <v>997</v>
+      </c>
+      <c r="I328" s="111" t="s">
+        <v>954</v>
+      </c>
+      <c r="J328" s="111" t="s">
+        <v>955</v>
+      </c>
+      <c r="K328" s="111" t="s">
+        <v>641</v>
+      </c>
+      <c r="L328" s="132" t="s">
         <v>839</v>
       </c>
       <c r="M328" s="114" t="s">
@@ -16320,7 +16631,9 @@
       <c r="C329" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D329" s="132"/>
+      <c r="D329" s="133">
+        <v>33595578</v>
+      </c>
       <c r="E329" s="109" t="s">
         <v>155</v>
       </c>
@@ -16330,7 +16643,19 @@
       <c r="G329" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L329" s="133" t="s">
+      <c r="H329" s="112" t="s">
+        <v>998</v>
+      </c>
+      <c r="I329" s="111" t="s">
+        <v>956</v>
+      </c>
+      <c r="J329" s="111" t="s">
+        <v>957</v>
+      </c>
+      <c r="K329" s="111" t="s">
+        <v>951</v>
+      </c>
+      <c r="L329" s="132" t="s">
         <v>841</v>
       </c>
       <c r="M329" s="114" t="s">
@@ -16347,7 +16672,9 @@
       <c r="C330" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D330" s="132"/>
+      <c r="D330" s="133">
+        <v>33583901</v>
+      </c>
       <c r="E330" s="109" t="s">
         <v>155</v>
       </c>
@@ -16357,7 +16684,19 @@
       <c r="G330" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L330" s="133" t="s">
+      <c r="H330" s="112" t="s">
+        <v>999</v>
+      </c>
+      <c r="I330" s="111" t="s">
+        <v>958</v>
+      </c>
+      <c r="J330" s="111" t="s">
+        <v>957</v>
+      </c>
+      <c r="K330" s="111" t="s">
+        <v>951</v>
+      </c>
+      <c r="L330" s="132" t="s">
         <v>844</v>
       </c>
       <c r="M330" s="114" t="s">
@@ -16374,7 +16713,9 @@
       <c r="C331" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D331" s="132"/>
+      <c r="D331" s="133">
+        <v>33576317</v>
+      </c>
       <c r="E331" s="109" t="s">
         <v>155</v>
       </c>
@@ -16384,7 +16725,19 @@
       <c r="G331" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L331" s="133" t="s">
+      <c r="H331" s="112" t="s">
+        <v>1000</v>
+      </c>
+      <c r="I331" s="111" t="s">
+        <v>959</v>
+      </c>
+      <c r="J331" s="111" t="s">
+        <v>953</v>
+      </c>
+      <c r="K331" s="111" t="s">
+        <v>641</v>
+      </c>
+      <c r="L331" s="132" t="s">
         <v>847</v>
       </c>
       <c r="M331" s="114" t="s">
@@ -16401,7 +16754,9 @@
       <c r="C332" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D332" s="132"/>
+      <c r="D332" s="133">
+        <v>33581367</v>
+      </c>
       <c r="E332" s="109" t="s">
         <v>155</v>
       </c>
@@ -16411,7 +16766,19 @@
       <c r="G332" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L332" s="133" t="s">
+      <c r="H332" s="112" t="s">
+        <v>1001</v>
+      </c>
+      <c r="I332" s="111" t="s">
+        <v>960</v>
+      </c>
+      <c r="J332" s="111" t="s">
+        <v>961</v>
+      </c>
+      <c r="K332" s="111" t="s">
+        <v>948</v>
+      </c>
+      <c r="L332" s="132" t="s">
         <v>849</v>
       </c>
       <c r="M332" s="114" t="s">
@@ -16428,7 +16795,9 @@
       <c r="C333" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D333" s="132"/>
+      <c r="D333" s="133">
+        <v>33585994</v>
+      </c>
       <c r="E333" s="109" t="s">
         <v>155</v>
       </c>
@@ -16438,7 +16807,19 @@
       <c r="G333" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L333" s="133" t="s">
+      <c r="H333" s="112" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I333" s="111" t="s">
+        <v>962</v>
+      </c>
+      <c r="J333" s="111" t="s">
+        <v>947</v>
+      </c>
+      <c r="K333" s="111" t="s">
+        <v>948</v>
+      </c>
+      <c r="L333" s="132" t="s">
         <v>851</v>
       </c>
       <c r="M333" s="114" t="s">
@@ -16455,7 +16836,9 @@
       <c r="C334" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D334" s="132"/>
+      <c r="D334" s="133">
+        <v>33596039</v>
+      </c>
       <c r="E334" s="109" t="s">
         <v>155</v>
       </c>
@@ -16465,7 +16848,19 @@
       <c r="G334" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L334" s="133" t="s">
+      <c r="H334" s="112" t="s">
+        <v>1003</v>
+      </c>
+      <c r="I334" s="111" t="s">
+        <v>963</v>
+      </c>
+      <c r="J334" s="111" t="s">
+        <v>961</v>
+      </c>
+      <c r="K334" s="111" t="s">
+        <v>948</v>
+      </c>
+      <c r="L334" s="132" t="s">
         <v>854</v>
       </c>
       <c r="M334" s="114" t="s">
@@ -16482,7 +16877,9 @@
       <c r="C335" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D335" s="132"/>
+      <c r="D335" s="133">
+        <v>33583392</v>
+      </c>
       <c r="E335" s="109" t="s">
         <v>155</v>
       </c>
@@ -16492,7 +16889,19 @@
       <c r="G335" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L335" s="133" t="s">
+      <c r="H335" s="112" t="s">
+        <v>1004</v>
+      </c>
+      <c r="I335" s="111" t="s">
+        <v>964</v>
+      </c>
+      <c r="J335" s="111" t="s">
+        <v>957</v>
+      </c>
+      <c r="K335" s="111" t="s">
+        <v>951</v>
+      </c>
+      <c r="L335" s="132" t="s">
         <v>856</v>
       </c>
       <c r="M335" s="114" t="s">
@@ -16509,7 +16918,9 @@
       <c r="C336" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D336" s="132"/>
+      <c r="D336" s="133">
+        <v>33598446</v>
+      </c>
       <c r="E336" s="109" t="s">
         <v>155</v>
       </c>
@@ -16519,7 +16930,19 @@
       <c r="G336" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L336" s="133" t="s">
+      <c r="H336" s="112" t="s">
+        <v>1005</v>
+      </c>
+      <c r="I336" s="111" t="s">
+        <v>965</v>
+      </c>
+      <c r="J336" s="111" t="s">
+        <v>961</v>
+      </c>
+      <c r="K336" s="111" t="s">
+        <v>641</v>
+      </c>
+      <c r="L336" s="132" t="s">
         <v>859</v>
       </c>
       <c r="M336" s="114" t="s">
@@ -16536,7 +16959,9 @@
       <c r="C337" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D337" s="132"/>
+      <c r="D337" s="133">
+        <v>33597912</v>
+      </c>
       <c r="E337" s="109" t="s">
         <v>155</v>
       </c>
@@ -16546,7 +16971,19 @@
       <c r="G337" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L337" s="133" t="s">
+      <c r="H337" s="112" t="s">
+        <v>1006</v>
+      </c>
+      <c r="I337" s="111" t="s">
+        <v>966</v>
+      </c>
+      <c r="J337" s="111" t="s">
+        <v>953</v>
+      </c>
+      <c r="K337" s="111" t="s">
+        <v>641</v>
+      </c>
+      <c r="L337" s="132" t="s">
         <v>861</v>
       </c>
       <c r="M337" s="114" t="s">
@@ -16563,7 +17000,9 @@
       <c r="C338" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D338" s="132"/>
+      <c r="D338" s="133">
+        <v>33601543</v>
+      </c>
       <c r="E338" s="109" t="s">
         <v>155</v>
       </c>
@@ -16573,7 +17012,19 @@
       <c r="G338" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L338" s="133" t="s">
+      <c r="H338" s="112" t="s">
+        <v>1007</v>
+      </c>
+      <c r="I338" s="111" t="s">
+        <v>967</v>
+      </c>
+      <c r="J338" s="111" t="s">
+        <v>268</v>
+      </c>
+      <c r="K338" s="111" t="s">
+        <v>948</v>
+      </c>
+      <c r="L338" s="132" t="s">
         <v>863</v>
       </c>
       <c r="M338" s="114" t="s">
@@ -16590,7 +17041,9 @@
       <c r="C339" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D339" s="132"/>
+      <c r="D339" s="133">
+        <v>33596920</v>
+      </c>
       <c r="E339" s="109" t="s">
         <v>155</v>
       </c>
@@ -16600,7 +17053,19 @@
       <c r="G339" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L339" s="133" t="s">
+      <c r="H339" s="112" t="s">
+        <v>1008</v>
+      </c>
+      <c r="I339" s="111" t="s">
+        <v>968</v>
+      </c>
+      <c r="J339" s="111" t="s">
+        <v>955</v>
+      </c>
+      <c r="K339" s="111" t="s">
+        <v>948</v>
+      </c>
+      <c r="L339" s="132" t="s">
         <v>866</v>
       </c>
       <c r="M339" s="114" t="s">
@@ -16617,7 +17082,9 @@
       <c r="C340" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D340" s="132"/>
+      <c r="D340" s="133">
+        <v>33579329</v>
+      </c>
       <c r="E340" s="109" t="s">
         <v>155</v>
       </c>
@@ -16627,7 +17094,19 @@
       <c r="G340" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L340" s="133" t="s">
+      <c r="H340" s="112" t="s">
+        <v>1009</v>
+      </c>
+      <c r="I340" s="111" t="s">
+        <v>969</v>
+      </c>
+      <c r="J340" s="111" t="s">
+        <v>950</v>
+      </c>
+      <c r="K340" s="111" t="s">
+        <v>641</v>
+      </c>
+      <c r="L340" s="132" t="s">
         <v>869</v>
       </c>
       <c r="M340" s="114" t="s">
@@ -16644,7 +17123,9 @@
       <c r="C341" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D341" s="132"/>
+      <c r="D341" s="133">
+        <v>33598379</v>
+      </c>
       <c r="E341" s="109" t="s">
         <v>155</v>
       </c>
@@ -16654,7 +17135,19 @@
       <c r="G341" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L341" s="133" t="s">
+      <c r="H341" s="112" t="s">
+        <v>1010</v>
+      </c>
+      <c r="I341" s="111" t="s">
+        <v>970</v>
+      </c>
+      <c r="J341" s="111" t="s">
+        <v>955</v>
+      </c>
+      <c r="K341" s="111" t="s">
+        <v>948</v>
+      </c>
+      <c r="L341" s="132" t="s">
         <v>871</v>
       </c>
       <c r="M341" s="114" t="s">
@@ -16671,7 +17164,9 @@
       <c r="C342" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D342" s="132"/>
+      <c r="D342" s="133">
+        <v>33603691</v>
+      </c>
       <c r="E342" s="109" t="s">
         <v>155</v>
       </c>
@@ -16681,7 +17176,19 @@
       <c r="G342" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L342" s="133" t="s">
+      <c r="H342" s="112" t="s">
+        <v>1011</v>
+      </c>
+      <c r="I342" s="111" t="s">
+        <v>971</v>
+      </c>
+      <c r="J342" s="111" t="s">
+        <v>953</v>
+      </c>
+      <c r="K342" s="111" t="s">
+        <v>641</v>
+      </c>
+      <c r="L342" s="132" t="s">
         <v>873</v>
       </c>
       <c r="M342" s="114" t="s">
@@ -16698,7 +17205,9 @@
       <c r="C343" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D343" s="132"/>
+      <c r="D343" s="133">
+        <v>33585246</v>
+      </c>
       <c r="E343" s="109" t="s">
         <v>155</v>
       </c>
@@ -16708,7 +17217,19 @@
       <c r="G343" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L343" s="133" t="s">
+      <c r="H343" s="112" t="s">
+        <v>1012</v>
+      </c>
+      <c r="I343" s="111" t="s">
+        <v>972</v>
+      </c>
+      <c r="J343" s="111" t="s">
+        <v>955</v>
+      </c>
+      <c r="K343" s="111" t="s">
+        <v>948</v>
+      </c>
+      <c r="L343" s="132" t="s">
         <v>875</v>
       </c>
       <c r="M343" s="114" t="s">
@@ -16725,7 +17246,9 @@
       <c r="C344" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D344" s="132"/>
+      <c r="D344" s="133">
+        <v>33574035</v>
+      </c>
       <c r="E344" s="109" t="s">
         <v>155</v>
       </c>
@@ -16735,7 +17258,19 @@
       <c r="G344" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L344" s="133" t="s">
+      <c r="H344" s="112" t="s">
+        <v>1013</v>
+      </c>
+      <c r="I344" s="111" t="s">
+        <v>973</v>
+      </c>
+      <c r="J344" s="111" t="s">
+        <v>950</v>
+      </c>
+      <c r="K344" s="111" t="s">
+        <v>641</v>
+      </c>
+      <c r="L344" s="132" t="s">
         <v>877</v>
       </c>
       <c r="M344" s="114" t="s">
@@ -16752,7 +17287,9 @@
       <c r="C345" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D345" s="132"/>
+      <c r="D345" s="133">
+        <v>33597942</v>
+      </c>
       <c r="E345" s="109" t="s">
         <v>155</v>
       </c>
@@ -16762,7 +17299,19 @@
       <c r="G345" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L345" s="133" t="s">
+      <c r="H345" s="112" t="s">
+        <v>1014</v>
+      </c>
+      <c r="I345" s="111" t="s">
+        <v>974</v>
+      </c>
+      <c r="J345" s="111" t="s">
+        <v>953</v>
+      </c>
+      <c r="K345" s="111" t="s">
+        <v>641</v>
+      </c>
+      <c r="L345" s="132" t="s">
         <v>879</v>
       </c>
       <c r="M345" s="114" t="s">
@@ -16779,7 +17328,9 @@
       <c r="C346" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D346" s="132"/>
+      <c r="D346" s="133">
+        <v>33581276</v>
+      </c>
       <c r="E346" s="109" t="s">
         <v>155</v>
       </c>
@@ -16789,7 +17340,19 @@
       <c r="G346" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L346" s="133" t="s">
+      <c r="H346" s="112" t="s">
+        <v>1015</v>
+      </c>
+      <c r="I346" s="111" t="s">
+        <v>975</v>
+      </c>
+      <c r="J346" s="111" t="s">
+        <v>955</v>
+      </c>
+      <c r="K346" s="111" t="s">
+        <v>948</v>
+      </c>
+      <c r="L346" s="132" t="s">
         <v>882</v>
       </c>
       <c r="M346" s="114" t="s">
@@ -16806,7 +17369,9 @@
       <c r="C347" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D347" s="132"/>
+      <c r="D347" s="133">
+        <v>33583276</v>
+      </c>
       <c r="E347" s="109" t="s">
         <v>155</v>
       </c>
@@ -16816,7 +17381,19 @@
       <c r="G347" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L347" s="133" t="s">
+      <c r="H347" s="112" t="s">
+        <v>1016</v>
+      </c>
+      <c r="I347" s="111" t="s">
+        <v>976</v>
+      </c>
+      <c r="J347" s="111" t="s">
+        <v>961</v>
+      </c>
+      <c r="K347" s="111" t="s">
+        <v>948</v>
+      </c>
+      <c r="L347" s="132" t="s">
         <v>884</v>
       </c>
       <c r="M347" s="114" t="s">
@@ -16833,7 +17410,9 @@
       <c r="C348" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D348" s="132"/>
+      <c r="D348" s="133">
+        <v>33576136</v>
+      </c>
       <c r="E348" s="109" t="s">
         <v>155</v>
       </c>
@@ -16843,7 +17422,19 @@
       <c r="G348" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L348" s="133" t="s">
+      <c r="H348" s="112" t="s">
+        <v>1017</v>
+      </c>
+      <c r="I348" s="111" t="s">
+        <v>977</v>
+      </c>
+      <c r="J348" s="111" t="s">
+        <v>947</v>
+      </c>
+      <c r="K348" s="111" t="s">
+        <v>948</v>
+      </c>
+      <c r="L348" s="132" t="s">
         <v>886</v>
       </c>
       <c r="M348" s="114" t="s">
@@ -16860,7 +17451,9 @@
       <c r="C349" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D349" s="132"/>
+      <c r="D349" s="133">
+        <v>33603750</v>
+      </c>
       <c r="E349" s="109" t="s">
         <v>155</v>
       </c>
@@ -16870,7 +17463,19 @@
       <c r="G349" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L349" s="133" t="s">
+      <c r="H349" s="112" t="s">
+        <v>1018</v>
+      </c>
+      <c r="I349" s="111" t="s">
+        <v>978</v>
+      </c>
+      <c r="J349" s="111" t="s">
+        <v>979</v>
+      </c>
+      <c r="K349" s="111" t="s">
+        <v>951</v>
+      </c>
+      <c r="L349" s="132" t="s">
         <v>889</v>
       </c>
       <c r="M349" s="114" t="s">
@@ -16887,7 +17492,9 @@
       <c r="C350" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D350" s="132"/>
+      <c r="D350" s="133">
+        <v>33602876</v>
+      </c>
       <c r="E350" s="109" t="s">
         <v>155</v>
       </c>
@@ -16897,7 +17504,19 @@
       <c r="G350" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L350" s="133" t="s">
+      <c r="H350" s="112" t="s">
+        <v>1019</v>
+      </c>
+      <c r="I350" s="111" t="s">
+        <v>980</v>
+      </c>
+      <c r="J350" s="111" t="s">
+        <v>955</v>
+      </c>
+      <c r="K350" s="111" t="s">
+        <v>948</v>
+      </c>
+      <c r="L350" s="132" t="s">
         <v>891</v>
       </c>
       <c r="M350" s="114" t="s">
@@ -16914,7 +17533,9 @@
       <c r="C351" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D351" s="132"/>
+      <c r="D351" s="133">
+        <v>33598168</v>
+      </c>
       <c r="E351" s="109" t="s">
         <v>155</v>
       </c>
@@ -16924,7 +17545,19 @@
       <c r="G351" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L351" s="133" t="s">
+      <c r="H351" s="112" t="s">
+        <v>1020</v>
+      </c>
+      <c r="I351" s="111" t="s">
+        <v>981</v>
+      </c>
+      <c r="J351" s="111" t="s">
+        <v>947</v>
+      </c>
+      <c r="K351" s="111" t="s">
+        <v>948</v>
+      </c>
+      <c r="L351" s="132" t="s">
         <v>893</v>
       </c>
       <c r="M351" s="114" t="s">
@@ -16941,7 +17574,9 @@
       <c r="C352" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D352" s="132"/>
+      <c r="D352" s="133">
+        <v>33583060</v>
+      </c>
       <c r="E352" s="109" t="s">
         <v>155</v>
       </c>
@@ -16951,7 +17586,19 @@
       <c r="G352" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L352" s="133" t="s">
+      <c r="H352" s="112" t="s">
+        <v>1021</v>
+      </c>
+      <c r="I352" s="111" t="s">
+        <v>982</v>
+      </c>
+      <c r="J352" s="111" t="s">
+        <v>947</v>
+      </c>
+      <c r="K352" s="111" t="s">
+        <v>948</v>
+      </c>
+      <c r="L352" s="132" t="s">
         <v>895</v>
       </c>
       <c r="M352" s="114" t="s">
@@ -16968,7 +17615,9 @@
       <c r="C353" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D353" s="132"/>
+      <c r="D353" s="133">
+        <v>33583208</v>
+      </c>
       <c r="E353" s="109" t="s">
         <v>155</v>
       </c>
@@ -16978,7 +17627,19 @@
       <c r="G353" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L353" s="133" t="s">
+      <c r="H353" s="112" t="s">
+        <v>1022</v>
+      </c>
+      <c r="I353" s="111" t="s">
+        <v>983</v>
+      </c>
+      <c r="J353" s="111" t="s">
+        <v>953</v>
+      </c>
+      <c r="K353" s="111" t="s">
+        <v>641</v>
+      </c>
+      <c r="L353" s="132" t="s">
         <v>897</v>
       </c>
       <c r="M353" s="114" t="s">
@@ -16995,7 +17656,9 @@
       <c r="C354" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D354" s="132"/>
+      <c r="D354" s="133">
+        <v>33596804</v>
+      </c>
       <c r="E354" s="109" t="s">
         <v>155</v>
       </c>
@@ -17005,7 +17668,19 @@
       <c r="G354" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L354" s="133" t="s">
+      <c r="H354" s="112" t="s">
+        <v>1023</v>
+      </c>
+      <c r="I354" s="111" t="s">
+        <v>984</v>
+      </c>
+      <c r="J354" s="111" t="s">
+        <v>950</v>
+      </c>
+      <c r="K354" s="111" t="s">
+        <v>641</v>
+      </c>
+      <c r="L354" s="132" t="s">
         <v>899</v>
       </c>
       <c r="M354" s="114" t="s">
@@ -17022,7 +17697,9 @@
       <c r="C355" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D355" s="132"/>
+      <c r="D355" s="133">
+        <v>33585715</v>
+      </c>
       <c r="E355" s="109" t="s">
         <v>155</v>
       </c>
@@ -17032,7 +17709,19 @@
       <c r="G355" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L355" s="133" t="s">
+      <c r="H355" s="112" t="s">
+        <v>1024</v>
+      </c>
+      <c r="I355" s="111" t="s">
+        <v>985</v>
+      </c>
+      <c r="J355" s="111" t="s">
+        <v>953</v>
+      </c>
+      <c r="K355" s="111" t="s">
+        <v>641</v>
+      </c>
+      <c r="L355" s="132" t="s">
         <v>902</v>
       </c>
       <c r="M355" s="114" t="s">
@@ -17049,7 +17738,9 @@
       <c r="C356" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D356" s="132"/>
+      <c r="D356" s="133">
+        <v>33583569</v>
+      </c>
       <c r="E356" s="109" t="s">
         <v>155</v>
       </c>
@@ -17059,7 +17750,19 @@
       <c r="G356" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L356" s="133" t="s">
+      <c r="H356" s="112" t="s">
+        <v>1025</v>
+      </c>
+      <c r="I356" s="111" t="s">
+        <v>986</v>
+      </c>
+      <c r="J356" s="111" t="s">
+        <v>955</v>
+      </c>
+      <c r="K356" s="111" t="s">
+        <v>948</v>
+      </c>
+      <c r="L356" s="132" t="s">
         <v>904</v>
       </c>
       <c r="M356" s="114" t="s">
@@ -17076,7 +17779,9 @@
       <c r="C357" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D357" s="132"/>
+      <c r="D357" s="133">
+        <v>33586015</v>
+      </c>
       <c r="E357" s="109" t="s">
         <v>155</v>
       </c>
@@ -17086,7 +17791,19 @@
       <c r="G357" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L357" s="133" t="s">
+      <c r="H357" s="112" t="s">
+        <v>1026</v>
+      </c>
+      <c r="I357" s="111" t="s">
+        <v>987</v>
+      </c>
+      <c r="J357" s="111" t="s">
+        <v>955</v>
+      </c>
+      <c r="K357" s="111" t="s">
+        <v>948</v>
+      </c>
+      <c r="L357" s="132" t="s">
         <v>906</v>
       </c>
       <c r="M357" s="114" t="s">
@@ -17103,7 +17820,9 @@
       <c r="C358" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D358" s="132"/>
+      <c r="D358" s="133">
+        <v>33598546</v>
+      </c>
       <c r="E358" s="109" t="s">
         <v>155</v>
       </c>
@@ -17113,7 +17832,19 @@
       <c r="G358" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L358" s="133" t="s">
+      <c r="H358" s="112" t="s">
+        <v>1027</v>
+      </c>
+      <c r="I358" s="111" t="s">
+        <v>988</v>
+      </c>
+      <c r="J358" s="111" t="s">
+        <v>989</v>
+      </c>
+      <c r="K358" s="111" t="s">
+        <v>641</v>
+      </c>
+      <c r="L358" s="132" t="s">
         <v>908</v>
       </c>
       <c r="M358" s="114" t="s">
@@ -17130,7 +17861,9 @@
       <c r="C359" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D359" s="132"/>
+      <c r="D359" s="133">
+        <v>33585194</v>
+      </c>
       <c r="E359" s="109" t="s">
         <v>155</v>
       </c>
@@ -17140,7 +17873,19 @@
       <c r="G359" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L359" s="133" t="s">
+      <c r="H359" s="112" t="s">
+        <v>1028</v>
+      </c>
+      <c r="I359" s="111" t="s">
+        <v>990</v>
+      </c>
+      <c r="J359" s="111" t="s">
+        <v>991</v>
+      </c>
+      <c r="K359" s="111" t="s">
+        <v>641</v>
+      </c>
+      <c r="L359" s="132" t="s">
         <v>911</v>
       </c>
       <c r="M359" s="114" t="s">
@@ -17157,7 +17902,9 @@
       <c r="C360" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D360" s="132"/>
+      <c r="D360" s="133">
+        <v>33585725</v>
+      </c>
       <c r="E360" s="109" t="s">
         <v>155</v>
       </c>
@@ -17167,7 +17914,19 @@
       <c r="G360" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L360" s="133" t="s">
+      <c r="H360" s="112" t="s">
+        <v>1029</v>
+      </c>
+      <c r="I360" s="111" t="s">
+        <v>992</v>
+      </c>
+      <c r="J360" s="111" t="s">
+        <v>953</v>
+      </c>
+      <c r="K360" s="111" t="s">
+        <v>641</v>
+      </c>
+      <c r="L360" s="132" t="s">
         <v>913</v>
       </c>
       <c r="M360" s="114" t="s">
@@ -17184,7 +17943,9 @@
       <c r="C361" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D361" s="132"/>
+      <c r="D361" s="133">
+        <v>33602786</v>
+      </c>
       <c r="E361" s="109" t="s">
         <v>155</v>
       </c>
@@ -17194,7 +17955,19 @@
       <c r="G361" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L361" s="133" t="s">
+      <c r="H361" s="112" t="s">
+        <v>1030</v>
+      </c>
+      <c r="I361" s="111" t="s">
+        <v>993</v>
+      </c>
+      <c r="J361" s="111" t="s">
+        <v>947</v>
+      </c>
+      <c r="K361" s="111" t="s">
+        <v>948</v>
+      </c>
+      <c r="L361" s="132" t="s">
         <v>915</v>
       </c>
       <c r="M361" s="114" t="s">
@@ -17211,7 +17984,9 @@
       <c r="C362" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D362" s="132"/>
+      <c r="D362" s="133">
+        <v>33574061</v>
+      </c>
       <c r="E362" s="109" t="s">
         <v>155</v>
       </c>
@@ -17221,7 +17996,7 @@
       <c r="G362" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L362" s="133" t="s">
+      <c r="L362" s="132" t="s">
         <v>917</v>
       </c>
       <c r="M362" s="114" t="s">
@@ -17238,7 +18013,9 @@
       <c r="C363" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D363" s="132"/>
+      <c r="D363" s="133">
+        <v>33603712</v>
+      </c>
       <c r="E363" s="109" t="s">
         <v>155</v>
       </c>
@@ -17248,7 +18025,7 @@
       <c r="G363" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L363" s="133" t="s">
+      <c r="L363" s="132" t="s">
         <v>919</v>
       </c>
       <c r="M363" s="114" t="s">
@@ -17265,7 +18042,9 @@
       <c r="C364" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D364" s="132"/>
+      <c r="D364" s="133">
+        <v>33581478</v>
+      </c>
       <c r="E364" s="109" t="s">
         <v>155</v>
       </c>
@@ -17275,7 +18054,7 @@
       <c r="G364" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L364" s="133" t="s">
+      <c r="L364" s="132" t="s">
         <v>922</v>
       </c>
       <c r="M364" s="114" t="s">
@@ -17292,7 +18071,9 @@
       <c r="C365" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D365" s="132"/>
+      <c r="D365" s="133">
+        <v>33571896</v>
+      </c>
       <c r="E365" s="109" t="s">
         <v>155</v>
       </c>
@@ -17302,7 +18083,7 @@
       <c r="G365" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L365" s="133" t="s">
+      <c r="L365" s="132" t="s">
         <v>924</v>
       </c>
       <c r="M365" s="114" t="s">
@@ -17319,7 +18100,9 @@
       <c r="C366" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D366" s="132"/>
+      <c r="D366" s="133">
+        <v>33602734</v>
+      </c>
       <c r="E366" s="109" t="s">
         <v>155</v>
       </c>
@@ -17329,7 +18112,7 @@
       <c r="G366" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L366" s="133" t="s">
+      <c r="L366" s="132" t="s">
         <v>926</v>
       </c>
       <c r="M366" s="114" t="s">
@@ -17346,7 +18129,9 @@
       <c r="C367" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D367" s="132"/>
+      <c r="D367" s="133">
+        <v>33575532</v>
+      </c>
       <c r="E367" s="109" t="s">
         <v>155</v>
       </c>
@@ -17356,7 +18141,7 @@
       <c r="G367" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L367" s="133" t="s">
+      <c r="L367" s="132" t="s">
         <v>928</v>
       </c>
       <c r="M367" s="114" t="s">
@@ -17373,7 +18158,9 @@
       <c r="C368" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D368" s="132"/>
+      <c r="D368" s="133">
+        <v>33585921</v>
+      </c>
       <c r="E368" s="109" t="s">
         <v>155</v>
       </c>
@@ -17383,7 +18170,7 @@
       <c r="G368" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L368" s="133" t="s">
+      <c r="L368" s="132" t="s">
         <v>930</v>
       </c>
       <c r="M368" s="114" t="s">
@@ -17400,7 +18187,9 @@
       <c r="C369" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D369" s="132"/>
+      <c r="D369" s="133">
+        <v>33603487</v>
+      </c>
       <c r="E369" s="109" t="s">
         <v>155</v>
       </c>
@@ -17410,7 +18199,7 @@
       <c r="G369" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L369" s="133" t="s">
+      <c r="L369" s="132" t="s">
         <v>933</v>
       </c>
       <c r="M369" s="114" t="s">

</xml_diff>

<commit_message>
ooredoo event: marked completed the 45 nsa request
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1190" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33C552F9-0481-4126-9BEB-C5050DCF8CA4}"/>
+  <xr:revisionPtr revIDLastSave="1330" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{184B62CC-A911-4BEE-A5B1-18884ADE7200}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="OoredooMasterFile" sheetId="2" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2375" uniqueCount="1031">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2330" uniqueCount="1016">
   <si>
     <t>ICC ID</t>
   </si>
@@ -2578,316 +2578,136 @@
     <t>8997401002188647416</t>
   </si>
   <si>
-    <t>R-13</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:35 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
     <t>8997401002220200976</t>
   </si>
   <si>
-    <t>R-14</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:37 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
     <t>8997401002220200984</t>
   </si>
   <si>
-    <t>R-15</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:38 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
     <t>8997401002220200992</t>
   </si>
   <si>
-    <t>R-16</t>
-  </si>
-  <si>
     <t>8997401002220201099</t>
   </si>
   <si>
-    <t>R-17</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:41 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
     <t>8997401002220201081</t>
   </si>
   <si>
-    <t>R-18</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:42 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
     <t>8997401002220201065</t>
   </si>
   <si>
-    <t>R-19</t>
-  </si>
-  <si>
     <t>8997401002220201008</t>
   </si>
   <si>
-    <t>R-20</t>
-  </si>
-  <si>
     <t>8997401002220201073</t>
   </si>
   <si>
-    <t>R-21</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:45 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
     <t>8997401002220201024</t>
   </si>
   <si>
-    <t>R-22</t>
-  </si>
-  <si>
     <t>8997401002220201032</t>
   </si>
   <si>
-    <t>R-23</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:46 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
     <t>8997401002220201040</t>
   </si>
   <si>
-    <t>R-24</t>
-  </si>
-  <si>
     <t>8997401002220201057</t>
   </si>
   <si>
-    <t>R-25</t>
-  </si>
-  <si>
     <t>8997401002220201107</t>
   </si>
   <si>
-    <t>R-26</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:47 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
     <t>8997401002220201115</t>
   </si>
   <si>
-    <t>R-27</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:48 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
     <t>8997401002220201123</t>
   </si>
   <si>
-    <t>R-28</t>
-  </si>
-  <si>
     <t>8997401002220201131</t>
   </si>
   <si>
-    <t>R-29</t>
-  </si>
-  <si>
     <t>8997401002220201149</t>
   </si>
   <si>
-    <t>R-30</t>
-  </si>
-  <si>
     <t>8997401002220201156</t>
   </si>
   <si>
-    <t>R-31</t>
-  </si>
-  <si>
     <t>8997401002220201164</t>
   </si>
   <si>
-    <t>R-32</t>
-  </si>
-  <si>
     <t>8997401002220201172</t>
   </si>
   <si>
-    <t>R-33</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:49 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
     <t>8997401002220201180</t>
   </si>
   <si>
-    <t>R-34</t>
-  </si>
-  <si>
     <t>8997401002220201198</t>
   </si>
   <si>
-    <t>R-35</t>
-  </si>
-  <si>
     <t>8997401002220201206</t>
   </si>
   <si>
-    <t>R-36</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:50 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
     <t>8997401002220201214</t>
   </si>
   <si>
-    <t>R-37</t>
-  </si>
-  <si>
     <t>8997401002220201222</t>
   </si>
   <si>
-    <t>R-38</t>
-  </si>
-  <si>
     <t>8997401002220201230</t>
   </si>
   <si>
-    <t>R-39</t>
-  </si>
-  <si>
     <t>8997401002220201248</t>
   </si>
   <si>
-    <t>R-40</t>
-  </si>
-  <si>
     <t>8997401002220201255</t>
   </si>
   <si>
-    <t>R-41</t>
-  </si>
-  <si>
     <t>8997401002220201263</t>
   </si>
   <si>
-    <t>R-42</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:51 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
     <t>8997401002220201271</t>
   </si>
   <si>
-    <t>R-43</t>
-  </si>
-  <si>
     <t>8997401002220201289</t>
   </si>
   <si>
-    <t>R-44</t>
-  </si>
-  <si>
     <t>8997401002220201297</t>
   </si>
   <si>
-    <t>R-45</t>
-  </si>
-  <si>
     <t>8997401002220201305</t>
   </si>
   <si>
-    <t>R-46</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:52 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
     <t>8997401002220201313</t>
   </si>
   <si>
-    <t>R-47</t>
-  </si>
-  <si>
     <t>8997401002220201321</t>
   </si>
   <si>
-    <t>R-48</t>
-  </si>
-  <si>
     <t>8997401002220201339</t>
   </si>
   <si>
-    <t>R-49</t>
-  </si>
-  <si>
     <t>8997401002220201347</t>
   </si>
   <si>
-    <t>R-50</t>
-  </si>
-  <si>
     <t>8997401002220201354</t>
   </si>
   <si>
-    <t>R-51</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:53 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
     <t>8997401002220201362</t>
   </si>
   <si>
-    <t>R-52</t>
-  </si>
-  <si>
     <t>8997401002220201370</t>
   </si>
   <si>
-    <t>R-53</t>
-  </si>
-  <si>
     <t>8997401002220201388</t>
   </si>
   <si>
-    <t>R-54</t>
-  </si>
-  <si>
     <t>8997401002220201396</t>
   </si>
   <si>
-    <t>R-55</t>
-  </si>
-  <si>
     <t>8997401002220201404</t>
   </si>
   <si>
-    <t>R-56</t>
-  </si>
-  <si>
-    <t>07-Feb-2023 @11:54 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM</t>
-  </si>
-  <si>
     <t>8997401002220201420</t>
-  </si>
-  <si>
-    <t>R-57</t>
   </si>
   <si>
     <t>PRF # 3197
@@ -3198,6 +3018,186 @@
   </si>
   <si>
     <t>001813 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:35 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33574156 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:37 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33603140 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:38 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33585461 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:38 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33576710 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:41 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33595578 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:42 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33583901 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:42 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33576317 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:42 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33581367 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:45 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33585994 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:45 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33596039 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:46 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33583392 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:46 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33598446 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:46 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33597912 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:47 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33601543 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:48 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33596920 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:48 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33579329 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:48 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33598379 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:48 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33603691 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:48 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33585246 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:48 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33574035 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:49 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33597942 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:49 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33581276 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:49 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33583276 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:50 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33576136 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:50 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33603750 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:50 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33602876 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:50 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33598168 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:50 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33583060 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:50 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33583208 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:51 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33596804 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:51 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33585715 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:51 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33583569 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:51 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33586015 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:52 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33598546 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:52 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33585194 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:52 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33585725 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:52 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33602786 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:52 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33574061 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:53 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33603712 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:53 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33581478 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:53 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33571896 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:53 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33602734 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:53 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33575532 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:54 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33585921 with Plan C</t>
+  </si>
+  <si>
+    <t>07-Feb-2023 @11:54 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
+11-Feb-2023 @20:47 - Request was Completed; Service Number is 33603487 with Plan C</t>
   </si>
 </sst>
 </file>
@@ -3335,7 +3335,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3411,12 +3411,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3567,7 +3561,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3940,12 +3934,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="14" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5288,10 +5276,10 @@
   <dimension ref="A1:W369"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E341" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E360" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D370" sqref="D370"/>
+      <selection pane="bottomRight" activeCell="G363" sqref="G363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15969,7 +15957,7 @@
         <v>44965</v>
       </c>
       <c r="M313" s="99" t="s">
-        <v>934</v>
+        <v>874</v>
       </c>
     </row>
     <row r="314" spans="1:23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -16008,7 +15996,7 @@
         <v>44965</v>
       </c>
       <c r="M314" s="106" t="s">
-        <v>944</v>
+        <v>884</v>
       </c>
     </row>
     <row r="315" spans="1:23" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -16047,7 +16035,7 @@
         <v>44965</v>
       </c>
       <c r="M315" s="106" t="s">
-        <v>935</v>
+        <v>875</v>
       </c>
       <c r="N315"/>
       <c r="O315"/>
@@ -16094,7 +16082,7 @@
         <v>44965</v>
       </c>
       <c r="M316" s="99" t="s">
-        <v>937</v>
+        <v>877</v>
       </c>
       <c r="N316"/>
       <c r="O316"/>
@@ -16143,7 +16131,7 @@
         <v>44965</v>
       </c>
       <c r="M317" s="99" t="s">
-        <v>939</v>
+        <v>879</v>
       </c>
       <c r="N317"/>
       <c r="O317"/>
@@ -16190,7 +16178,7 @@
         <v>44965</v>
       </c>
       <c r="M318" s="99" t="s">
-        <v>943</v>
+        <v>883</v>
       </c>
       <c r="N318"/>
       <c r="O318"/>
@@ -16237,7 +16225,7 @@
         <v>44965</v>
       </c>
       <c r="M319" s="99" t="s">
-        <v>940</v>
+        <v>880</v>
       </c>
       <c r="N319"/>
       <c r="O319"/>
@@ -16288,7 +16276,7 @@
         <v>44965</v>
       </c>
       <c r="M320" s="99" t="s">
-        <v>938</v>
+        <v>878</v>
       </c>
     </row>
     <row r="321" spans="1:23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -16329,7 +16317,7 @@
         <v>44965</v>
       </c>
       <c r="M321" s="99" t="s">
-        <v>936</v>
+        <v>876</v>
       </c>
     </row>
     <row r="322" spans="1:23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -16366,7 +16354,7 @@
         <v>44965</v>
       </c>
       <c r="M322" s="107" t="s">
-        <v>941</v>
+        <v>881</v>
       </c>
     </row>
     <row r="323" spans="1:23" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -16405,7 +16393,7 @@
         <v>44965</v>
       </c>
       <c r="M323" s="99" t="s">
-        <v>942</v>
+        <v>882</v>
       </c>
       <c r="N323"/>
       <c r="O323"/>
@@ -16454,10 +16442,10 @@
         <v>44965</v>
       </c>
       <c r="M324" s="127" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="325" spans="1:23" x14ac:dyDescent="0.3">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="325" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A325" s="108">
         <v>44964</v>
       </c>
@@ -16467,7 +16455,7 @@
       <c r="C325" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D325" s="133">
+      <c r="D325" s="75">
         <v>33574156</v>
       </c>
       <c r="E325" s="109" t="s">
@@ -16480,35 +16468,35 @@
         <v>777</v>
       </c>
       <c r="H325" s="112" t="s">
-        <v>994</v>
+        <v>934</v>
       </c>
       <c r="I325" s="111" t="s">
-        <v>946</v>
+        <v>886</v>
       </c>
       <c r="J325" s="111" t="s">
-        <v>947</v>
+        <v>887</v>
       </c>
       <c r="K325" s="111" t="s">
-        <v>948</v>
-      </c>
-      <c r="L325" s="132" t="s">
-        <v>830</v>
+        <v>888</v>
+      </c>
+      <c r="L325" s="113">
+        <v>44968</v>
       </c>
       <c r="M325" s="114" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="326" spans="1:23" x14ac:dyDescent="0.3">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="326" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A326" s="108">
         <v>44964</v>
       </c>
       <c r="B326" s="109" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="C326" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D326" s="133">
+      <c r="D326" s="75">
         <v>33603140</v>
       </c>
       <c r="E326" s="109" t="s">
@@ -16521,35 +16509,35 @@
         <v>777</v>
       </c>
       <c r="H326" s="112" t="s">
-        <v>995</v>
+        <v>935</v>
       </c>
       <c r="I326" s="111" t="s">
-        <v>949</v>
+        <v>889</v>
       </c>
       <c r="J326" s="111" t="s">
-        <v>950</v>
+        <v>890</v>
       </c>
       <c r="K326" s="111" t="s">
-        <v>951</v>
-      </c>
-      <c r="L326" s="132" t="s">
-        <v>833</v>
+        <v>891</v>
+      </c>
+      <c r="L326" s="113">
+        <v>44968</v>
       </c>
       <c r="M326" s="114" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="327" spans="1:23" x14ac:dyDescent="0.3">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="327" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A327" s="108">
         <v>44964</v>
       </c>
       <c r="B327" s="109" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="C327" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D327" s="133">
+      <c r="D327" s="75">
         <v>33585461</v>
       </c>
       <c r="E327" s="109" t="s">
@@ -16562,35 +16550,35 @@
         <v>777</v>
       </c>
       <c r="H327" s="112" t="s">
-        <v>996</v>
+        <v>936</v>
       </c>
       <c r="I327" s="111" t="s">
-        <v>952</v>
+        <v>892</v>
       </c>
       <c r="J327" s="111" t="s">
-        <v>953</v>
+        <v>893</v>
       </c>
       <c r="K327" s="111" t="s">
         <v>641</v>
       </c>
-      <c r="L327" s="132" t="s">
-        <v>836</v>
+      <c r="L327" s="113">
+        <v>44968</v>
       </c>
       <c r="M327" s="114" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="328" spans="1:23" x14ac:dyDescent="0.3">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="328" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A328" s="108">
         <v>44964</v>
       </c>
       <c r="B328" s="109" t="s">
-        <v>838</v>
+        <v>832</v>
       </c>
       <c r="C328" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D328" s="133">
+      <c r="D328" s="75">
         <v>33576710</v>
       </c>
       <c r="E328" s="109" t="s">
@@ -16603,35 +16591,35 @@
         <v>777</v>
       </c>
       <c r="H328" s="112" t="s">
-        <v>997</v>
+        <v>937</v>
       </c>
       <c r="I328" s="111" t="s">
-        <v>954</v>
+        <v>894</v>
       </c>
       <c r="J328" s="111" t="s">
-        <v>955</v>
+        <v>895</v>
       </c>
       <c r="K328" s="111" t="s">
         <v>641</v>
       </c>
-      <c r="L328" s="132" t="s">
-        <v>839</v>
+      <c r="L328" s="113">
+        <v>44968</v>
       </c>
       <c r="M328" s="114" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="329" spans="1:23" x14ac:dyDescent="0.3">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="329" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A329" s="108">
         <v>44964</v>
       </c>
       <c r="B329" s="109" t="s">
-        <v>840</v>
+        <v>833</v>
       </c>
       <c r="C329" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D329" s="133">
+      <c r="D329" s="75">
         <v>33595578</v>
       </c>
       <c r="E329" s="109" t="s">
@@ -16644,35 +16632,35 @@
         <v>777</v>
       </c>
       <c r="H329" s="112" t="s">
-        <v>998</v>
+        <v>938</v>
       </c>
       <c r="I329" s="111" t="s">
-        <v>956</v>
+        <v>896</v>
       </c>
       <c r="J329" s="111" t="s">
-        <v>957</v>
+        <v>897</v>
       </c>
       <c r="K329" s="111" t="s">
-        <v>951</v>
-      </c>
-      <c r="L329" s="132" t="s">
-        <v>841</v>
+        <v>891</v>
+      </c>
+      <c r="L329" s="113">
+        <v>44968</v>
       </c>
       <c r="M329" s="114" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="330" spans="1:23" x14ac:dyDescent="0.3">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="330" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A330" s="108">
         <v>44964</v>
       </c>
       <c r="B330" s="109" t="s">
-        <v>843</v>
+        <v>834</v>
       </c>
       <c r="C330" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D330" s="133">
+      <c r="D330" s="75">
         <v>33583901</v>
       </c>
       <c r="E330" s="109" t="s">
@@ -16685,35 +16673,35 @@
         <v>777</v>
       </c>
       <c r="H330" s="112" t="s">
-        <v>999</v>
+        <v>939</v>
       </c>
       <c r="I330" s="111" t="s">
-        <v>958</v>
+        <v>898</v>
       </c>
       <c r="J330" s="111" t="s">
-        <v>957</v>
+        <v>897</v>
       </c>
       <c r="K330" s="111" t="s">
-        <v>951</v>
-      </c>
-      <c r="L330" s="132" t="s">
-        <v>844</v>
+        <v>891</v>
+      </c>
+      <c r="L330" s="113">
+        <v>44968</v>
       </c>
       <c r="M330" s="114" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="331" spans="1:23" x14ac:dyDescent="0.3">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="331" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A331" s="108">
         <v>44964</v>
       </c>
       <c r="B331" s="109" t="s">
-        <v>846</v>
+        <v>835</v>
       </c>
       <c r="C331" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D331" s="133">
+      <c r="D331" s="75">
         <v>33576317</v>
       </c>
       <c r="E331" s="109" t="s">
@@ -16726,35 +16714,35 @@
         <v>777</v>
       </c>
       <c r="H331" s="112" t="s">
-        <v>1000</v>
+        <v>940</v>
       </c>
       <c r="I331" s="111" t="s">
-        <v>959</v>
+        <v>899</v>
       </c>
       <c r="J331" s="111" t="s">
-        <v>953</v>
+        <v>893</v>
       </c>
       <c r="K331" s="111" t="s">
         <v>641</v>
       </c>
-      <c r="L331" s="132" t="s">
-        <v>847</v>
+      <c r="L331" s="113">
+        <v>44968</v>
       </c>
       <c r="M331" s="114" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="332" spans="1:23" x14ac:dyDescent="0.3">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="332" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A332" s="108">
         <v>44964</v>
       </c>
       <c r="B332" s="109" t="s">
-        <v>848</v>
+        <v>836</v>
       </c>
       <c r="C332" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D332" s="133">
+      <c r="D332" s="75">
         <v>33581367</v>
       </c>
       <c r="E332" s="109" t="s">
@@ -16767,35 +16755,35 @@
         <v>777</v>
       </c>
       <c r="H332" s="112" t="s">
-        <v>1001</v>
+        <v>941</v>
       </c>
       <c r="I332" s="111" t="s">
-        <v>960</v>
+        <v>900</v>
       </c>
       <c r="J332" s="111" t="s">
-        <v>961</v>
+        <v>901</v>
       </c>
       <c r="K332" s="111" t="s">
-        <v>948</v>
-      </c>
-      <c r="L332" s="132" t="s">
-        <v>849</v>
+        <v>888</v>
+      </c>
+      <c r="L332" s="113">
+        <v>44968</v>
       </c>
       <c r="M332" s="114" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="333" spans="1:23" x14ac:dyDescent="0.3">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="333" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A333" s="108">
         <v>44964</v>
       </c>
       <c r="B333" s="109" t="s">
-        <v>850</v>
+        <v>837</v>
       </c>
       <c r="C333" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D333" s="133">
+      <c r="D333" s="75">
         <v>33585994</v>
       </c>
       <c r="E333" s="109" t="s">
@@ -16808,35 +16796,35 @@
         <v>777</v>
       </c>
       <c r="H333" s="112" t="s">
-        <v>1002</v>
+        <v>942</v>
       </c>
       <c r="I333" s="111" t="s">
-        <v>962</v>
+        <v>902</v>
       </c>
       <c r="J333" s="111" t="s">
-        <v>947</v>
+        <v>887</v>
       </c>
       <c r="K333" s="111" t="s">
-        <v>948</v>
-      </c>
-      <c r="L333" s="132" t="s">
-        <v>851</v>
+        <v>888</v>
+      </c>
+      <c r="L333" s="113">
+        <v>44968</v>
       </c>
       <c r="M333" s="114" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="334" spans="1:23" x14ac:dyDescent="0.3">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="334" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A334" s="108">
         <v>44964</v>
       </c>
       <c r="B334" s="109" t="s">
-        <v>853</v>
+        <v>838</v>
       </c>
       <c r="C334" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D334" s="133">
+      <c r="D334" s="75">
         <v>33596039</v>
       </c>
       <c r="E334" s="109" t="s">
@@ -16849,35 +16837,35 @@
         <v>777</v>
       </c>
       <c r="H334" s="112" t="s">
-        <v>1003</v>
+        <v>943</v>
       </c>
       <c r="I334" s="111" t="s">
-        <v>963</v>
+        <v>903</v>
       </c>
       <c r="J334" s="111" t="s">
-        <v>961</v>
+        <v>901</v>
       </c>
       <c r="K334" s="111" t="s">
-        <v>948</v>
-      </c>
-      <c r="L334" s="132" t="s">
-        <v>854</v>
+        <v>888</v>
+      </c>
+      <c r="L334" s="113">
+        <v>44968</v>
       </c>
       <c r="M334" s="114" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="335" spans="1:23" x14ac:dyDescent="0.3">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="335" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A335" s="108">
         <v>44964</v>
       </c>
       <c r="B335" s="109" t="s">
-        <v>855</v>
+        <v>839</v>
       </c>
       <c r="C335" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D335" s="133">
+      <c r="D335" s="75">
         <v>33583392</v>
       </c>
       <c r="E335" s="109" t="s">
@@ -16890,35 +16878,35 @@
         <v>777</v>
       </c>
       <c r="H335" s="112" t="s">
-        <v>1004</v>
+        <v>944</v>
       </c>
       <c r="I335" s="111" t="s">
-        <v>964</v>
+        <v>904</v>
       </c>
       <c r="J335" s="111" t="s">
-        <v>957</v>
+        <v>897</v>
       </c>
       <c r="K335" s="111" t="s">
-        <v>951</v>
-      </c>
-      <c r="L335" s="132" t="s">
-        <v>856</v>
+        <v>891</v>
+      </c>
+      <c r="L335" s="113">
+        <v>44968</v>
       </c>
       <c r="M335" s="114" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="336" spans="1:23" x14ac:dyDescent="0.3">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="336" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A336" s="108">
         <v>44964</v>
       </c>
       <c r="B336" s="109" t="s">
-        <v>858</v>
+        <v>840</v>
       </c>
       <c r="C336" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D336" s="133">
+      <c r="D336" s="75">
         <v>33598446</v>
       </c>
       <c r="E336" s="109" t="s">
@@ -16931,35 +16919,35 @@
         <v>777</v>
       </c>
       <c r="H336" s="112" t="s">
-        <v>1005</v>
+        <v>945</v>
       </c>
       <c r="I336" s="111" t="s">
-        <v>965</v>
+        <v>905</v>
       </c>
       <c r="J336" s="111" t="s">
-        <v>961</v>
+        <v>901</v>
       </c>
       <c r="K336" s="111" t="s">
         <v>641</v>
       </c>
-      <c r="L336" s="132" t="s">
-        <v>859</v>
+      <c r="L336" s="113">
+        <v>44968</v>
       </c>
       <c r="M336" s="114" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.3">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="337" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A337" s="108">
         <v>44964</v>
       </c>
       <c r="B337" s="109" t="s">
-        <v>860</v>
+        <v>841</v>
       </c>
       <c r="C337" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D337" s="133">
+      <c r="D337" s="75">
         <v>33597912</v>
       </c>
       <c r="E337" s="109" t="s">
@@ -16972,35 +16960,35 @@
         <v>777</v>
       </c>
       <c r="H337" s="112" t="s">
-        <v>1006</v>
+        <v>946</v>
       </c>
       <c r="I337" s="111" t="s">
-        <v>966</v>
+        <v>906</v>
       </c>
       <c r="J337" s="111" t="s">
-        <v>953</v>
+        <v>893</v>
       </c>
       <c r="K337" s="111" t="s">
         <v>641</v>
       </c>
-      <c r="L337" s="132" t="s">
-        <v>861</v>
+      <c r="L337" s="113">
+        <v>44968</v>
       </c>
       <c r="M337" s="114" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="338" spans="1:13" x14ac:dyDescent="0.3">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="338" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A338" s="108">
         <v>44964</v>
       </c>
       <c r="B338" s="109" t="s">
-        <v>862</v>
+        <v>842</v>
       </c>
       <c r="C338" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D338" s="133">
+      <c r="D338" s="75">
         <v>33601543</v>
       </c>
       <c r="E338" s="109" t="s">
@@ -17013,35 +17001,35 @@
         <v>777</v>
       </c>
       <c r="H338" s="112" t="s">
-        <v>1007</v>
+        <v>947</v>
       </c>
       <c r="I338" s="111" t="s">
-        <v>967</v>
+        <v>907</v>
       </c>
       <c r="J338" s="111" t="s">
         <v>268</v>
       </c>
       <c r="K338" s="111" t="s">
-        <v>948</v>
-      </c>
-      <c r="L338" s="132" t="s">
-        <v>863</v>
+        <v>888</v>
+      </c>
+      <c r="L338" s="113">
+        <v>44968</v>
       </c>
       <c r="M338" s="114" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="339" spans="1:13" x14ac:dyDescent="0.3">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="339" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A339" s="108">
         <v>44964</v>
       </c>
       <c r="B339" s="109" t="s">
-        <v>865</v>
+        <v>843</v>
       </c>
       <c r="C339" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D339" s="133">
+      <c r="D339" s="75">
         <v>33596920</v>
       </c>
       <c r="E339" s="109" t="s">
@@ -17054,35 +17042,35 @@
         <v>777</v>
       </c>
       <c r="H339" s="112" t="s">
-        <v>1008</v>
+        <v>948</v>
       </c>
       <c r="I339" s="111" t="s">
-        <v>968</v>
+        <v>908</v>
       </c>
       <c r="J339" s="111" t="s">
-        <v>955</v>
+        <v>895</v>
       </c>
       <c r="K339" s="111" t="s">
-        <v>948</v>
-      </c>
-      <c r="L339" s="132" t="s">
-        <v>866</v>
+        <v>888</v>
+      </c>
+      <c r="L339" s="113">
+        <v>44968</v>
       </c>
       <c r="M339" s="114" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="340" spans="1:13" x14ac:dyDescent="0.3">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="340" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A340" s="108">
         <v>44964</v>
       </c>
       <c r="B340" s="109" t="s">
-        <v>868</v>
+        <v>844</v>
       </c>
       <c r="C340" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D340" s="133">
+      <c r="D340" s="75">
         <v>33579329</v>
       </c>
       <c r="E340" s="109" t="s">
@@ -17095,35 +17083,35 @@
         <v>777</v>
       </c>
       <c r="H340" s="112" t="s">
-        <v>1009</v>
+        <v>949</v>
       </c>
       <c r="I340" s="111" t="s">
-        <v>969</v>
+        <v>909</v>
       </c>
       <c r="J340" s="111" t="s">
-        <v>950</v>
+        <v>890</v>
       </c>
       <c r="K340" s="111" t="s">
         <v>641</v>
       </c>
-      <c r="L340" s="132" t="s">
-        <v>869</v>
+      <c r="L340" s="113">
+        <v>44968</v>
       </c>
       <c r="M340" s="114" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="341" spans="1:13" x14ac:dyDescent="0.3">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="341" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A341" s="108">
         <v>44964</v>
       </c>
       <c r="B341" s="109" t="s">
-        <v>870</v>
+        <v>845</v>
       </c>
       <c r="C341" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D341" s="133">
+      <c r="D341" s="75">
         <v>33598379</v>
       </c>
       <c r="E341" s="109" t="s">
@@ -17136,35 +17124,35 @@
         <v>777</v>
       </c>
       <c r="H341" s="112" t="s">
-        <v>1010</v>
+        <v>950</v>
       </c>
       <c r="I341" s="111" t="s">
-        <v>970</v>
+        <v>910</v>
       </c>
       <c r="J341" s="111" t="s">
-        <v>955</v>
+        <v>895</v>
       </c>
       <c r="K341" s="111" t="s">
-        <v>948</v>
-      </c>
-      <c r="L341" s="132" t="s">
-        <v>871</v>
+        <v>888</v>
+      </c>
+      <c r="L341" s="113">
+        <v>44968</v>
       </c>
       <c r="M341" s="114" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="342" spans="1:13" x14ac:dyDescent="0.3">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="342" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A342" s="108">
         <v>44964</v>
       </c>
       <c r="B342" s="109" t="s">
-        <v>872</v>
+        <v>846</v>
       </c>
       <c r="C342" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D342" s="133">
+      <c r="D342" s="75">
         <v>33603691</v>
       </c>
       <c r="E342" s="109" t="s">
@@ -17177,35 +17165,35 @@
         <v>777</v>
       </c>
       <c r="H342" s="112" t="s">
-        <v>1011</v>
+        <v>951</v>
       </c>
       <c r="I342" s="111" t="s">
-        <v>971</v>
+        <v>911</v>
       </c>
       <c r="J342" s="111" t="s">
-        <v>953</v>
+        <v>893</v>
       </c>
       <c r="K342" s="111" t="s">
         <v>641</v>
       </c>
-      <c r="L342" s="132" t="s">
-        <v>873</v>
+      <c r="L342" s="113">
+        <v>44968</v>
       </c>
       <c r="M342" s="114" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="343" spans="1:13" x14ac:dyDescent="0.3">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="343" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A343" s="108">
         <v>44964</v>
       </c>
       <c r="B343" s="109" t="s">
-        <v>874</v>
+        <v>847</v>
       </c>
       <c r="C343" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D343" s="133">
+      <c r="D343" s="75">
         <v>33585246</v>
       </c>
       <c r="E343" s="109" t="s">
@@ -17218,35 +17206,35 @@
         <v>777</v>
       </c>
       <c r="H343" s="112" t="s">
-        <v>1012</v>
+        <v>952</v>
       </c>
       <c r="I343" s="111" t="s">
-        <v>972</v>
+        <v>912</v>
       </c>
       <c r="J343" s="111" t="s">
-        <v>955</v>
+        <v>895</v>
       </c>
       <c r="K343" s="111" t="s">
-        <v>948</v>
-      </c>
-      <c r="L343" s="132" t="s">
-        <v>875</v>
+        <v>888</v>
+      </c>
+      <c r="L343" s="113">
+        <v>44968</v>
       </c>
       <c r="M343" s="114" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="344" spans="1:13" x14ac:dyDescent="0.3">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="344" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A344" s="108">
         <v>44964</v>
       </c>
       <c r="B344" s="109" t="s">
-        <v>876</v>
+        <v>848</v>
       </c>
       <c r="C344" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D344" s="133">
+      <c r="D344" s="75">
         <v>33574035</v>
       </c>
       <c r="E344" s="109" t="s">
@@ -17259,35 +17247,35 @@
         <v>777</v>
       </c>
       <c r="H344" s="112" t="s">
-        <v>1013</v>
+        <v>953</v>
       </c>
       <c r="I344" s="111" t="s">
-        <v>973</v>
+        <v>913</v>
       </c>
       <c r="J344" s="111" t="s">
-        <v>950</v>
+        <v>890</v>
       </c>
       <c r="K344" s="111" t="s">
         <v>641</v>
       </c>
-      <c r="L344" s="132" t="s">
-        <v>877</v>
+      <c r="L344" s="113">
+        <v>44968</v>
       </c>
       <c r="M344" s="114" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="345" spans="1:13" x14ac:dyDescent="0.3">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="345" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A345" s="108">
         <v>44964</v>
       </c>
       <c r="B345" s="109" t="s">
-        <v>878</v>
+        <v>849</v>
       </c>
       <c r="C345" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D345" s="133">
+      <c r="D345" s="75">
         <v>33597942</v>
       </c>
       <c r="E345" s="109" t="s">
@@ -17300,35 +17288,35 @@
         <v>777</v>
       </c>
       <c r="H345" s="112" t="s">
-        <v>1014</v>
+        <v>954</v>
       </c>
       <c r="I345" s="111" t="s">
-        <v>974</v>
+        <v>914</v>
       </c>
       <c r="J345" s="111" t="s">
-        <v>953</v>
+        <v>893</v>
       </c>
       <c r="K345" s="111" t="s">
         <v>641</v>
       </c>
-      <c r="L345" s="132" t="s">
-        <v>879</v>
+      <c r="L345" s="113">
+        <v>44968</v>
       </c>
       <c r="M345" s="114" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="346" spans="1:13" x14ac:dyDescent="0.3">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="346" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A346" s="108">
         <v>44964</v>
       </c>
       <c r="B346" s="109" t="s">
-        <v>881</v>
+        <v>850</v>
       </c>
       <c r="C346" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D346" s="133">
+      <c r="D346" s="75">
         <v>33581276</v>
       </c>
       <c r="E346" s="109" t="s">
@@ -17341,35 +17329,35 @@
         <v>777</v>
       </c>
       <c r="H346" s="112" t="s">
-        <v>1015</v>
+        <v>955</v>
       </c>
       <c r="I346" s="111" t="s">
-        <v>975</v>
+        <v>915</v>
       </c>
       <c r="J346" s="111" t="s">
-        <v>955</v>
+        <v>895</v>
       </c>
       <c r="K346" s="111" t="s">
-        <v>948</v>
-      </c>
-      <c r="L346" s="132" t="s">
-        <v>882</v>
+        <v>888</v>
+      </c>
+      <c r="L346" s="113">
+        <v>44968</v>
       </c>
       <c r="M346" s="114" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="347" spans="1:13" x14ac:dyDescent="0.3">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="347" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A347" s="108">
         <v>44964</v>
       </c>
       <c r="B347" s="109" t="s">
-        <v>883</v>
+        <v>851</v>
       </c>
       <c r="C347" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D347" s="133">
+      <c r="D347" s="75">
         <v>33583276</v>
       </c>
       <c r="E347" s="109" t="s">
@@ -17382,35 +17370,35 @@
         <v>777</v>
       </c>
       <c r="H347" s="112" t="s">
-        <v>1016</v>
+        <v>956</v>
       </c>
       <c r="I347" s="111" t="s">
-        <v>976</v>
+        <v>916</v>
       </c>
       <c r="J347" s="111" t="s">
-        <v>961</v>
+        <v>901</v>
       </c>
       <c r="K347" s="111" t="s">
-        <v>948</v>
-      </c>
-      <c r="L347" s="132" t="s">
-        <v>884</v>
+        <v>888</v>
+      </c>
+      <c r="L347" s="113">
+        <v>44968</v>
       </c>
       <c r="M347" s="114" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="348" spans="1:13" x14ac:dyDescent="0.3">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="348" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A348" s="108">
         <v>44964</v>
       </c>
       <c r="B348" s="109" t="s">
-        <v>885</v>
+        <v>852</v>
       </c>
       <c r="C348" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D348" s="133">
+      <c r="D348" s="75">
         <v>33576136</v>
       </c>
       <c r="E348" s="109" t="s">
@@ -17423,35 +17411,35 @@
         <v>777</v>
       </c>
       <c r="H348" s="112" t="s">
-        <v>1017</v>
+        <v>957</v>
       </c>
       <c r="I348" s="111" t="s">
-        <v>977</v>
+        <v>917</v>
       </c>
       <c r="J348" s="111" t="s">
-        <v>947</v>
+        <v>887</v>
       </c>
       <c r="K348" s="111" t="s">
-        <v>948</v>
-      </c>
-      <c r="L348" s="132" t="s">
-        <v>886</v>
+        <v>888</v>
+      </c>
+      <c r="L348" s="113">
+        <v>44968</v>
       </c>
       <c r="M348" s="114" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="349" spans="1:13" x14ac:dyDescent="0.3">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="349" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A349" s="108">
         <v>44964</v>
       </c>
       <c r="B349" s="109" t="s">
-        <v>888</v>
+        <v>853</v>
       </c>
       <c r="C349" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D349" s="133">
+      <c r="D349" s="75">
         <v>33603750</v>
       </c>
       <c r="E349" s="109" t="s">
@@ -17464,35 +17452,35 @@
         <v>777</v>
       </c>
       <c r="H349" s="112" t="s">
-        <v>1018</v>
+        <v>958</v>
       </c>
       <c r="I349" s="111" t="s">
-        <v>978</v>
+        <v>918</v>
       </c>
       <c r="J349" s="111" t="s">
-        <v>979</v>
+        <v>919</v>
       </c>
       <c r="K349" s="111" t="s">
-        <v>951</v>
-      </c>
-      <c r="L349" s="132" t="s">
-        <v>889</v>
+        <v>891</v>
+      </c>
+      <c r="L349" s="113">
+        <v>44968</v>
       </c>
       <c r="M349" s="114" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="350" spans="1:13" x14ac:dyDescent="0.3">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="350" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A350" s="108">
         <v>44964</v>
       </c>
       <c r="B350" s="109" t="s">
-        <v>890</v>
+        <v>854</v>
       </c>
       <c r="C350" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D350" s="133">
+      <c r="D350" s="75">
         <v>33602876</v>
       </c>
       <c r="E350" s="109" t="s">
@@ -17505,35 +17493,35 @@
         <v>777</v>
       </c>
       <c r="H350" s="112" t="s">
-        <v>1019</v>
+        <v>959</v>
       </c>
       <c r="I350" s="111" t="s">
-        <v>980</v>
+        <v>920</v>
       </c>
       <c r="J350" s="111" t="s">
-        <v>955</v>
+        <v>895</v>
       </c>
       <c r="K350" s="111" t="s">
-        <v>948</v>
-      </c>
-      <c r="L350" s="132" t="s">
-        <v>891</v>
+        <v>888</v>
+      </c>
+      <c r="L350" s="113">
+        <v>44968</v>
       </c>
       <c r="M350" s="114" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="351" spans="1:13" x14ac:dyDescent="0.3">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="351" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A351" s="108">
         <v>44964</v>
       </c>
       <c r="B351" s="109" t="s">
-        <v>892</v>
+        <v>855</v>
       </c>
       <c r="C351" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D351" s="133">
+      <c r="D351" s="75">
         <v>33598168</v>
       </c>
       <c r="E351" s="109" t="s">
@@ -17546,35 +17534,35 @@
         <v>777</v>
       </c>
       <c r="H351" s="112" t="s">
-        <v>1020</v>
+        <v>960</v>
       </c>
       <c r="I351" s="111" t="s">
-        <v>981</v>
+        <v>921</v>
       </c>
       <c r="J351" s="111" t="s">
-        <v>947</v>
+        <v>887</v>
       </c>
       <c r="K351" s="111" t="s">
-        <v>948</v>
-      </c>
-      <c r="L351" s="132" t="s">
-        <v>893</v>
+        <v>888</v>
+      </c>
+      <c r="L351" s="113">
+        <v>44968</v>
       </c>
       <c r="M351" s="114" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="352" spans="1:13" x14ac:dyDescent="0.3">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="352" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A352" s="108">
         <v>44964</v>
       </c>
       <c r="B352" s="109" t="s">
-        <v>894</v>
+        <v>856</v>
       </c>
       <c r="C352" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D352" s="133">
+      <c r="D352" s="75">
         <v>33583060</v>
       </c>
       <c r="E352" s="109" t="s">
@@ -17587,35 +17575,35 @@
         <v>777</v>
       </c>
       <c r="H352" s="112" t="s">
-        <v>1021</v>
+        <v>961</v>
       </c>
       <c r="I352" s="111" t="s">
-        <v>982</v>
+        <v>922</v>
       </c>
       <c r="J352" s="111" t="s">
-        <v>947</v>
+        <v>887</v>
       </c>
       <c r="K352" s="111" t="s">
-        <v>948</v>
-      </c>
-      <c r="L352" s="132" t="s">
-        <v>895</v>
+        <v>888</v>
+      </c>
+      <c r="L352" s="113">
+        <v>44968</v>
       </c>
       <c r="M352" s="114" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="353" spans="1:13" x14ac:dyDescent="0.3">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="353" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A353" s="108">
         <v>44964</v>
       </c>
       <c r="B353" s="109" t="s">
-        <v>896</v>
+        <v>857</v>
       </c>
       <c r="C353" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D353" s="133">
+      <c r="D353" s="75">
         <v>33583208</v>
       </c>
       <c r="E353" s="109" t="s">
@@ -17628,35 +17616,35 @@
         <v>777</v>
       </c>
       <c r="H353" s="112" t="s">
-        <v>1022</v>
+        <v>962</v>
       </c>
       <c r="I353" s="111" t="s">
-        <v>983</v>
+        <v>923</v>
       </c>
       <c r="J353" s="111" t="s">
-        <v>953</v>
+        <v>893</v>
       </c>
       <c r="K353" s="111" t="s">
         <v>641</v>
       </c>
-      <c r="L353" s="132" t="s">
-        <v>897</v>
+      <c r="L353" s="113">
+        <v>44968</v>
       </c>
       <c r="M353" s="114" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="354" spans="1:13" x14ac:dyDescent="0.3">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="354" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A354" s="108">
         <v>44964</v>
       </c>
       <c r="B354" s="109" t="s">
-        <v>898</v>
+        <v>858</v>
       </c>
       <c r="C354" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D354" s="133">
+      <c r="D354" s="75">
         <v>33596804</v>
       </c>
       <c r="E354" s="109" t="s">
@@ -17669,35 +17657,35 @@
         <v>777</v>
       </c>
       <c r="H354" s="112" t="s">
-        <v>1023</v>
+        <v>963</v>
       </c>
       <c r="I354" s="111" t="s">
-        <v>984</v>
+        <v>924</v>
       </c>
       <c r="J354" s="111" t="s">
-        <v>950</v>
+        <v>890</v>
       </c>
       <c r="K354" s="111" t="s">
         <v>641</v>
       </c>
-      <c r="L354" s="132" t="s">
-        <v>899</v>
+      <c r="L354" s="113">
+        <v>44968</v>
       </c>
       <c r="M354" s="114" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="355" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="355" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A355" s="108">
         <v>44964</v>
       </c>
       <c r="B355" s="109" t="s">
-        <v>901</v>
+        <v>859</v>
       </c>
       <c r="C355" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D355" s="133">
+      <c r="D355" s="75">
         <v>33585715</v>
       </c>
       <c r="E355" s="109" t="s">
@@ -17710,35 +17698,35 @@
         <v>777</v>
       </c>
       <c r="H355" s="112" t="s">
-        <v>1024</v>
+        <v>964</v>
       </c>
       <c r="I355" s="111" t="s">
-        <v>985</v>
+        <v>925</v>
       </c>
       <c r="J355" s="111" t="s">
-        <v>953</v>
+        <v>893</v>
       </c>
       <c r="K355" s="111" t="s">
         <v>641</v>
       </c>
-      <c r="L355" s="132" t="s">
-        <v>902</v>
+      <c r="L355" s="113">
+        <v>44968</v>
       </c>
       <c r="M355" s="114" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="356" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="356" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A356" s="108">
         <v>44964</v>
       </c>
       <c r="B356" s="109" t="s">
-        <v>903</v>
+        <v>860</v>
       </c>
       <c r="C356" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D356" s="133">
+      <c r="D356" s="75">
         <v>33583569</v>
       </c>
       <c r="E356" s="109" t="s">
@@ -17751,35 +17739,35 @@
         <v>777</v>
       </c>
       <c r="H356" s="112" t="s">
-        <v>1025</v>
+        <v>965</v>
       </c>
       <c r="I356" s="111" t="s">
-        <v>986</v>
+        <v>926</v>
       </c>
       <c r="J356" s="111" t="s">
-        <v>955</v>
+        <v>895</v>
       </c>
       <c r="K356" s="111" t="s">
-        <v>948</v>
-      </c>
-      <c r="L356" s="132" t="s">
-        <v>904</v>
+        <v>888</v>
+      </c>
+      <c r="L356" s="113">
+        <v>44968</v>
       </c>
       <c r="M356" s="114" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="357" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="357" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A357" s="108">
         <v>44964</v>
       </c>
       <c r="B357" s="109" t="s">
-        <v>905</v>
+        <v>861</v>
       </c>
       <c r="C357" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D357" s="133">
+      <c r="D357" s="75">
         <v>33586015</v>
       </c>
       <c r="E357" s="109" t="s">
@@ -17792,35 +17780,35 @@
         <v>777</v>
       </c>
       <c r="H357" s="112" t="s">
-        <v>1026</v>
+        <v>966</v>
       </c>
       <c r="I357" s="111" t="s">
-        <v>987</v>
+        <v>927</v>
       </c>
       <c r="J357" s="111" t="s">
-        <v>955</v>
+        <v>895</v>
       </c>
       <c r="K357" s="111" t="s">
-        <v>948</v>
-      </c>
-      <c r="L357" s="132" t="s">
-        <v>906</v>
+        <v>888</v>
+      </c>
+      <c r="L357" s="113">
+        <v>44968</v>
       </c>
       <c r="M357" s="114" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="358" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="358" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A358" s="108">
         <v>44964</v>
       </c>
       <c r="B358" s="109" t="s">
-        <v>907</v>
+        <v>862</v>
       </c>
       <c r="C358" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D358" s="133">
+      <c r="D358" s="75">
         <v>33598546</v>
       </c>
       <c r="E358" s="109" t="s">
@@ -17833,35 +17821,35 @@
         <v>777</v>
       </c>
       <c r="H358" s="112" t="s">
-        <v>1027</v>
+        <v>967</v>
       </c>
       <c r="I358" s="111" t="s">
-        <v>988</v>
+        <v>928</v>
       </c>
       <c r="J358" s="111" t="s">
-        <v>989</v>
+        <v>929</v>
       </c>
       <c r="K358" s="111" t="s">
         <v>641</v>
       </c>
-      <c r="L358" s="132" t="s">
-        <v>908</v>
+      <c r="L358" s="113">
+        <v>44968</v>
       </c>
       <c r="M358" s="114" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="359" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="359" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A359" s="108">
         <v>44964</v>
       </c>
       <c r="B359" s="109" t="s">
-        <v>910</v>
+        <v>863</v>
       </c>
       <c r="C359" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D359" s="133">
+      <c r="D359" s="75">
         <v>33585194</v>
       </c>
       <c r="E359" s="109" t="s">
@@ -17874,35 +17862,35 @@
         <v>777</v>
       </c>
       <c r="H359" s="112" t="s">
-        <v>1028</v>
+        <v>968</v>
       </c>
       <c r="I359" s="111" t="s">
-        <v>990</v>
+        <v>930</v>
       </c>
       <c r="J359" s="111" t="s">
-        <v>991</v>
+        <v>931</v>
       </c>
       <c r="K359" s="111" t="s">
         <v>641</v>
       </c>
-      <c r="L359" s="132" t="s">
-        <v>911</v>
+      <c r="L359" s="113">
+        <v>44968</v>
       </c>
       <c r="M359" s="114" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="360" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="360" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A360" s="108">
         <v>44964</v>
       </c>
       <c r="B360" s="109" t="s">
-        <v>912</v>
+        <v>864</v>
       </c>
       <c r="C360" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D360" s="133">
+      <c r="D360" s="75">
         <v>33585725</v>
       </c>
       <c r="E360" s="109" t="s">
@@ -17915,35 +17903,35 @@
         <v>777</v>
       </c>
       <c r="H360" s="112" t="s">
-        <v>1029</v>
+        <v>969</v>
       </c>
       <c r="I360" s="111" t="s">
-        <v>992</v>
+        <v>932</v>
       </c>
       <c r="J360" s="111" t="s">
-        <v>953</v>
+        <v>893</v>
       </c>
       <c r="K360" s="111" t="s">
         <v>641</v>
       </c>
-      <c r="L360" s="132" t="s">
-        <v>913</v>
+      <c r="L360" s="113">
+        <v>44968</v>
       </c>
       <c r="M360" s="114" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="361" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="361" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A361" s="108">
         <v>44964</v>
       </c>
       <c r="B361" s="109" t="s">
-        <v>914</v>
+        <v>865</v>
       </c>
       <c r="C361" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D361" s="133">
+      <c r="D361" s="75">
         <v>33602786</v>
       </c>
       <c r="E361" s="109" t="s">
@@ -17956,35 +17944,35 @@
         <v>777</v>
       </c>
       <c r="H361" s="112" t="s">
-        <v>1030</v>
+        <v>970</v>
       </c>
       <c r="I361" s="111" t="s">
-        <v>993</v>
+        <v>933</v>
       </c>
       <c r="J361" s="111" t="s">
-        <v>947</v>
+        <v>887</v>
       </c>
       <c r="K361" s="111" t="s">
-        <v>948</v>
-      </c>
-      <c r="L361" s="132" t="s">
-        <v>915</v>
+        <v>888</v>
+      </c>
+      <c r="L361" s="113">
+        <v>44968</v>
       </c>
       <c r="M361" s="114" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="362" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="362" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A362" s="108">
         <v>44964</v>
       </c>
       <c r="B362" s="109" t="s">
-        <v>916</v>
+        <v>866</v>
       </c>
       <c r="C362" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D362" s="133">
+      <c r="D362" s="75">
         <v>33574061</v>
       </c>
       <c r="E362" s="109" t="s">
@@ -17996,24 +17984,24 @@
       <c r="G362" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L362" s="132" t="s">
-        <v>917</v>
+      <c r="L362" s="113">
+        <v>44968</v>
       </c>
       <c r="M362" s="114" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="363" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="363" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A363" s="108">
         <v>44964</v>
       </c>
       <c r="B363" s="109" t="s">
-        <v>918</v>
+        <v>867</v>
       </c>
       <c r="C363" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D363" s="133">
+      <c r="D363" s="75">
         <v>33603712</v>
       </c>
       <c r="E363" s="109" t="s">
@@ -18025,24 +18013,24 @@
       <c r="G363" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L363" s="132" t="s">
-        <v>919</v>
+      <c r="L363" s="113">
+        <v>44968</v>
       </c>
       <c r="M363" s="114" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="364" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="364" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A364" s="108">
         <v>44964</v>
       </c>
       <c r="B364" s="109" t="s">
-        <v>921</v>
+        <v>868</v>
       </c>
       <c r="C364" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D364" s="133">
+      <c r="D364" s="75">
         <v>33581478</v>
       </c>
       <c r="E364" s="109" t="s">
@@ -18054,24 +18042,24 @@
       <c r="G364" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L364" s="132" t="s">
-        <v>922</v>
+      <c r="L364" s="113">
+        <v>44968</v>
       </c>
       <c r="M364" s="114" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="365" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="365" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A365" s="108">
         <v>44964</v>
       </c>
       <c r="B365" s="109" t="s">
-        <v>923</v>
+        <v>869</v>
       </c>
       <c r="C365" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D365" s="133">
+      <c r="D365" s="75">
         <v>33571896</v>
       </c>
       <c r="E365" s="109" t="s">
@@ -18083,24 +18071,24 @@
       <c r="G365" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L365" s="132" t="s">
-        <v>924</v>
+      <c r="L365" s="113">
+        <v>44968</v>
       </c>
       <c r="M365" s="114" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="366" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="366" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A366" s="108">
         <v>44964</v>
       </c>
       <c r="B366" s="109" t="s">
-        <v>925</v>
+        <v>870</v>
       </c>
       <c r="C366" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D366" s="133">
+      <c r="D366" s="75">
         <v>33602734</v>
       </c>
       <c r="E366" s="109" t="s">
@@ -18112,24 +18100,24 @@
       <c r="G366" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L366" s="132" t="s">
-        <v>926</v>
+      <c r="L366" s="113">
+        <v>44968</v>
       </c>
       <c r="M366" s="114" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="367" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="367" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A367" s="108">
         <v>44964</v>
       </c>
       <c r="B367" s="109" t="s">
-        <v>927</v>
+        <v>871</v>
       </c>
       <c r="C367" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D367" s="133">
+      <c r="D367" s="75">
         <v>33575532</v>
       </c>
       <c r="E367" s="109" t="s">
@@ -18141,24 +18129,24 @@
       <c r="G367" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L367" s="132" t="s">
-        <v>928</v>
+      <c r="L367" s="113">
+        <v>44968</v>
       </c>
       <c r="M367" s="114" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="368" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="368" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A368" s="108">
         <v>44964</v>
       </c>
       <c r="B368" s="109" t="s">
-        <v>929</v>
+        <v>872</v>
       </c>
       <c r="C368" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D368" s="133">
+      <c r="D368" s="75">
         <v>33585921</v>
       </c>
       <c r="E368" s="109" t="s">
@@ -18170,24 +18158,24 @@
       <c r="G368" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L368" s="132" t="s">
-        <v>930</v>
+      <c r="L368" s="113">
+        <v>44968</v>
       </c>
       <c r="M368" s="114" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="369" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="369" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A369" s="108">
         <v>44964</v>
       </c>
       <c r="B369" s="109" t="s">
-        <v>932</v>
+        <v>873</v>
       </c>
       <c r="C369" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D369" s="133">
+      <c r="D369" s="75">
         <v>33603487</v>
       </c>
       <c r="E369" s="109" t="s">
@@ -18199,11 +18187,11 @@
       <c r="G369" s="111" t="s">
         <v>777</v>
       </c>
-      <c r="L369" s="132" t="s">
-        <v>933</v>
+      <c r="L369" s="113">
+        <v>44968</v>
       </c>
       <c r="M369" s="114" t="s">
-        <v>931</v>
+        <v>1015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ooredoo event: applied details for 8 remaining MEP
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1330" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{184B62CC-A911-4BEE-A5B1-18884ADE7200}"/>
+  <xr:revisionPtr revIDLastSave="1355" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A22FB05-DC7F-45E0-8092-6D459340A1FD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2330" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2362" uniqueCount="1037">
   <si>
     <t>ICC ID</t>
   </si>
@@ -3198,6 +3198,69 @@
   <si>
     <t>07-Feb-2023 @11:54 - Ooredoo Sim Requested with Plan C; 45 MEP Staff Sim Request as per GM
 11-Feb-2023 @20:47 - Request was Completed; Service Number is 33603487 with Plan C</t>
+  </si>
+  <si>
+    <t>MOHAMMED IBRAHIM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRANK KATAMBA </t>
+  </si>
+  <si>
+    <t>SOTHIRASA SELLAMANI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SENIOR HVAC TECHNICIAN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHERAZ ARSHAD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MD REJBI AHAMED </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DARWIN VISTA </t>
+  </si>
+  <si>
+    <t>SENIOR MAINTENANCE TECHNICIAN</t>
+  </si>
+  <si>
+    <t>SENIOR MECHANICAL TECHNICIAN (PIC)</t>
+  </si>
+  <si>
+    <t>HVAC TECHNICIAN  (PIC)</t>
+  </si>
+  <si>
+    <t>001826 - MEP</t>
+  </si>
+  <si>
+    <t>000718 - MEP</t>
+  </si>
+  <si>
+    <t>001840 - MEP</t>
+  </si>
+  <si>
+    <t>001865 - MEP</t>
+  </si>
+  <si>
+    <t>000846 - MEP</t>
+  </si>
+  <si>
+    <t>001368 - MEP</t>
+  </si>
+  <si>
+    <t>001800 - MEP</t>
+  </si>
+  <si>
+    <t>001530 - MEP</t>
+  </si>
+  <si>
+    <t>BMS OPERATOR</t>
+  </si>
+  <si>
+    <t>NOMAN SHAH</t>
+  </si>
+  <si>
+    <t>MOHAMMAD SHAMIM</t>
   </si>
 </sst>
 </file>
@@ -3943,6 +4006,579 @@
   </cellStyles>
   <dxfs count="75">
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <u val="double"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -4348,579 +4984,6 @@
         </horizontal>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <u val="double"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4941,25 +5004,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}" name="OoredooActiveUsers" displayName="OoredooActiveUsers" ref="A2:M369" headerRowDxfId="17" totalsRowDxfId="14" headerRowBorderDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}" name="OoredooActiveUsers" displayName="OoredooActiveUsers" ref="A2:M369" headerRowDxfId="74" totalsRowDxfId="71" headerRowBorderDxfId="73" tableBorderDxfId="72">
   <autoFilter ref="A2:M369" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:M324">
     <sortCondition ref="A2:A323"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{04FAFA61-B55D-4A3B-9F7F-E5235C6B0C57}" name="Date Requested/Date Last Modified" totalsRowLabel="Total" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{DFF4E101-F3A1-41F6-BD45-E2AA15F2F6D6}" name="ICC ID" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{DC1A38D8-E152-4538-AB7B-5271462660B2}" name="Request Type" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{ECF686BF-8B19-4235-B13B-9DB19EC39696}" name="MSISDN" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{C8A5C358-D0E1-484F-AA20-0133965F8A62}" name="Current Plan" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{EE7C2EE9-27A5-4C0E-AB88-DD1DDA81C0F1}" name="Plan Rate" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{75A60B80-9E05-4910-AD92-7AEDA7965E82}" name="Category/Location" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{1322683F-6244-4779-8AE4-4850E20CB5A3}" name="Employee No./Department" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{55D64C5A-D4E1-4BEB-BDA9-D80326A95532}" name="NAME" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{961CD649-F349-40D3-B59B-1E63441377B2}" name="Designation" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{BFBB0D34-92DE-44B7-833E-D9456CD4F70F}" name="Staff Grade" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{A8C5E603-61F1-492C-8C18-4E7F13573D41}" name="Request Completion Date" dataDxfId="1"/>
-    <tableColumn id="15" xr3:uid="{A4FDF428-1629-4A29-B8FB-679D6B99BC5A}" name="Remarks" totalsRowFunction="count" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{04FAFA61-B55D-4A3B-9F7F-E5235C6B0C57}" name="Date Requested/Date Last Modified" totalsRowLabel="Total" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{DFF4E101-F3A1-41F6-BD45-E2AA15F2F6D6}" name="ICC ID" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{DC1A38D8-E152-4538-AB7B-5271462660B2}" name="Request Type" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{ECF686BF-8B19-4235-B13B-9DB19EC39696}" name="MSISDN" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="7" xr3:uid="{C8A5C358-D0E1-484F-AA20-0133965F8A62}" name="Current Plan" dataDxfId="65"/>
+    <tableColumn id="8" xr3:uid="{EE7C2EE9-27A5-4C0E-AB88-DD1DDA81C0F1}" name="Plan Rate" dataDxfId="64"/>
+    <tableColumn id="9" xr3:uid="{75A60B80-9E05-4910-AD92-7AEDA7965E82}" name="Category/Location" dataDxfId="63"/>
+    <tableColumn id="10" xr3:uid="{1322683F-6244-4779-8AE4-4850E20CB5A3}" name="Employee No./Department" dataDxfId="62"/>
+    <tableColumn id="11" xr3:uid="{55D64C5A-D4E1-4BEB-BDA9-D80326A95532}" name="NAME" dataDxfId="61"/>
+    <tableColumn id="12" xr3:uid="{961CD649-F349-40D3-B59B-1E63441377B2}" name="Designation" dataDxfId="60"/>
+    <tableColumn id="13" xr3:uid="{BFBB0D34-92DE-44B7-833E-D9456CD4F70F}" name="Staff Grade" dataDxfId="59"/>
+    <tableColumn id="14" xr3:uid="{A8C5E603-61F1-492C-8C18-4E7F13573D41}" name="Request Completion Date" dataDxfId="58"/>
+    <tableColumn id="15" xr3:uid="{A4FDF428-1629-4A29-B8FB-679D6B99BC5A}" name="Remarks" totalsRowFunction="count" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5279,7 +5342,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E360" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G363" sqref="G363"/>
+      <selection pane="bottomRight" activeCell="A369" sqref="A369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17984,6 +18047,18 @@
       <c r="G362" s="111" t="s">
         <v>777</v>
       </c>
+      <c r="H362" s="112" t="s">
+        <v>1026</v>
+      </c>
+      <c r="I362" s="111" t="s">
+        <v>1016</v>
+      </c>
+      <c r="J362" s="111" t="s">
+        <v>1024</v>
+      </c>
+      <c r="K362" s="111" t="s">
+        <v>888</v>
+      </c>
       <c r="L362" s="113">
         <v>44968</v>
       </c>
@@ -18013,6 +18088,18 @@
       <c r="G363" s="111" t="s">
         <v>777</v>
       </c>
+      <c r="H363" s="112" t="s">
+        <v>1027</v>
+      </c>
+      <c r="I363" s="111" t="s">
+        <v>1017</v>
+      </c>
+      <c r="J363" s="111" t="s">
+        <v>1025</v>
+      </c>
+      <c r="K363" s="111" t="s">
+        <v>641</v>
+      </c>
       <c r="L363" s="113">
         <v>44968</v>
       </c>
@@ -18042,6 +18129,18 @@
       <c r="G364" s="111" t="s">
         <v>777</v>
       </c>
+      <c r="H364" s="112" t="s">
+        <v>1028</v>
+      </c>
+      <c r="I364" s="111" t="s">
+        <v>1018</v>
+      </c>
+      <c r="J364" s="111" t="s">
+        <v>1019</v>
+      </c>
+      <c r="K364" s="111" t="s">
+        <v>888</v>
+      </c>
       <c r="L364" s="113">
         <v>44968</v>
       </c>
@@ -18071,6 +18170,18 @@
       <c r="G365" s="111" t="s">
         <v>777</v>
       </c>
+      <c r="H365" s="112" t="s">
+        <v>1029</v>
+      </c>
+      <c r="I365" s="111" t="s">
+        <v>1020</v>
+      </c>
+      <c r="J365" s="111" t="s">
+        <v>887</v>
+      </c>
+      <c r="K365" s="111" t="s">
+        <v>888</v>
+      </c>
       <c r="L365" s="113">
         <v>44968</v>
       </c>
@@ -18100,6 +18211,18 @@
       <c r="G366" s="111" t="s">
         <v>777</v>
       </c>
+      <c r="H366" s="112" t="s">
+        <v>1030</v>
+      </c>
+      <c r="I366" s="111" t="s">
+        <v>1021</v>
+      </c>
+      <c r="J366" s="111" t="s">
+        <v>895</v>
+      </c>
+      <c r="K366" s="111" t="s">
+        <v>888</v>
+      </c>
       <c r="L366" s="113">
         <v>44968</v>
       </c>
@@ -18129,6 +18252,18 @@
       <c r="G367" s="111" t="s">
         <v>777</v>
       </c>
+      <c r="H367" s="112" t="s">
+        <v>1031</v>
+      </c>
+      <c r="I367" s="111" t="s">
+        <v>1022</v>
+      </c>
+      <c r="J367" s="111" t="s">
+        <v>1023</v>
+      </c>
+      <c r="K367" s="111" t="s">
+        <v>888</v>
+      </c>
       <c r="L367" s="113">
         <v>44968</v>
       </c>
@@ -18158,6 +18293,18 @@
       <c r="G368" s="111" t="s">
         <v>777</v>
       </c>
+      <c r="H368" s="112" t="s">
+        <v>1032</v>
+      </c>
+      <c r="I368" s="111" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J368" s="111" t="s">
+        <v>890</v>
+      </c>
+      <c r="K368" s="111" t="s">
+        <v>641</v>
+      </c>
       <c r="L368" s="113">
         <v>44968</v>
       </c>
@@ -18186,6 +18333,18 @@
       </c>
       <c r="G369" s="111" t="s">
         <v>777</v>
+      </c>
+      <c r="H369" s="112" t="s">
+        <v>1033</v>
+      </c>
+      <c r="I369" s="111" t="s">
+        <v>1036</v>
+      </c>
+      <c r="J369" s="111" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K369" s="111" t="s">
+        <v>641</v>
       </c>
       <c r="L369" s="113">
         <v>44968</v>
@@ -18200,128 +18359,106 @@
     <protectedRange algorithmName="SHA-512" hashValue="VOn69kCIhJPEp5fNyicRsZTWI4n6cpwYePqeJDn2AdBqyZDxUDzXUErBOdnjSHJCqzM2mdxlwA6ZKQ3eZHgJGw==" saltValue="K/CRNethjJZ2P0+HnPZE0g==" spinCount="100000" sqref="H283" name="Range1_1"/>
   </protectedRanges>
   <phoneticPr fontId="11" type="noConversion"/>
-  <conditionalFormatting sqref="D315:D316 D1:D241 D243:D283">
-    <cfRule type="duplicateValues" dxfId="74" priority="46"/>
+  <conditionalFormatting sqref="D1:D241 D243:D283 D315:D316">
+    <cfRule type="duplicateValues" dxfId="56" priority="46"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D241 D243:D295 D315:D316">
+    <cfRule type="duplicateValues" dxfId="55" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="34"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11:D1048576">
+    <cfRule type="duplicateValues" dxfId="52" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D284">
-    <cfRule type="duplicateValues" dxfId="73" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D285:D286">
-    <cfRule type="duplicateValues" dxfId="72" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D287">
-    <cfRule type="duplicateValues" dxfId="71" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D288:D289">
-    <cfRule type="duplicateValues" dxfId="70" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D290">
-    <cfRule type="duplicateValues" dxfId="69" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D291:D292">
-    <cfRule type="duplicateValues" dxfId="68" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D293">
-    <cfRule type="duplicateValues" dxfId="67" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D294:D295">
-    <cfRule type="duplicateValues" dxfId="66" priority="38"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D315:D316 D1:D241 D243:D295">
-    <cfRule type="duplicateValues" dxfId="65" priority="34"/>
-    <cfRule type="duplicateValues" dxfId="64" priority="35"/>
-    <cfRule type="duplicateValues" dxfId="63" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D296">
-    <cfRule type="duplicateValues" dxfId="62" priority="33"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D296">
-    <cfRule type="duplicateValues" dxfId="61" priority="30"/>
-    <cfRule type="duplicateValues" dxfId="60" priority="31"/>
-    <cfRule type="duplicateValues" dxfId="59" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D297:D300">
-    <cfRule type="duplicateValues" dxfId="58" priority="29"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D297:D300">
-    <cfRule type="duplicateValues" dxfId="57" priority="26"/>
-    <cfRule type="duplicateValues" dxfId="56" priority="27"/>
-    <cfRule type="duplicateValues" dxfId="55" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D301">
-    <cfRule type="duplicateValues" dxfId="54" priority="25"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D301">
-    <cfRule type="duplicateValues" dxfId="53" priority="22"/>
-    <cfRule type="duplicateValues" dxfId="52" priority="23"/>
-    <cfRule type="duplicateValues" dxfId="51" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D302:D303">
-    <cfRule type="duplicateValues" dxfId="50" priority="21"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D302:D303">
-    <cfRule type="duplicateValues" dxfId="49" priority="18"/>
-    <cfRule type="duplicateValues" dxfId="48" priority="19"/>
-    <cfRule type="duplicateValues" dxfId="47" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D304:D309">
-    <cfRule type="duplicateValues" dxfId="46" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="48"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="50"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D304:D309">
-    <cfRule type="duplicateValues" dxfId="45" priority="48"/>
-    <cfRule type="duplicateValues" dxfId="44" priority="49"/>
-    <cfRule type="duplicateValues" dxfId="43" priority="50"/>
+  <conditionalFormatting sqref="D310:D311 D316">
+    <cfRule type="duplicateValues" dxfId="23" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D316 D310:D311">
-    <cfRule type="duplicateValues" dxfId="42" priority="14"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D316 D310:D311">
-    <cfRule type="duplicateValues" dxfId="41" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="40" priority="16"/>
-    <cfRule type="duplicateValues" dxfId="39" priority="17"/>
+  <conditionalFormatting sqref="D311 D321">
+    <cfRule type="duplicateValues" dxfId="19" priority="58"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D312 D314:D315 D321:D1048576">
-    <cfRule type="duplicateValues" dxfId="38" priority="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D312 D314:D315 D321:D1048576">
-    <cfRule type="duplicateValues" dxfId="37" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="36" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="35" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D312:D313">
-    <cfRule type="duplicateValues" dxfId="34" priority="51"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D312:D313">
-    <cfRule type="duplicateValues" dxfId="33" priority="52"/>
-    <cfRule type="duplicateValues" dxfId="32" priority="53"/>
-    <cfRule type="duplicateValues" dxfId="31" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D313:D314">
-    <cfRule type="duplicateValues" dxfId="30" priority="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D313:D314">
-    <cfRule type="duplicateValues" dxfId="29" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="28" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="27" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D320">
-    <cfRule type="duplicateValues" dxfId="26" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D320">
-    <cfRule type="duplicateValues" dxfId="25" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="24" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="23" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D321 D311">
-    <cfRule type="duplicateValues" dxfId="22" priority="55"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D321 D311">
-    <cfRule type="duplicateValues" dxfId="21" priority="56"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="57"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="58"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D11:D1048576">
-    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed ooredoo master file details
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1355" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A22FB05-DC7F-45E0-8092-6D459340A1FD}"/>
+  <xr:revisionPtr revIDLastSave="1362" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EE1071B-B06B-4340-9531-DE449AEED6EC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2362" uniqueCount="1037">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2361" uniqueCount="1036">
   <si>
     <t>ICC ID</t>
   </si>
@@ -2495,9 +2495,6 @@
     <t>Request Completion Date</t>
   </si>
   <si>
-    <t>19-Jan-2023 @10:17 - Request was Completed</t>
-  </si>
-  <si>
     <t>55784038</t>
   </si>
   <si>
@@ -2508,9 +2505,6 @@
   </si>
   <si>
     <t>Cancelled (55683664)</t>
-  </si>
-  <si>
-    <t>Current Ooredoo Active Users</t>
   </si>
   <si>
     <t>22-Jan-2023 @10:10 - Requested to be Cancelled by Finance Dept.
@@ -3261,6 +3255,9 @@
   </si>
   <si>
     <t>MOHAMMAD SHAMIM</t>
+  </si>
+  <si>
+    <t>Ooredoo Users</t>
   </si>
 </sst>
 </file>
@@ -5006,9 +5003,6 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}" name="OoredooActiveUsers" displayName="OoredooActiveUsers" ref="A2:M369" headerRowDxfId="74" totalsRowDxfId="71" headerRowBorderDxfId="73" tableBorderDxfId="72">
   <autoFilter ref="A2:M369" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:M324">
-    <sortCondition ref="A2:A323"/>
-  </sortState>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{04FAFA61-B55D-4A3B-9F7F-E5235C6B0C57}" name="Date Requested/Date Last Modified" totalsRowLabel="Total" dataDxfId="70"/>
     <tableColumn id="2" xr3:uid="{DFF4E101-F3A1-41F6-BD45-E2AA15F2F6D6}" name="ICC ID" dataDxfId="69"/>
@@ -5339,10 +5333,10 @@
   <dimension ref="A1:W369"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E360" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A369" sqref="A369"/>
+      <selection pane="bottomRight" activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5370,7 +5364,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="95" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="87" t="s">
-        <v>808</v>
+        <v>1035</v>
       </c>
       <c r="B1" s="87"/>
       <c r="C1" s="88"/>
@@ -5466,12 +5460,8 @@
       </c>
       <c r="J3" s="16"/>
       <c r="K3" s="16"/>
-      <c r="L3" s="48">
-        <v>44945</v>
-      </c>
-      <c r="M3" s="99" t="s">
-        <v>803</v>
-      </c>
+      <c r="L3" s="48"/>
+      <c r="M3" s="99"/>
     </row>
     <row r="4" spans="1:23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
@@ -13355,7 +13345,7 @@
         <v>76</v>
       </c>
       <c r="D247" s="69" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E247" s="41" t="s">
         <v>86</v>
@@ -13396,7 +13386,7 @@
         <v>76</v>
       </c>
       <c r="D248" s="55" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E248" s="29" t="s">
         <v>155</v>
@@ -13437,7 +13427,7 @@
         <v>76</v>
       </c>
       <c r="D249" s="69" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E249" s="41" t="s">
         <v>127</v>
@@ -15893,7 +15883,7 @@
         <v>76</v>
       </c>
       <c r="D311" s="69" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E311" s="41" t="s">
         <v>127</v>
@@ -15918,7 +15908,7 @@
         <v>44949</v>
       </c>
       <c r="M311" s="99" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="N311" s="7"/>
       <c r="O311" s="7"/>
@@ -15936,13 +15926,13 @@
         <v>44956</v>
       </c>
       <c r="B312" s="120" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="C312" s="120" t="s">
         <v>76</v>
       </c>
       <c r="D312" s="69" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="E312" s="120" t="s">
         <v>155</v>
@@ -15951,16 +15941,16 @@
         <v>90</v>
       </c>
       <c r="G312" s="122" t="s">
+        <v>809</v>
+      </c>
+      <c r="H312" s="123" t="s">
+        <v>810</v>
+      </c>
+      <c r="I312" s="122" t="s">
         <v>811</v>
       </c>
-      <c r="H312" s="123" t="s">
+      <c r="J312" s="122" t="s">
         <v>812</v>
-      </c>
-      <c r="I312" s="122" t="s">
-        <v>813</v>
-      </c>
-      <c r="J312" s="122" t="s">
-        <v>814</v>
       </c>
       <c r="K312" s="122" t="s">
         <v>585</v>
@@ -15969,7 +15959,7 @@
         <v>44958</v>
       </c>
       <c r="M312" s="125" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="N312"/>
       <c r="O312"/>
@@ -16020,7 +16010,7 @@
         <v>44965</v>
       </c>
       <c r="M313" s="99" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="314" spans="1:23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -16043,7 +16033,7 @@
         <v>110.5</v>
       </c>
       <c r="G314" s="39" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="H314" s="45" t="s">
         <v>775</v>
@@ -16052,14 +16042,14 @@
         <v>370</v>
       </c>
       <c r="J314" s="39" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="K314" s="16"/>
       <c r="L314" s="48">
         <v>44965</v>
       </c>
       <c r="M314" s="106" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row r="315" spans="1:23" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -16082,7 +16072,7 @@
         <v>110.5</v>
       </c>
       <c r="G315" s="39" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="H315" s="45" t="s">
         <v>149</v>
@@ -16091,14 +16081,14 @@
         <v>150</v>
       </c>
       <c r="J315" s="39" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="K315" s="16"/>
       <c r="L315" s="48">
         <v>44965</v>
       </c>
       <c r="M315" s="106" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="N315"/>
       <c r="O315"/>
@@ -16131,13 +16121,13 @@
         <v>110.5</v>
       </c>
       <c r="G316" s="16" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="H316" s="17" t="s">
         <v>88</v>
       </c>
       <c r="I316" s="16" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="J316" s="16"/>
       <c r="K316" s="16"/>
@@ -16145,7 +16135,7 @@
         <v>44965</v>
       </c>
       <c r="M316" s="99" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="N316"/>
       <c r="O316"/>
@@ -16187,14 +16177,14 @@
         <v>203</v>
       </c>
       <c r="J317" s="16" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="K317" s="16"/>
       <c r="L317" s="48">
         <v>44965</v>
       </c>
       <c r="M317" s="99" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="N317"/>
       <c r="O317"/>
@@ -16233,7 +16223,7 @@
         <v>88</v>
       </c>
       <c r="I318" s="16" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="J318" s="16"/>
       <c r="K318" s="16"/>
@@ -16241,7 +16231,7 @@
         <v>44965</v>
       </c>
       <c r="M318" s="99" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="N318"/>
       <c r="O318"/>
@@ -16288,7 +16278,7 @@
         <v>44965</v>
       </c>
       <c r="M319" s="99" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="N319"/>
       <c r="O319"/>
@@ -16330,16 +16320,16 @@
         <v>532</v>
       </c>
       <c r="J320" s="16" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="K320" s="16" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="L320" s="48">
         <v>44965</v>
       </c>
       <c r="M320" s="99" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
     </row>
     <row r="321" spans="1:23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -16371,16 +16361,16 @@
         <v>538</v>
       </c>
       <c r="J321" s="16" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="K321" s="16" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="L321" s="48">
         <v>44965</v>
       </c>
       <c r="M321" s="99" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="322" spans="1:23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -16417,7 +16407,7 @@
         <v>44965</v>
       </c>
       <c r="M322" s="107" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="323" spans="1:23" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -16456,7 +16446,7 @@
         <v>44965</v>
       </c>
       <c r="M323" s="99" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="N323"/>
       <c r="O323"/>
@@ -16480,7 +16470,7 @@
         <v>76</v>
       </c>
       <c r="D324" s="130" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="E324" s="128" t="s">
         <v>77</v>
@@ -16489,7 +16479,7 @@
         <v>195</v>
       </c>
       <c r="G324" s="131" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="H324" s="130" t="s">
         <v>79</v>
@@ -16498,14 +16488,14 @@
         <v>80</v>
       </c>
       <c r="J324" s="131" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="K324" s="16"/>
       <c r="L324" s="113">
         <v>44965</v>
       </c>
       <c r="M324" s="127" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
     </row>
     <row r="325" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16513,7 +16503,7 @@
         <v>44964</v>
       </c>
       <c r="B325" s="109" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="C325" s="109" t="s">
         <v>76</v>
@@ -16531,22 +16521,22 @@
         <v>777</v>
       </c>
       <c r="H325" s="112" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="I325" s="111" t="s">
+        <v>884</v>
+      </c>
+      <c r="J325" s="111" t="s">
+        <v>885</v>
+      </c>
+      <c r="K325" s="111" t="s">
         <v>886</v>
-      </c>
-      <c r="J325" s="111" t="s">
-        <v>887</v>
-      </c>
-      <c r="K325" s="111" t="s">
-        <v>888</v>
       </c>
       <c r="L325" s="113">
         <v>44968</v>
       </c>
       <c r="M325" s="114" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
     </row>
     <row r="326" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16554,7 +16544,7 @@
         <v>44964</v>
       </c>
       <c r="B326" s="109" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="C326" s="109" t="s">
         <v>76</v>
@@ -16572,22 +16562,22 @@
         <v>777</v>
       </c>
       <c r="H326" s="112" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="I326" s="111" t="s">
+        <v>887</v>
+      </c>
+      <c r="J326" s="111" t="s">
+        <v>888</v>
+      </c>
+      <c r="K326" s="111" t="s">
         <v>889</v>
-      </c>
-      <c r="J326" s="111" t="s">
-        <v>890</v>
-      </c>
-      <c r="K326" s="111" t="s">
-        <v>891</v>
       </c>
       <c r="L326" s="113">
         <v>44968</v>
       </c>
       <c r="M326" s="114" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
     </row>
     <row r="327" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16595,7 +16585,7 @@
         <v>44964</v>
       </c>
       <c r="B327" s="109" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="C327" s="109" t="s">
         <v>76</v>
@@ -16613,13 +16603,13 @@
         <v>777</v>
       </c>
       <c r="H327" s="112" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="I327" s="111" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="J327" s="111" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="K327" s="111" t="s">
         <v>641</v>
@@ -16628,7 +16618,7 @@
         <v>44968</v>
       </c>
       <c r="M327" s="114" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
     </row>
     <row r="328" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16636,7 +16626,7 @@
         <v>44964</v>
       </c>
       <c r="B328" s="109" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="C328" s="109" t="s">
         <v>76</v>
@@ -16654,13 +16644,13 @@
         <v>777</v>
       </c>
       <c r="H328" s="112" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="I328" s="111" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="J328" s="111" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="K328" s="111" t="s">
         <v>641</v>
@@ -16669,7 +16659,7 @@
         <v>44968</v>
       </c>
       <c r="M328" s="114" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
     </row>
     <row r="329" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16677,7 +16667,7 @@
         <v>44964</v>
       </c>
       <c r="B329" s="109" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="C329" s="109" t="s">
         <v>76</v>
@@ -16695,22 +16685,22 @@
         <v>777</v>
       </c>
       <c r="H329" s="112" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="I329" s="111" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="J329" s="111" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="K329" s="111" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="L329" s="113">
         <v>44968</v>
       </c>
       <c r="M329" s="114" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="330" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16718,7 +16708,7 @@
         <v>44964</v>
       </c>
       <c r="B330" s="109" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="C330" s="109" t="s">
         <v>76</v>
@@ -16736,22 +16726,22 @@
         <v>777</v>
       </c>
       <c r="H330" s="112" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="I330" s="111" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="J330" s="111" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="K330" s="111" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="L330" s="113">
         <v>44968</v>
       </c>
       <c r="M330" s="114" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="331" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16759,7 +16749,7 @@
         <v>44964</v>
       </c>
       <c r="B331" s="109" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="C331" s="109" t="s">
         <v>76</v>
@@ -16777,13 +16767,13 @@
         <v>777</v>
       </c>
       <c r="H331" s="112" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="I331" s="111" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="J331" s="111" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="K331" s="111" t="s">
         <v>641</v>
@@ -16792,7 +16782,7 @@
         <v>44968</v>
       </c>
       <c r="M331" s="114" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
     </row>
     <row r="332" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16800,7 +16790,7 @@
         <v>44964</v>
       </c>
       <c r="B332" s="109" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="C332" s="109" t="s">
         <v>76</v>
@@ -16818,22 +16808,22 @@
         <v>777</v>
       </c>
       <c r="H332" s="112" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="I332" s="111" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="J332" s="111" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="K332" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L332" s="113">
         <v>44968</v>
       </c>
       <c r="M332" s="114" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
     </row>
     <row r="333" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16841,7 +16831,7 @@
         <v>44964</v>
       </c>
       <c r="B333" s="109" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="C333" s="109" t="s">
         <v>76</v>
@@ -16859,22 +16849,22 @@
         <v>777</v>
       </c>
       <c r="H333" s="112" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="I333" s="111" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="J333" s="111" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="K333" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L333" s="113">
         <v>44968</v>
       </c>
       <c r="M333" s="114" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
     </row>
     <row r="334" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16882,7 +16872,7 @@
         <v>44964</v>
       </c>
       <c r="B334" s="109" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="C334" s="109" t="s">
         <v>76</v>
@@ -16900,22 +16890,22 @@
         <v>777</v>
       </c>
       <c r="H334" s="112" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="I334" s="111" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="J334" s="111" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="K334" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L334" s="113">
         <v>44968</v>
       </c>
       <c r="M334" s="114" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
     </row>
     <row r="335" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16923,7 +16913,7 @@
         <v>44964</v>
       </c>
       <c r="B335" s="109" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="C335" s="109" t="s">
         <v>76</v>
@@ -16941,22 +16931,22 @@
         <v>777</v>
       </c>
       <c r="H335" s="112" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="I335" s="111" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="J335" s="111" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="K335" s="111" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="L335" s="113">
         <v>44968</v>
       </c>
       <c r="M335" s="114" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
     </row>
     <row r="336" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16964,7 +16954,7 @@
         <v>44964</v>
       </c>
       <c r="B336" s="109" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="C336" s="109" t="s">
         <v>76</v>
@@ -16982,13 +16972,13 @@
         <v>777</v>
       </c>
       <c r="H336" s="112" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="I336" s="111" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="J336" s="111" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="K336" s="111" t="s">
         <v>641</v>
@@ -16997,7 +16987,7 @@
         <v>44968</v>
       </c>
       <c r="M336" s="114" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
     </row>
     <row r="337" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17005,7 +16995,7 @@
         <v>44964</v>
       </c>
       <c r="B337" s="109" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="C337" s="109" t="s">
         <v>76</v>
@@ -17023,13 +17013,13 @@
         <v>777</v>
       </c>
       <c r="H337" s="112" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="I337" s="111" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="J337" s="111" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="K337" s="111" t="s">
         <v>641</v>
@@ -17038,7 +17028,7 @@
         <v>44968</v>
       </c>
       <c r="M337" s="114" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
     </row>
     <row r="338" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17046,7 +17036,7 @@
         <v>44964</v>
       </c>
       <c r="B338" s="109" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="C338" s="109" t="s">
         <v>76</v>
@@ -17064,22 +17054,22 @@
         <v>777</v>
       </c>
       <c r="H338" s="112" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="I338" s="111" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="J338" s="111" t="s">
         <v>268</v>
       </c>
       <c r="K338" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L338" s="113">
         <v>44968</v>
       </c>
       <c r="M338" s="114" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="339" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17087,7 +17077,7 @@
         <v>44964</v>
       </c>
       <c r="B339" s="109" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="C339" s="109" t="s">
         <v>76</v>
@@ -17105,22 +17095,22 @@
         <v>777</v>
       </c>
       <c r="H339" s="112" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="I339" s="111" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="J339" s="111" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="K339" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L339" s="113">
         <v>44968</v>
       </c>
       <c r="M339" s="114" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="340" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17128,7 +17118,7 @@
         <v>44964</v>
       </c>
       <c r="B340" s="109" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C340" s="109" t="s">
         <v>76</v>
@@ -17146,13 +17136,13 @@
         <v>777</v>
       </c>
       <c r="H340" s="112" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="I340" s="111" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="J340" s="111" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="K340" s="111" t="s">
         <v>641</v>
@@ -17161,7 +17151,7 @@
         <v>44968</v>
       </c>
       <c r="M340" s="114" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
     </row>
     <row r="341" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17169,7 +17159,7 @@
         <v>44964</v>
       </c>
       <c r="B341" s="109" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C341" s="109" t="s">
         <v>76</v>
@@ -17187,22 +17177,22 @@
         <v>777</v>
       </c>
       <c r="H341" s="112" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="I341" s="111" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="J341" s="111" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="K341" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L341" s="113">
         <v>44968</v>
       </c>
       <c r="M341" s="114" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="342" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17210,7 +17200,7 @@
         <v>44964</v>
       </c>
       <c r="B342" s="109" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C342" s="109" t="s">
         <v>76</v>
@@ -17228,13 +17218,13 @@
         <v>777</v>
       </c>
       <c r="H342" s="112" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="I342" s="111" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="J342" s="111" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="K342" s="111" t="s">
         <v>641</v>
@@ -17243,7 +17233,7 @@
         <v>44968</v>
       </c>
       <c r="M342" s="114" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
     </row>
     <row r="343" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17251,7 +17241,7 @@
         <v>44964</v>
       </c>
       <c r="B343" s="109" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="C343" s="109" t="s">
         <v>76</v>
@@ -17269,22 +17259,22 @@
         <v>777</v>
       </c>
       <c r="H343" s="112" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="I343" s="111" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="J343" s="111" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="K343" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L343" s="113">
         <v>44968</v>
       </c>
       <c r="M343" s="114" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
     </row>
     <row r="344" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17292,7 +17282,7 @@
         <v>44964</v>
       </c>
       <c r="B344" s="109" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C344" s="109" t="s">
         <v>76</v>
@@ -17310,13 +17300,13 @@
         <v>777</v>
       </c>
       <c r="H344" s="112" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="I344" s="111" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="J344" s="111" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="K344" s="111" t="s">
         <v>641</v>
@@ -17325,7 +17315,7 @@
         <v>44968</v>
       </c>
       <c r="M344" s="114" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="345" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17333,7 +17323,7 @@
         <v>44964</v>
       </c>
       <c r="B345" s="109" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C345" s="109" t="s">
         <v>76</v>
@@ -17351,13 +17341,13 @@
         <v>777</v>
       </c>
       <c r="H345" s="112" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="I345" s="111" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="J345" s="111" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="K345" s="111" t="s">
         <v>641</v>
@@ -17366,7 +17356,7 @@
         <v>44968</v>
       </c>
       <c r="M345" s="114" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
     </row>
     <row r="346" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17374,7 +17364,7 @@
         <v>44964</v>
       </c>
       <c r="B346" s="109" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="C346" s="109" t="s">
         <v>76</v>
@@ -17392,22 +17382,22 @@
         <v>777</v>
       </c>
       <c r="H346" s="112" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="I346" s="111" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="J346" s="111" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="K346" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L346" s="113">
         <v>44968</v>
       </c>
       <c r="M346" s="114" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
     </row>
     <row r="347" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17415,7 +17405,7 @@
         <v>44964</v>
       </c>
       <c r="B347" s="109" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="C347" s="109" t="s">
         <v>76</v>
@@ -17433,22 +17423,22 @@
         <v>777</v>
       </c>
       <c r="H347" s="112" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="I347" s="111" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="J347" s="111" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="K347" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L347" s="113">
         <v>44968</v>
       </c>
       <c r="M347" s="114" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="348" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17456,7 +17446,7 @@
         <v>44964</v>
       </c>
       <c r="B348" s="109" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="C348" s="109" t="s">
         <v>76</v>
@@ -17474,22 +17464,22 @@
         <v>777</v>
       </c>
       <c r="H348" s="112" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="I348" s="111" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="J348" s="111" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="K348" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L348" s="113">
         <v>44968</v>
       </c>
       <c r="M348" s="114" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
     </row>
     <row r="349" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17497,7 +17487,7 @@
         <v>44964</v>
       </c>
       <c r="B349" s="109" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="C349" s="109" t="s">
         <v>76</v>
@@ -17515,22 +17505,22 @@
         <v>777</v>
       </c>
       <c r="H349" s="112" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="I349" s="111" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="J349" s="111" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="K349" s="111" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="L349" s="113">
         <v>44968</v>
       </c>
       <c r="M349" s="114" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
     </row>
     <row r="350" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17538,7 +17528,7 @@
         <v>44964</v>
       </c>
       <c r="B350" s="109" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="C350" s="109" t="s">
         <v>76</v>
@@ -17556,22 +17546,22 @@
         <v>777</v>
       </c>
       <c r="H350" s="112" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="I350" s="111" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="J350" s="111" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="K350" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L350" s="113">
         <v>44968</v>
       </c>
       <c r="M350" s="114" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
     </row>
     <row r="351" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17579,7 +17569,7 @@
         <v>44964</v>
       </c>
       <c r="B351" s="109" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="C351" s="109" t="s">
         <v>76</v>
@@ -17597,22 +17587,22 @@
         <v>777</v>
       </c>
       <c r="H351" s="112" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="I351" s="111" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="J351" s="111" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="K351" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L351" s="113">
         <v>44968</v>
       </c>
       <c r="M351" s="114" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
     </row>
     <row r="352" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17620,7 +17610,7 @@
         <v>44964</v>
       </c>
       <c r="B352" s="109" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="C352" s="109" t="s">
         <v>76</v>
@@ -17638,22 +17628,22 @@
         <v>777</v>
       </c>
       <c r="H352" s="112" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="I352" s="111" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="J352" s="111" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="K352" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L352" s="113">
         <v>44968</v>
       </c>
       <c r="M352" s="114" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
     </row>
     <row r="353" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17661,7 +17651,7 @@
         <v>44964</v>
       </c>
       <c r="B353" s="109" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="C353" s="109" t="s">
         <v>76</v>
@@ -17679,13 +17669,13 @@
         <v>777</v>
       </c>
       <c r="H353" s="112" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="I353" s="111" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="J353" s="111" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="K353" s="111" t="s">
         <v>641</v>
@@ -17694,7 +17684,7 @@
         <v>44968</v>
       </c>
       <c r="M353" s="114" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
     </row>
     <row r="354" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17702,7 +17692,7 @@
         <v>44964</v>
       </c>
       <c r="B354" s="109" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="C354" s="109" t="s">
         <v>76</v>
@@ -17720,13 +17710,13 @@
         <v>777</v>
       </c>
       <c r="H354" s="112" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="I354" s="111" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="J354" s="111" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="K354" s="111" t="s">
         <v>641</v>
@@ -17735,7 +17725,7 @@
         <v>44968</v>
       </c>
       <c r="M354" s="114" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
     </row>
     <row r="355" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17743,7 +17733,7 @@
         <v>44964</v>
       </c>
       <c r="B355" s="109" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="C355" s="109" t="s">
         <v>76</v>
@@ -17761,13 +17751,13 @@
         <v>777</v>
       </c>
       <c r="H355" s="112" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="I355" s="111" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="J355" s="111" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="K355" s="111" t="s">
         <v>641</v>
@@ -17776,7 +17766,7 @@
         <v>44968</v>
       </c>
       <c r="M355" s="114" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
     </row>
     <row r="356" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17784,7 +17774,7 @@
         <v>44964</v>
       </c>
       <c r="B356" s="109" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="C356" s="109" t="s">
         <v>76</v>
@@ -17802,22 +17792,22 @@
         <v>777</v>
       </c>
       <c r="H356" s="112" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="I356" s="111" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="J356" s="111" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="K356" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L356" s="113">
         <v>44968</v>
       </c>
       <c r="M356" s="114" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="357" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17825,7 +17815,7 @@
         <v>44964</v>
       </c>
       <c r="B357" s="109" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="C357" s="109" t="s">
         <v>76</v>
@@ -17843,22 +17833,22 @@
         <v>777</v>
       </c>
       <c r="H357" s="112" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="I357" s="111" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="J357" s="111" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="K357" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L357" s="113">
         <v>44968</v>
       </c>
       <c r="M357" s="114" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="358" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17866,7 +17856,7 @@
         <v>44964</v>
       </c>
       <c r="B358" s="109" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="C358" s="109" t="s">
         <v>76</v>
@@ -17884,13 +17874,13 @@
         <v>777</v>
       </c>
       <c r="H358" s="112" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="I358" s="111" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="J358" s="111" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="K358" s="111" t="s">
         <v>641</v>
@@ -17899,7 +17889,7 @@
         <v>44968</v>
       </c>
       <c r="M358" s="114" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="359" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17907,7 +17897,7 @@
         <v>44964</v>
       </c>
       <c r="B359" s="109" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="C359" s="109" t="s">
         <v>76</v>
@@ -17925,13 +17915,13 @@
         <v>777</v>
       </c>
       <c r="H359" s="112" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="I359" s="111" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="J359" s="111" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="K359" s="111" t="s">
         <v>641</v>
@@ -17940,7 +17930,7 @@
         <v>44968</v>
       </c>
       <c r="M359" s="114" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="360" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17948,7 +17938,7 @@
         <v>44964</v>
       </c>
       <c r="B360" s="109" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="C360" s="109" t="s">
         <v>76</v>
@@ -17966,13 +17956,13 @@
         <v>777</v>
       </c>
       <c r="H360" s="112" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="I360" s="111" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="J360" s="111" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="K360" s="111" t="s">
         <v>641</v>
@@ -17981,7 +17971,7 @@
         <v>44968</v>
       </c>
       <c r="M360" s="114" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="361" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17989,7 +17979,7 @@
         <v>44964</v>
       </c>
       <c r="B361" s="109" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="C361" s="109" t="s">
         <v>76</v>
@@ -18007,22 +17997,22 @@
         <v>777</v>
       </c>
       <c r="H361" s="112" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="I361" s="111" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="J361" s="111" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="K361" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L361" s="113">
         <v>44968</v>
       </c>
       <c r="M361" s="114" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="362" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18030,7 +18020,7 @@
         <v>44964</v>
       </c>
       <c r="B362" s="109" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="C362" s="109" t="s">
         <v>76</v>
@@ -18048,22 +18038,22 @@
         <v>777</v>
       </c>
       <c r="H362" s="112" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I362" s="111" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="J362" s="111" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="K362" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L362" s="113">
         <v>44968</v>
       </c>
       <c r="M362" s="114" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="363" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18071,7 +18061,7 @@
         <v>44964</v>
       </c>
       <c r="B363" s="109" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="C363" s="109" t="s">
         <v>76</v>
@@ -18089,13 +18079,13 @@
         <v>777</v>
       </c>
       <c r="H363" s="112" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="I363" s="111" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="J363" s="111" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="K363" s="111" t="s">
         <v>641</v>
@@ -18104,7 +18094,7 @@
         <v>44968</v>
       </c>
       <c r="M363" s="114" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="364" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18112,7 +18102,7 @@
         <v>44964</v>
       </c>
       <c r="B364" s="109" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="C364" s="109" t="s">
         <v>76</v>
@@ -18130,22 +18120,22 @@
         <v>777</v>
       </c>
       <c r="H364" s="112" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I364" s="111" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="J364" s="111" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="K364" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L364" s="113">
         <v>44968</v>
       </c>
       <c r="M364" s="114" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="365" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18153,7 +18143,7 @@
         <v>44964</v>
       </c>
       <c r="B365" s="109" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="C365" s="109" t="s">
         <v>76</v>
@@ -18171,22 +18161,22 @@
         <v>777</v>
       </c>
       <c r="H365" s="112" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="I365" s="111" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="J365" s="111" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="K365" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L365" s="113">
         <v>44968</v>
       </c>
       <c r="M365" s="114" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="366" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18194,7 +18184,7 @@
         <v>44964</v>
       </c>
       <c r="B366" s="109" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="C366" s="109" t="s">
         <v>76</v>
@@ -18212,22 +18202,22 @@
         <v>777</v>
       </c>
       <c r="H366" s="112" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="I366" s="111" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="J366" s="111" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="K366" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L366" s="113">
         <v>44968</v>
       </c>
       <c r="M366" s="114" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="367" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18235,7 +18225,7 @@
         <v>44964</v>
       </c>
       <c r="B367" s="109" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="C367" s="109" t="s">
         <v>76</v>
@@ -18253,22 +18243,22 @@
         <v>777</v>
       </c>
       <c r="H367" s="112" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="I367" s="111" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="J367" s="111" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="K367" s="111" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="L367" s="113">
         <v>44968</v>
       </c>
       <c r="M367" s="114" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="368" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18276,7 +18266,7 @@
         <v>44964</v>
       </c>
       <c r="B368" s="109" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C368" s="109" t="s">
         <v>76</v>
@@ -18294,13 +18284,13 @@
         <v>777</v>
       </c>
       <c r="H368" s="112" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="I368" s="111" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="J368" s="111" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="K368" s="111" t="s">
         <v>641</v>
@@ -18309,7 +18299,7 @@
         <v>44968</v>
       </c>
       <c r="M368" s="114" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="369" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18317,7 +18307,7 @@
         <v>44964</v>
       </c>
       <c r="B369" s="109" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="C369" s="109" t="s">
         <v>76</v>
@@ -18335,13 +18325,13 @@
         <v>777</v>
       </c>
       <c r="H369" s="112" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="I369" s="111" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="J369" s="111" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="K369" s="111" t="s">
         <v>641</v>
@@ -18350,7 +18340,7 @@
         <v>44968</v>
       </c>
       <c r="M369" s="114" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ooredoo event: replaced one sim
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1362" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EE1071B-B06B-4340-9531-DE449AEED6EC}"/>
+  <xr:revisionPtr revIDLastSave="1369" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4E268CA-B1D7-4F99-AD6C-B61B6CC36A70}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
+    <workbookView xWindow="35850" yWindow="4245" windowWidth="21600" windowHeight="11235" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="OoredooMasterFile" sheetId="2" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2361" uniqueCount="1036">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2362" uniqueCount="1038">
   <si>
     <t>ICC ID</t>
   </si>
@@ -2749,11 +2749,6 @@
 08-Feb-2023 @11:31 - Request was Completed with Plan D; </t>
   </si>
   <si>
-    <t xml:space="preserve">Upgraded from Plan C to Plan D at November 15, 2022
-02-Feb-2023 @11:47 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS
-08-Feb-2023 @11:31 - Request was Completed with Plan D; </t>
-  </si>
-  <si>
     <t>RESIGNED
 05-Feb-2023 @11:38 - Cancellation of this Ooredoo Account and Service Number (Resigned) - Dan
 08-Feb-2023 @11:35 - Request was Completed with Plan G; Successfully Cancelled</t>
@@ -3258,6 +3253,18 @@
   </si>
   <si>
     <t>Ooredoo Users</t>
+  </si>
+  <si>
+    <t>8997401002220201412</t>
+  </si>
+  <si>
+    <t>R-1</t>
+  </si>
+  <si>
+    <t>Upgraded from Plan C to Plan D at November 15, 2022
+02-Feb-2023 @11:47 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS
+08-Feb-2023 @11:31 - Request was Completed with Plan D; 
+08-Mar-2023 @15:42 - Sim Card Replacement</t>
   </si>
 </sst>
 </file>
@@ -3395,7 +3402,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3471,6 +3478,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3621,7 +3634,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3994,6 +4007,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5364,7 +5380,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="95" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="87" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="B1" s="87"/>
       <c r="C1" s="88"/>
@@ -11667,7 +11683,7 @@
       <c r="V197" s="6"/>
       <c r="W197" s="6"/>
     </row>
-    <row r="198" spans="1:23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A198" s="15">
         <v>43831</v>
       </c>
@@ -14362,7 +14378,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="273" spans="1:13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A273" s="15">
         <v>44315</v>
       </c>
@@ -14403,7 +14419,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="274" spans="1:13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A274" s="15">
         <v>44335</v>
       </c>
@@ -15833,7 +15849,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="310" spans="1:23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A310" s="15">
         <v>44929</v>
       </c>
@@ -16013,12 +16029,12 @@
         <v>872</v>
       </c>
     </row>
-    <row r="314" spans="1:23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A314" s="38">
-        <v>44959</v>
+        <v>44993</v>
       </c>
       <c r="B314" s="71" t="s">
-        <v>369</v>
+        <v>1035</v>
       </c>
       <c r="C314" s="71" t="s">
         <v>76</v>
@@ -16045,11 +16061,11 @@
         <v>822</v>
       </c>
       <c r="K314" s="16"/>
-      <c r="L314" s="48">
-        <v>44965</v>
+      <c r="L314" s="132" t="s">
+        <v>1036</v>
       </c>
       <c r="M314" s="106" t="s">
-        <v>882</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="315" spans="1:23" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -16495,7 +16511,7 @@
         <v>44965</v>
       </c>
       <c r="M324" s="127" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="325" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16521,22 +16537,22 @@
         <v>777</v>
       </c>
       <c r="H325" s="112" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="I325" s="111" t="s">
+        <v>883</v>
+      </c>
+      <c r="J325" s="111" t="s">
         <v>884</v>
       </c>
-      <c r="J325" s="111" t="s">
+      <c r="K325" s="111" t="s">
         <v>885</v>
-      </c>
-      <c r="K325" s="111" t="s">
-        <v>886</v>
       </c>
       <c r="L325" s="113">
         <v>44968</v>
       </c>
       <c r="M325" s="114" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="326" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16562,22 +16578,22 @@
         <v>777</v>
       </c>
       <c r="H326" s="112" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="I326" s="111" t="s">
+        <v>886</v>
+      </c>
+      <c r="J326" s="111" t="s">
         <v>887</v>
       </c>
-      <c r="J326" s="111" t="s">
+      <c r="K326" s="111" t="s">
         <v>888</v>
-      </c>
-      <c r="K326" s="111" t="s">
-        <v>889</v>
       </c>
       <c r="L326" s="113">
         <v>44968</v>
       </c>
       <c r="M326" s="114" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="327" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16603,13 +16619,13 @@
         <v>777</v>
       </c>
       <c r="H327" s="112" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="I327" s="111" t="s">
+        <v>889</v>
+      </c>
+      <c r="J327" s="111" t="s">
         <v>890</v>
-      </c>
-      <c r="J327" s="111" t="s">
-        <v>891</v>
       </c>
       <c r="K327" s="111" t="s">
         <v>641</v>
@@ -16618,7 +16634,7 @@
         <v>44968</v>
       </c>
       <c r="M327" s="114" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="328" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16644,13 +16660,13 @@
         <v>777</v>
       </c>
       <c r="H328" s="112" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="I328" s="111" t="s">
+        <v>891</v>
+      </c>
+      <c r="J328" s="111" t="s">
         <v>892</v>
-      </c>
-      <c r="J328" s="111" t="s">
-        <v>893</v>
       </c>
       <c r="K328" s="111" t="s">
         <v>641</v>
@@ -16659,7 +16675,7 @@
         <v>44968</v>
       </c>
       <c r="M328" s="114" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="329" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16685,22 +16701,22 @@
         <v>777</v>
       </c>
       <c r="H329" s="112" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="I329" s="111" t="s">
+        <v>893</v>
+      </c>
+      <c r="J329" s="111" t="s">
         <v>894</v>
       </c>
-      <c r="J329" s="111" t="s">
-        <v>895</v>
-      </c>
       <c r="K329" s="111" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="L329" s="113">
         <v>44968</v>
       </c>
       <c r="M329" s="114" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="330" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16726,22 +16742,22 @@
         <v>777</v>
       </c>
       <c r="H330" s="112" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="I330" s="111" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="J330" s="111" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="K330" s="111" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="L330" s="113">
         <v>44968</v>
       </c>
       <c r="M330" s="114" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="331" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16767,13 +16783,13 @@
         <v>777</v>
       </c>
       <c r="H331" s="112" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="I331" s="111" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J331" s="111" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="K331" s="111" t="s">
         <v>641</v>
@@ -16782,7 +16798,7 @@
         <v>44968</v>
       </c>
       <c r="M331" s="114" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="332" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16808,22 +16824,22 @@
         <v>777</v>
       </c>
       <c r="H332" s="112" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="I332" s="111" t="s">
+        <v>897</v>
+      </c>
+      <c r="J332" s="111" t="s">
         <v>898</v>
       </c>
-      <c r="J332" s="111" t="s">
-        <v>899</v>
-      </c>
       <c r="K332" s="111" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L332" s="113">
         <v>44968</v>
       </c>
       <c r="M332" s="114" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="333" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16849,22 +16865,22 @@
         <v>777</v>
       </c>
       <c r="H333" s="112" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="I333" s="111" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="J333" s="111" t="s">
+        <v>884</v>
+      </c>
+      <c r="K333" s="111" t="s">
         <v>885</v>
-      </c>
-      <c r="K333" s="111" t="s">
-        <v>886</v>
       </c>
       <c r="L333" s="113">
         <v>44968</v>
       </c>
       <c r="M333" s="114" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="334" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16890,22 +16906,22 @@
         <v>777</v>
       </c>
       <c r="H334" s="112" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="I334" s="111" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="J334" s="111" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="K334" s="111" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L334" s="113">
         <v>44968</v>
       </c>
       <c r="M334" s="114" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="335" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16931,22 +16947,22 @@
         <v>777</v>
       </c>
       <c r="H335" s="112" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="I335" s="111" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="J335" s="111" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="K335" s="111" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="L335" s="113">
         <v>44968</v>
       </c>
       <c r="M335" s="114" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="336" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16972,13 +16988,13 @@
         <v>777</v>
       </c>
       <c r="H336" s="112" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="I336" s="111" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="J336" s="111" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="K336" s="111" t="s">
         <v>641</v>
@@ -16987,7 +17003,7 @@
         <v>44968</v>
       </c>
       <c r="M336" s="114" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="337" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17013,13 +17029,13 @@
         <v>777</v>
       </c>
       <c r="H337" s="112" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="I337" s="111" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="J337" s="111" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="K337" s="111" t="s">
         <v>641</v>
@@ -17028,7 +17044,7 @@
         <v>44968</v>
       </c>
       <c r="M337" s="114" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="338" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17054,22 +17070,22 @@
         <v>777</v>
       </c>
       <c r="H338" s="112" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="I338" s="111" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="J338" s="111" t="s">
         <v>268</v>
       </c>
       <c r="K338" s="111" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L338" s="113">
         <v>44968</v>
       </c>
       <c r="M338" s="114" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="339" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17095,22 +17111,22 @@
         <v>777</v>
       </c>
       <c r="H339" s="112" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="I339" s="111" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="J339" s="111" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="K339" s="111" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L339" s="113">
         <v>44968</v>
       </c>
       <c r="M339" s="114" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="340" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17136,13 +17152,13 @@
         <v>777</v>
       </c>
       <c r="H340" s="112" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="I340" s="111" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="J340" s="111" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="K340" s="111" t="s">
         <v>641</v>
@@ -17151,7 +17167,7 @@
         <v>44968</v>
       </c>
       <c r="M340" s="114" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="341" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17177,22 +17193,22 @@
         <v>777</v>
       </c>
       <c r="H341" s="112" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="I341" s="111" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="J341" s="111" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="K341" s="111" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L341" s="113">
         <v>44968</v>
       </c>
       <c r="M341" s="114" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="342" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17218,13 +17234,13 @@
         <v>777</v>
       </c>
       <c r="H342" s="112" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="I342" s="111" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="J342" s="111" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="K342" s="111" t="s">
         <v>641</v>
@@ -17233,7 +17249,7 @@
         <v>44968</v>
       </c>
       <c r="M342" s="114" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="343" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17259,22 +17275,22 @@
         <v>777</v>
       </c>
       <c r="H343" s="112" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="I343" s="111" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="J343" s="111" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="K343" s="111" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L343" s="113">
         <v>44968</v>
       </c>
       <c r="M343" s="114" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="344" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17300,13 +17316,13 @@
         <v>777</v>
       </c>
       <c r="H344" s="112" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I344" s="111" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="J344" s="111" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="K344" s="111" t="s">
         <v>641</v>
@@ -17315,7 +17331,7 @@
         <v>44968</v>
       </c>
       <c r="M344" s="114" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="345" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17341,13 +17357,13 @@
         <v>777</v>
       </c>
       <c r="H345" s="112" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I345" s="111" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="J345" s="111" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="K345" s="111" t="s">
         <v>641</v>
@@ -17356,7 +17372,7 @@
         <v>44968</v>
       </c>
       <c r="M345" s="114" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="346" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17382,22 +17398,22 @@
         <v>777</v>
       </c>
       <c r="H346" s="112" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="I346" s="111" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="J346" s="111" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="K346" s="111" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L346" s="113">
         <v>44968</v>
       </c>
       <c r="M346" s="114" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="347" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17423,22 +17439,22 @@
         <v>777</v>
       </c>
       <c r="H347" s="112" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="I347" s="111" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="J347" s="111" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="K347" s="111" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L347" s="113">
         <v>44968</v>
       </c>
       <c r="M347" s="114" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="348" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17464,22 +17480,22 @@
         <v>777</v>
       </c>
       <c r="H348" s="112" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="I348" s="111" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="J348" s="111" t="s">
+        <v>884</v>
+      </c>
+      <c r="K348" s="111" t="s">
         <v>885</v>
-      </c>
-      <c r="K348" s="111" t="s">
-        <v>886</v>
       </c>
       <c r="L348" s="113">
         <v>44968</v>
       </c>
       <c r="M348" s="114" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="349" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17505,22 +17521,22 @@
         <v>777</v>
       </c>
       <c r="H349" s="112" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="I349" s="111" t="s">
+        <v>915</v>
+      </c>
+      <c r="J349" s="111" t="s">
         <v>916</v>
       </c>
-      <c r="J349" s="111" t="s">
-        <v>917</v>
-      </c>
       <c r="K349" s="111" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="L349" s="113">
         <v>44968</v>
       </c>
       <c r="M349" s="114" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="350" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17546,22 +17562,22 @@
         <v>777</v>
       </c>
       <c r="H350" s="112" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="I350" s="111" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="J350" s="111" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="K350" s="111" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L350" s="113">
         <v>44968</v>
       </c>
       <c r="M350" s="114" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="351" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17587,22 +17603,22 @@
         <v>777</v>
       </c>
       <c r="H351" s="112" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="I351" s="111" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="J351" s="111" t="s">
+        <v>884</v>
+      </c>
+      <c r="K351" s="111" t="s">
         <v>885</v>
-      </c>
-      <c r="K351" s="111" t="s">
-        <v>886</v>
       </c>
       <c r="L351" s="113">
         <v>44968</v>
       </c>
       <c r="M351" s="114" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="352" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17628,22 +17644,22 @@
         <v>777</v>
       </c>
       <c r="H352" s="112" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="I352" s="111" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="J352" s="111" t="s">
+        <v>884</v>
+      </c>
+      <c r="K352" s="111" t="s">
         <v>885</v>
-      </c>
-      <c r="K352" s="111" t="s">
-        <v>886</v>
       </c>
       <c r="L352" s="113">
         <v>44968</v>
       </c>
       <c r="M352" s="114" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="353" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17669,13 +17685,13 @@
         <v>777</v>
       </c>
       <c r="H353" s="112" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="I353" s="111" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="J353" s="111" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="K353" s="111" t="s">
         <v>641</v>
@@ -17684,7 +17700,7 @@
         <v>44968</v>
       </c>
       <c r="M353" s="114" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="354" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17710,13 +17726,13 @@
         <v>777</v>
       </c>
       <c r="H354" s="112" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="I354" s="111" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="J354" s="111" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="K354" s="111" t="s">
         <v>641</v>
@@ -17725,7 +17741,7 @@
         <v>44968</v>
       </c>
       <c r="M354" s="114" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="355" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17751,13 +17767,13 @@
         <v>777</v>
       </c>
       <c r="H355" s="112" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="I355" s="111" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="J355" s="111" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="K355" s="111" t="s">
         <v>641</v>
@@ -17766,7 +17782,7 @@
         <v>44968</v>
       </c>
       <c r="M355" s="114" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="356" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17792,22 +17808,22 @@
         <v>777</v>
       </c>
       <c r="H356" s="112" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="I356" s="111" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="J356" s="111" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="K356" s="111" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L356" s="113">
         <v>44968</v>
       </c>
       <c r="M356" s="114" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="357" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17833,22 +17849,22 @@
         <v>777</v>
       </c>
       <c r="H357" s="112" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="I357" s="111" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="J357" s="111" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="K357" s="111" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L357" s="113">
         <v>44968</v>
       </c>
       <c r="M357" s="114" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="358" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17874,13 +17890,13 @@
         <v>777</v>
       </c>
       <c r="H358" s="112" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="I358" s="111" t="s">
+        <v>925</v>
+      </c>
+      <c r="J358" s="111" t="s">
         <v>926</v>
-      </c>
-      <c r="J358" s="111" t="s">
-        <v>927</v>
       </c>
       <c r="K358" s="111" t="s">
         <v>641</v>
@@ -17889,7 +17905,7 @@
         <v>44968</v>
       </c>
       <c r="M358" s="114" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="359" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17915,13 +17931,13 @@
         <v>777</v>
       </c>
       <c r="H359" s="112" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="I359" s="111" t="s">
+        <v>927</v>
+      </c>
+      <c r="J359" s="111" t="s">
         <v>928</v>
-      </c>
-      <c r="J359" s="111" t="s">
-        <v>929</v>
       </c>
       <c r="K359" s="111" t="s">
         <v>641</v>
@@ -17930,7 +17946,7 @@
         <v>44968</v>
       </c>
       <c r="M359" s="114" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="360" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17956,13 +17972,13 @@
         <v>777</v>
       </c>
       <c r="H360" s="112" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="I360" s="111" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="J360" s="111" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="K360" s="111" t="s">
         <v>641</v>
@@ -17971,7 +17987,7 @@
         <v>44968</v>
       </c>
       <c r="M360" s="114" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="361" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17997,22 +18013,22 @@
         <v>777</v>
       </c>
       <c r="H361" s="112" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="I361" s="111" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="J361" s="111" t="s">
+        <v>884</v>
+      </c>
+      <c r="K361" s="111" t="s">
         <v>885</v>
-      </c>
-      <c r="K361" s="111" t="s">
-        <v>886</v>
       </c>
       <c r="L361" s="113">
         <v>44968</v>
       </c>
       <c r="M361" s="114" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="362" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18038,22 +18054,22 @@
         <v>777</v>
       </c>
       <c r="H362" s="112" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="I362" s="111" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="J362" s="111" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="K362" s="111" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L362" s="113">
         <v>44968</v>
       </c>
       <c r="M362" s="114" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="363" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18079,13 +18095,13 @@
         <v>777</v>
       </c>
       <c r="H363" s="112" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I363" s="111" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="J363" s="111" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="K363" s="111" t="s">
         <v>641</v>
@@ -18094,7 +18110,7 @@
         <v>44968</v>
       </c>
       <c r="M363" s="114" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="364" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18120,22 +18136,22 @@
         <v>777</v>
       </c>
       <c r="H364" s="112" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="I364" s="111" t="s">
+        <v>1015</v>
+      </c>
+      <c r="J364" s="111" t="s">
         <v>1016</v>
       </c>
-      <c r="J364" s="111" t="s">
-        <v>1017</v>
-      </c>
       <c r="K364" s="111" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L364" s="113">
         <v>44968</v>
       </c>
       <c r="M364" s="114" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="365" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18161,22 +18177,22 @@
         <v>777</v>
       </c>
       <c r="H365" s="112" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="I365" s="111" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="J365" s="111" t="s">
+        <v>884</v>
+      </c>
+      <c r="K365" s="111" t="s">
         <v>885</v>
-      </c>
-      <c r="K365" s="111" t="s">
-        <v>886</v>
       </c>
       <c r="L365" s="113">
         <v>44968</v>
       </c>
       <c r="M365" s="114" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="366" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18202,22 +18218,22 @@
         <v>777</v>
       </c>
       <c r="H366" s="112" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="I366" s="111" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="J366" s="111" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="K366" s="111" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L366" s="113">
         <v>44968</v>
       </c>
       <c r="M366" s="114" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="367" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18243,22 +18259,22 @@
         <v>777</v>
       </c>
       <c r="H367" s="112" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="I367" s="111" t="s">
+        <v>1019</v>
+      </c>
+      <c r="J367" s="111" t="s">
         <v>1020</v>
       </c>
-      <c r="J367" s="111" t="s">
-        <v>1021</v>
-      </c>
       <c r="K367" s="111" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L367" s="113">
         <v>44968</v>
       </c>
       <c r="M367" s="114" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="368" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18284,13 +18300,13 @@
         <v>777</v>
       </c>
       <c r="H368" s="112" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="I368" s="111" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="J368" s="111" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="K368" s="111" t="s">
         <v>641</v>
@@ -18299,7 +18315,7 @@
         <v>44968</v>
       </c>
       <c r="M368" s="114" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="369" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18325,13 +18341,13 @@
         <v>777</v>
       </c>
       <c r="H369" s="112" t="s">
+        <v>1030</v>
+      </c>
+      <c r="I369" s="111" t="s">
+        <v>1033</v>
+      </c>
+      <c r="J369" s="111" t="s">
         <v>1031</v>
-      </c>
-      <c r="I369" s="111" t="s">
-        <v>1034</v>
-      </c>
-      <c r="J369" s="111" t="s">
-        <v>1032</v>
       </c>
       <c r="K369" s="111" t="s">
         <v>641</v>
@@ -18340,7 +18356,7 @@
         <v>44968</v>
       </c>
       <c r="M369" s="114" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor update for Ooredoo Master File
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1369" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4E268CA-B1D7-4F99-AD6C-B61B6CC36A70}"/>
+  <xr:revisionPtr revIDLastSave="1372" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1E2594B-E548-46C9-AA09-B73C05BE8D3E}"/>
   <bookViews>
-    <workbookView xWindow="35850" yWindow="4245" windowWidth="21600" windowHeight="11235" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="OoredooMasterFile" sheetId="2" r:id="rId1"/>
@@ -3634,7 +3634,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3991,26 +3991,44 @@
     <xf numFmtId="49" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="7" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5019,6 +5037,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}" name="OoredooActiveUsers" displayName="OoredooActiveUsers" ref="A2:M369" headerRowDxfId="74" totalsRowDxfId="71" headerRowBorderDxfId="73" tableBorderDxfId="72">
   <autoFilter ref="A2:M369" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:M369">
+    <sortCondition ref="A2:A369"/>
+  </sortState>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{04FAFA61-B55D-4A3B-9F7F-E5235C6B0C57}" name="Date Requested/Date Last Modified" totalsRowLabel="Total" dataDxfId="70"/>
     <tableColumn id="2" xr3:uid="{DFF4E101-F3A1-41F6-BD45-E2AA15F2F6D6}" name="ICC ID" dataDxfId="69"/>
@@ -5349,10 +5370,10 @@
   <dimension ref="A1:W369"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="J359" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D74" sqref="D74"/>
+      <selection pane="bottomRight" activeCell="A370" sqref="A370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16031,16 +16052,16 @@
     </row>
     <row r="314" spans="1:23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A314" s="38">
-        <v>44993</v>
+        <v>44959</v>
       </c>
       <c r="B314" s="71" t="s">
-        <v>1035</v>
+        <v>148</v>
       </c>
       <c r="C314" s="71" t="s">
         <v>76</v>
       </c>
       <c r="D314" s="72">
-        <v>55320856</v>
+        <v>33093329</v>
       </c>
       <c r="E314" s="71" t="s">
         <v>86</v>
@@ -16052,59 +16073,57 @@
         <v>821</v>
       </c>
       <c r="H314" s="45" t="s">
-        <v>775</v>
+        <v>149</v>
       </c>
       <c r="I314" s="39" t="s">
-        <v>370</v>
+        <v>150</v>
       </c>
       <c r="J314" s="39" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="K314" s="16"/>
-      <c r="L314" s="132" t="s">
-        <v>1036</v>
+      <c r="L314" s="48">
+        <v>44965</v>
       </c>
       <c r="M314" s="106" t="s">
-        <v>1037</v>
+        <v>873</v>
       </c>
     </row>
     <row r="315" spans="1:23" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A315" s="38">
+      <c r="A315" s="15">
         <v>44959</v>
       </c>
-      <c r="B315" s="71" t="s">
-        <v>148</v>
-      </c>
-      <c r="C315" s="71" t="s">
-        <v>76</v>
-      </c>
-      <c r="D315" s="72">
-        <v>33093329</v>
-      </c>
-      <c r="E315" s="71" t="s">
+      <c r="B315" s="41" t="s">
+        <v>488</v>
+      </c>
+      <c r="C315" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="D315" s="54">
+        <v>66983912</v>
+      </c>
+      <c r="E315" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="F315" s="85">
+      <c r="F315" s="76">
         <v>110.5</v>
       </c>
-      <c r="G315" s="39" t="s">
-        <v>821</v>
-      </c>
-      <c r="H315" s="45" t="s">
-        <v>149</v>
-      </c>
-      <c r="I315" s="39" t="s">
-        <v>150</v>
-      </c>
-      <c r="J315" s="39" t="s">
-        <v>823</v>
-      </c>
+      <c r="G315" s="16" t="s">
+        <v>815</v>
+      </c>
+      <c r="H315" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="I315" s="16" t="s">
+        <v>816</v>
+      </c>
+      <c r="J315" s="16"/>
       <c r="K315" s="16"/>
       <c r="L315" s="48">
         <v>44965</v>
       </c>
-      <c r="M315" s="106" t="s">
-        <v>873</v>
+      <c r="M315" s="99" t="s">
+        <v>875</v>
       </c>
       <c r="N315"/>
       <c r="O315"/>
@@ -16122,36 +16141,38 @@
         <v>44959</v>
       </c>
       <c r="B316" s="41" t="s">
-        <v>488</v>
+        <v>202</v>
       </c>
       <c r="C316" s="41" t="s">
         <v>76</v>
       </c>
       <c r="D316" s="54">
-        <v>66983912</v>
+        <v>33564180</v>
       </c>
       <c r="E316" s="41" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="F316" s="76">
-        <v>110.5</v>
+        <v>90</v>
       </c>
       <c r="G316" s="16" t="s">
-        <v>815</v>
+        <v>168</v>
       </c>
       <c r="H316" s="17" t="s">
-        <v>88</v>
+        <v>169</v>
       </c>
       <c r="I316" s="16" t="s">
-        <v>816</v>
-      </c>
-      <c r="J316" s="16"/>
+        <v>203</v>
+      </c>
+      <c r="J316" s="16" t="s">
+        <v>819</v>
+      </c>
       <c r="K316" s="16"/>
       <c r="L316" s="48">
         <v>44965</v>
       </c>
       <c r="M316" s="99" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="N316"/>
       <c r="O316"/>
@@ -16169,38 +16190,36 @@
         <v>44959</v>
       </c>
       <c r="B317" s="41" t="s">
-        <v>202</v>
+        <v>400</v>
       </c>
       <c r="C317" s="41" t="s">
         <v>76</v>
       </c>
       <c r="D317" s="54">
-        <v>33564180</v>
+        <v>66027138</v>
       </c>
       <c r="E317" s="41" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="F317" s="76">
-        <v>90</v>
+        <v>110.5</v>
       </c>
       <c r="G317" s="16" t="s">
-        <v>168</v>
+        <v>87</v>
       </c>
       <c r="H317" s="17" t="s">
-        <v>169</v>
+        <v>88</v>
       </c>
       <c r="I317" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="J317" s="16" t="s">
-        <v>819</v>
-      </c>
+        <v>820</v>
+      </c>
+      <c r="J317" s="16"/>
       <c r="K317" s="16"/>
       <c r="L317" s="48">
         <v>44965</v>
       </c>
       <c r="M317" s="99" t="s">
-        <v>877</v>
+        <v>881</v>
       </c>
       <c r="N317"/>
       <c r="O317"/>
@@ -16218,13 +16237,13 @@
         <v>44959</v>
       </c>
       <c r="B318" s="41" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C318" s="41" t="s">
         <v>76</v>
       </c>
       <c r="D318" s="54">
-        <v>66027138</v>
+        <v>66019585</v>
       </c>
       <c r="E318" s="41" t="s">
         <v>86</v>
@@ -16239,7 +16258,7 @@
         <v>88</v>
       </c>
       <c r="I318" s="16" t="s">
-        <v>820</v>
+        <v>399</v>
       </c>
       <c r="J318" s="16"/>
       <c r="K318" s="16"/>
@@ -16247,7 +16266,7 @@
         <v>44965</v>
       </c>
       <c r="M318" s="99" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="N318"/>
       <c r="O318"/>
@@ -16265,36 +16284,40 @@
         <v>44959</v>
       </c>
       <c r="B319" s="41" t="s">
-        <v>398</v>
+        <v>81</v>
       </c>
       <c r="C319" s="41" t="s">
         <v>76</v>
       </c>
       <c r="D319" s="54">
-        <v>66019585</v>
+        <v>77015815</v>
       </c>
       <c r="E319" s="41" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F319" s="76">
-        <v>110.5</v>
+        <v>135</v>
       </c>
       <c r="G319" s="16" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="H319" s="17" t="s">
-        <v>88</v>
+        <v>531</v>
       </c>
       <c r="I319" s="16" t="s">
-        <v>399</v>
-      </c>
-      <c r="J319" s="16"/>
-      <c r="K319" s="16"/>
+        <v>532</v>
+      </c>
+      <c r="J319" s="16" t="s">
+        <v>818</v>
+      </c>
+      <c r="K319" s="16" t="s">
+        <v>824</v>
+      </c>
       <c r="L319" s="48">
         <v>44965</v>
       </c>
       <c r="M319" s="99" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="N319"/>
       <c r="O319"/>
@@ -16318,7 +16341,7 @@
         <v>76</v>
       </c>
       <c r="D320" s="54">
-        <v>77015815</v>
+        <v>77149189</v>
       </c>
       <c r="E320" s="41" t="s">
         <v>82</v>
@@ -16330,13 +16353,13 @@
         <v>78</v>
       </c>
       <c r="H320" s="17" t="s">
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="I320" s="16" t="s">
-        <v>532</v>
+        <v>538</v>
       </c>
       <c r="J320" s="16" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="K320" s="16" t="s">
         <v>824</v>
@@ -16345,124 +16368,122 @@
         <v>44965</v>
       </c>
       <c r="M320" s="99" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="321" spans="1:23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A321" s="15">
+      <c r="A321" s="42">
         <v>44959</v>
       </c>
-      <c r="B321" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="C321" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="D321" s="54">
-        <v>77149189</v>
-      </c>
-      <c r="E321" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="F321" s="76">
-        <v>135</v>
-      </c>
-      <c r="G321" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="H321" s="17" t="s">
-        <v>537</v>
-      </c>
-      <c r="I321" s="16" t="s">
-        <v>538</v>
-      </c>
-      <c r="J321" s="16" t="s">
-        <v>817</v>
-      </c>
-      <c r="K321" s="16" t="s">
-        <v>824</v>
-      </c>
+      <c r="B321" s="73" t="s">
+        <v>772</v>
+      </c>
+      <c r="C321" s="73" t="s">
+        <v>76</v>
+      </c>
+      <c r="D321" s="74">
+        <v>50497377</v>
+      </c>
+      <c r="E321" s="73" t="s">
+        <v>86</v>
+      </c>
+      <c r="F321" s="86">
+        <v>110.5</v>
+      </c>
+      <c r="G321" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="H321" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="I321" s="43" t="s">
+        <v>773</v>
+      </c>
+      <c r="J321" s="43"/>
+      <c r="K321" s="16"/>
       <c r="L321" s="48">
         <v>44965</v>
       </c>
-      <c r="M321" s="99" t="s">
-        <v>874</v>
+      <c r="M321" s="107" t="s">
+        <v>879</v>
       </c>
     </row>
     <row r="322" spans="1:23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A322" s="42">
+      <c r="A322" s="46">
         <v>44959</v>
       </c>
-      <c r="B322" s="73" t="s">
-        <v>772</v>
-      </c>
-      <c r="C322" s="73" t="s">
-        <v>76</v>
-      </c>
-      <c r="D322" s="74">
-        <v>50497377</v>
-      </c>
-      <c r="E322" s="73" t="s">
+      <c r="B322" s="47" t="s">
+        <v>638</v>
+      </c>
+      <c r="C322" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="D322" s="69">
+        <v>50266792</v>
+      </c>
+      <c r="E322" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="F322" s="86">
+      <c r="F322" s="76">
         <v>110.5</v>
       </c>
-      <c r="G322" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="H322" s="44" t="s">
+      <c r="G322" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="H322" s="17" t="s">
+        <v>792</v>
+      </c>
+      <c r="I322" s="16" t="s">
+        <v>793</v>
+      </c>
+      <c r="J322" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="I322" s="43" t="s">
-        <v>773</v>
-      </c>
-      <c r="J322" s="43"/>
       <c r="K322" s="16"/>
       <c r="L322" s="48">
         <v>44965</v>
       </c>
-      <c r="M322" s="107" t="s">
-        <v>879</v>
+      <c r="M322" s="99" t="s">
+        <v>880</v>
       </c>
     </row>
     <row r="323" spans="1:23" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A323" s="46">
-        <v>44959</v>
-      </c>
-      <c r="B323" s="47" t="s">
-        <v>638</v>
-      </c>
-      <c r="C323" s="47" t="s">
-        <v>76</v>
-      </c>
-      <c r="D323" s="69">
-        <v>50266792</v>
-      </c>
-      <c r="E323" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="F323" s="76">
-        <v>110.5</v>
+      <c r="A323" s="15">
+        <v>44962</v>
+      </c>
+      <c r="B323" s="126" t="s">
+        <v>75</v>
+      </c>
+      <c r="C323" s="126" t="s">
+        <v>76</v>
+      </c>
+      <c r="D323" s="17" t="s">
+        <v>825</v>
+      </c>
+      <c r="E323" s="126" t="s">
+        <v>77</v>
+      </c>
+      <c r="F323" s="127">
+        <v>195</v>
       </c>
       <c r="G323" s="16" t="s">
-        <v>78</v>
+        <v>821</v>
       </c>
       <c r="H323" s="17" t="s">
-        <v>792</v>
+        <v>79</v>
       </c>
       <c r="I323" s="16" t="s">
-        <v>793</v>
+        <v>80</v>
       </c>
       <c r="J323" s="16" t="s">
-        <v>88</v>
+        <v>826</v>
       </c>
       <c r="K323" s="16"/>
-      <c r="L323" s="46">
+      <c r="L323" s="119">
         <v>44965</v>
       </c>
-      <c r="M323" s="99" t="s">
-        <v>880</v>
+      <c r="M323" s="128" t="s">
+        <v>882</v>
       </c>
       <c r="N323"/>
       <c r="O323"/>
@@ -16476,42 +16497,44 @@
       <c r="W323"/>
     </row>
     <row r="324" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A324" s="126">
-        <v>44962</v>
-      </c>
-      <c r="B324" s="128" t="s">
-        <v>75</v>
-      </c>
-      <c r="C324" s="128" t="s">
-        <v>76</v>
-      </c>
-      <c r="D324" s="130" t="s">
-        <v>825</v>
-      </c>
-      <c r="E324" s="128" t="s">
-        <v>77</v>
-      </c>
-      <c r="F324" s="129">
-        <v>195</v>
-      </c>
-      <c r="G324" s="131" t="s">
-        <v>821</v>
-      </c>
-      <c r="H324" s="130" t="s">
-        <v>79</v>
-      </c>
-      <c r="I324" s="131" t="s">
-        <v>80</v>
-      </c>
-      <c r="J324" s="131" t="s">
-        <v>826</v>
-      </c>
-      <c r="K324" s="16"/>
+      <c r="A324" s="108">
+        <v>44964</v>
+      </c>
+      <c r="B324" s="109" t="s">
+        <v>827</v>
+      </c>
+      <c r="C324" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D324" s="75">
+        <v>33574156</v>
+      </c>
+      <c r="E324" s="109" t="s">
+        <v>155</v>
+      </c>
+      <c r="F324" s="110">
+        <v>90</v>
+      </c>
+      <c r="G324" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="H324" s="112" t="s">
+        <v>931</v>
+      </c>
+      <c r="I324" s="111" t="s">
+        <v>883</v>
+      </c>
+      <c r="J324" s="111" t="s">
+        <v>884</v>
+      </c>
+      <c r="K324" s="122" t="s">
+        <v>885</v>
+      </c>
       <c r="L324" s="113">
-        <v>44965</v>
-      </c>
-      <c r="M324" s="127" t="s">
-        <v>882</v>
+        <v>44968</v>
+      </c>
+      <c r="M324" s="114" t="s">
+        <v>968</v>
       </c>
     </row>
     <row r="325" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16519,13 +16542,13 @@
         <v>44964</v>
       </c>
       <c r="B325" s="109" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="C325" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D325" s="75">
-        <v>33574156</v>
+        <v>33603140</v>
       </c>
       <c r="E325" s="109" t="s">
         <v>155</v>
@@ -16537,22 +16560,22 @@
         <v>777</v>
       </c>
       <c r="H325" s="112" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="I325" s="111" t="s">
-        <v>883</v>
+        <v>886</v>
       </c>
       <c r="J325" s="111" t="s">
-        <v>884</v>
+        <v>887</v>
       </c>
       <c r="K325" s="111" t="s">
-        <v>885</v>
+        <v>888</v>
       </c>
       <c r="L325" s="113">
         <v>44968</v>
       </c>
       <c r="M325" s="114" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
     </row>
     <row r="326" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16560,13 +16583,13 @@
         <v>44964</v>
       </c>
       <c r="B326" s="109" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="C326" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D326" s="75">
-        <v>33603140</v>
+        <v>33585461</v>
       </c>
       <c r="E326" s="109" t="s">
         <v>155</v>
@@ -16578,22 +16601,22 @@
         <v>777</v>
       </c>
       <c r="H326" s="112" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="I326" s="111" t="s">
-        <v>886</v>
+        <v>889</v>
       </c>
       <c r="J326" s="111" t="s">
-        <v>887</v>
+        <v>890</v>
       </c>
       <c r="K326" s="111" t="s">
-        <v>888</v>
+        <v>641</v>
       </c>
       <c r="L326" s="113">
         <v>44968</v>
       </c>
       <c r="M326" s="114" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
     </row>
     <row r="327" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16601,13 +16624,13 @@
         <v>44964</v>
       </c>
       <c r="B327" s="109" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="C327" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D327" s="75">
-        <v>33585461</v>
+        <v>33576710</v>
       </c>
       <c r="E327" s="109" t="s">
         <v>155</v>
@@ -16619,13 +16642,13 @@
         <v>777</v>
       </c>
       <c r="H327" s="112" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="I327" s="111" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="J327" s="111" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="K327" s="111" t="s">
         <v>641</v>
@@ -16634,7 +16657,7 @@
         <v>44968</v>
       </c>
       <c r="M327" s="114" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
     </row>
     <row r="328" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16642,13 +16665,13 @@
         <v>44964</v>
       </c>
       <c r="B328" s="109" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="C328" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D328" s="75">
-        <v>33576710</v>
+        <v>33595578</v>
       </c>
       <c r="E328" s="109" t="s">
         <v>155</v>
@@ -16660,22 +16683,22 @@
         <v>777</v>
       </c>
       <c r="H328" s="112" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="I328" s="111" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="J328" s="111" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="K328" s="111" t="s">
-        <v>641</v>
+        <v>888</v>
       </c>
       <c r="L328" s="113">
         <v>44968</v>
       </c>
       <c r="M328" s="114" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
     </row>
     <row r="329" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16683,13 +16706,13 @@
         <v>44964</v>
       </c>
       <c r="B329" s="109" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="C329" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D329" s="75">
-        <v>33595578</v>
+        <v>33583901</v>
       </c>
       <c r="E329" s="109" t="s">
         <v>155</v>
@@ -16701,10 +16724,10 @@
         <v>777</v>
       </c>
       <c r="H329" s="112" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="I329" s="111" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="J329" s="111" t="s">
         <v>894</v>
@@ -16716,7 +16739,7 @@
         <v>44968</v>
       </c>
       <c r="M329" s="114" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="330" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16724,13 +16747,13 @@
         <v>44964</v>
       </c>
       <c r="B330" s="109" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="C330" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D330" s="75">
-        <v>33583901</v>
+        <v>33576317</v>
       </c>
       <c r="E330" s="109" t="s">
         <v>155</v>
@@ -16742,22 +16765,22 @@
         <v>777</v>
       </c>
       <c r="H330" s="112" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="I330" s="111" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="J330" s="111" t="s">
-        <v>894</v>
+        <v>890</v>
       </c>
       <c r="K330" s="111" t="s">
-        <v>888</v>
+        <v>641</v>
       </c>
       <c r="L330" s="113">
         <v>44968</v>
       </c>
       <c r="M330" s="114" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
     </row>
     <row r="331" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16765,13 +16788,13 @@
         <v>44964</v>
       </c>
       <c r="B331" s="109" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="C331" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D331" s="75">
-        <v>33576317</v>
+        <v>33581367</v>
       </c>
       <c r="E331" s="109" t="s">
         <v>155</v>
@@ -16783,22 +16806,22 @@
         <v>777</v>
       </c>
       <c r="H331" s="112" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="I331" s="111" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="J331" s="111" t="s">
-        <v>890</v>
+        <v>898</v>
       </c>
       <c r="K331" s="111" t="s">
-        <v>641</v>
+        <v>885</v>
       </c>
       <c r="L331" s="113">
         <v>44968</v>
       </c>
       <c r="M331" s="114" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
     </row>
     <row r="332" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16806,13 +16829,13 @@
         <v>44964</v>
       </c>
       <c r="B332" s="109" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="C332" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D332" s="75">
-        <v>33581367</v>
+        <v>33585994</v>
       </c>
       <c r="E332" s="109" t="s">
         <v>155</v>
@@ -16824,13 +16847,13 @@
         <v>777</v>
       </c>
       <c r="H332" s="112" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="I332" s="111" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="J332" s="111" t="s">
-        <v>898</v>
+        <v>884</v>
       </c>
       <c r="K332" s="111" t="s">
         <v>885</v>
@@ -16839,7 +16862,7 @@
         <v>44968</v>
       </c>
       <c r="M332" s="114" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
     </row>
     <row r="333" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16847,13 +16870,13 @@
         <v>44964</v>
       </c>
       <c r="B333" s="109" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="C333" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D333" s="75">
-        <v>33585994</v>
+        <v>33596039</v>
       </c>
       <c r="E333" s="109" t="s">
         <v>155</v>
@@ -16865,13 +16888,13 @@
         <v>777</v>
       </c>
       <c r="H333" s="112" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="I333" s="111" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="J333" s="111" t="s">
-        <v>884</v>
+        <v>898</v>
       </c>
       <c r="K333" s="111" t="s">
         <v>885</v>
@@ -16880,7 +16903,7 @@
         <v>44968</v>
       </c>
       <c r="M333" s="114" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
     </row>
     <row r="334" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16888,13 +16911,13 @@
         <v>44964</v>
       </c>
       <c r="B334" s="109" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="C334" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D334" s="75">
-        <v>33596039</v>
+        <v>33583392</v>
       </c>
       <c r="E334" s="109" t="s">
         <v>155</v>
@@ -16906,22 +16929,22 @@
         <v>777</v>
       </c>
       <c r="H334" s="112" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="I334" s="111" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="J334" s="111" t="s">
-        <v>898</v>
+        <v>894</v>
       </c>
       <c r="K334" s="111" t="s">
-        <v>885</v>
+        <v>888</v>
       </c>
       <c r="L334" s="113">
         <v>44968</v>
       </c>
       <c r="M334" s="114" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
     </row>
     <row r="335" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16929,13 +16952,13 @@
         <v>44964</v>
       </c>
       <c r="B335" s="109" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C335" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D335" s="75">
-        <v>33583392</v>
+        <v>33598446</v>
       </c>
       <c r="E335" s="109" t="s">
         <v>155</v>
@@ -16947,22 +16970,22 @@
         <v>777</v>
       </c>
       <c r="H335" s="112" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="I335" s="111" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="J335" s="111" t="s">
-        <v>894</v>
+        <v>898</v>
       </c>
       <c r="K335" s="111" t="s">
-        <v>888</v>
+        <v>641</v>
       </c>
       <c r="L335" s="113">
         <v>44968</v>
       </c>
       <c r="M335" s="114" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
     </row>
     <row r="336" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16970,13 +16993,13 @@
         <v>44964</v>
       </c>
       <c r="B336" s="109" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="C336" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D336" s="75">
-        <v>33598446</v>
+        <v>33597912</v>
       </c>
       <c r="E336" s="109" t="s">
         <v>155</v>
@@ -16988,13 +17011,13 @@
         <v>777</v>
       </c>
       <c r="H336" s="112" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="I336" s="111" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="J336" s="111" t="s">
-        <v>898</v>
+        <v>890</v>
       </c>
       <c r="K336" s="111" t="s">
         <v>641</v>
@@ -17003,7 +17026,7 @@
         <v>44968</v>
       </c>
       <c r="M336" s="114" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
     </row>
     <row r="337" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17011,13 +17034,13 @@
         <v>44964</v>
       </c>
       <c r="B337" s="109" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C337" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D337" s="75">
-        <v>33597912</v>
+        <v>33601543</v>
       </c>
       <c r="E337" s="109" t="s">
         <v>155</v>
@@ -17029,22 +17052,22 @@
         <v>777</v>
       </c>
       <c r="H337" s="112" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="I337" s="111" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="J337" s="111" t="s">
-        <v>890</v>
+        <v>268</v>
       </c>
       <c r="K337" s="111" t="s">
-        <v>641</v>
+        <v>885</v>
       </c>
       <c r="L337" s="113">
         <v>44968</v>
       </c>
       <c r="M337" s="114" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
     </row>
     <row r="338" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17052,13 +17075,13 @@
         <v>44964</v>
       </c>
       <c r="B338" s="109" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="C338" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D338" s="75">
-        <v>33601543</v>
+        <v>33596920</v>
       </c>
       <c r="E338" s="109" t="s">
         <v>155</v>
@@ -17070,13 +17093,13 @@
         <v>777</v>
       </c>
       <c r="H338" s="112" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="I338" s="111" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="J338" s="111" t="s">
-        <v>268</v>
+        <v>892</v>
       </c>
       <c r="K338" s="111" t="s">
         <v>885</v>
@@ -17085,7 +17108,7 @@
         <v>44968</v>
       </c>
       <c r="M338" s="114" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
     </row>
     <row r="339" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17093,13 +17116,13 @@
         <v>44964</v>
       </c>
       <c r="B339" s="109" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="C339" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D339" s="75">
-        <v>33596920</v>
+        <v>33579329</v>
       </c>
       <c r="E339" s="109" t="s">
         <v>155</v>
@@ -17111,22 +17134,22 @@
         <v>777</v>
       </c>
       <c r="H339" s="112" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="I339" s="111" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="J339" s="111" t="s">
-        <v>892</v>
+        <v>887</v>
       </c>
       <c r="K339" s="111" t="s">
-        <v>885</v>
+        <v>641</v>
       </c>
       <c r="L339" s="113">
         <v>44968</v>
       </c>
       <c r="M339" s="114" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
     </row>
     <row r="340" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17134,13 +17157,13 @@
         <v>44964</v>
       </c>
       <c r="B340" s="109" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="C340" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D340" s="75">
-        <v>33579329</v>
+        <v>33598379</v>
       </c>
       <c r="E340" s="109" t="s">
         <v>155</v>
@@ -17152,22 +17175,22 @@
         <v>777</v>
       </c>
       <c r="H340" s="112" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="I340" s="111" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="J340" s="111" t="s">
-        <v>887</v>
+        <v>892</v>
       </c>
       <c r="K340" s="111" t="s">
-        <v>641</v>
+        <v>885</v>
       </c>
       <c r="L340" s="113">
         <v>44968</v>
       </c>
       <c r="M340" s="114" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
     </row>
     <row r="341" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17175,13 +17198,13 @@
         <v>44964</v>
       </c>
       <c r="B341" s="109" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="C341" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D341" s="75">
-        <v>33598379</v>
+        <v>33603691</v>
       </c>
       <c r="E341" s="109" t="s">
         <v>155</v>
@@ -17193,22 +17216,22 @@
         <v>777</v>
       </c>
       <c r="H341" s="112" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="I341" s="111" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="J341" s="111" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="K341" s="111" t="s">
-        <v>885</v>
+        <v>641</v>
       </c>
       <c r="L341" s="113">
         <v>44968</v>
       </c>
       <c r="M341" s="114" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
     </row>
     <row r="342" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17216,13 +17239,13 @@
         <v>44964</v>
       </c>
       <c r="B342" s="109" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="C342" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D342" s="75">
-        <v>33603691</v>
+        <v>33585246</v>
       </c>
       <c r="E342" s="109" t="s">
         <v>155</v>
@@ -17234,22 +17257,22 @@
         <v>777</v>
       </c>
       <c r="H342" s="112" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="I342" s="111" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="J342" s="111" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="K342" s="111" t="s">
-        <v>641</v>
+        <v>885</v>
       </c>
       <c r="L342" s="113">
         <v>44968</v>
       </c>
       <c r="M342" s="114" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
     </row>
     <row r="343" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17257,13 +17280,13 @@
         <v>44964</v>
       </c>
       <c r="B343" s="109" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="C343" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D343" s="75">
-        <v>33585246</v>
+        <v>33574035</v>
       </c>
       <c r="E343" s="109" t="s">
         <v>155</v>
@@ -17275,22 +17298,22 @@
         <v>777</v>
       </c>
       <c r="H343" s="112" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="I343" s="111" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="J343" s="111" t="s">
-        <v>892</v>
+        <v>887</v>
       </c>
       <c r="K343" s="111" t="s">
-        <v>885</v>
+        <v>641</v>
       </c>
       <c r="L343" s="113">
         <v>44968</v>
       </c>
       <c r="M343" s="114" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
     </row>
     <row r="344" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17298,13 +17321,13 @@
         <v>44964</v>
       </c>
       <c r="B344" s="109" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="C344" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D344" s="75">
-        <v>33574035</v>
+        <v>33597942</v>
       </c>
       <c r="E344" s="109" t="s">
         <v>155</v>
@@ -17316,13 +17339,13 @@
         <v>777</v>
       </c>
       <c r="H344" s="112" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="I344" s="111" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="J344" s="111" t="s">
-        <v>887</v>
+        <v>890</v>
       </c>
       <c r="K344" s="111" t="s">
         <v>641</v>
@@ -17331,7 +17354,7 @@
         <v>44968</v>
       </c>
       <c r="M344" s="114" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
     </row>
     <row r="345" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17339,13 +17362,13 @@
         <v>44964</v>
       </c>
       <c r="B345" s="109" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="C345" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D345" s="75">
-        <v>33597942</v>
+        <v>33581276</v>
       </c>
       <c r="E345" s="109" t="s">
         <v>155</v>
@@ -17357,22 +17380,22 @@
         <v>777</v>
       </c>
       <c r="H345" s="112" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="I345" s="111" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="J345" s="111" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="K345" s="111" t="s">
-        <v>641</v>
+        <v>885</v>
       </c>
       <c r="L345" s="113">
         <v>44968</v>
       </c>
       <c r="M345" s="114" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
     </row>
     <row r="346" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17380,13 +17403,13 @@
         <v>44964</v>
       </c>
       <c r="B346" s="109" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C346" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D346" s="75">
-        <v>33581276</v>
+        <v>33583276</v>
       </c>
       <c r="E346" s="109" t="s">
         <v>155</v>
@@ -17398,13 +17421,13 @@
         <v>777</v>
       </c>
       <c r="H346" s="112" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="I346" s="111" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="J346" s="111" t="s">
-        <v>892</v>
+        <v>898</v>
       </c>
       <c r="K346" s="111" t="s">
         <v>885</v>
@@ -17413,7 +17436,7 @@
         <v>44968</v>
       </c>
       <c r="M346" s="114" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
     </row>
     <row r="347" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17421,13 +17444,13 @@
         <v>44964</v>
       </c>
       <c r="B347" s="109" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="C347" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D347" s="75">
-        <v>33583276</v>
+        <v>33576136</v>
       </c>
       <c r="E347" s="109" t="s">
         <v>155</v>
@@ -17439,13 +17462,13 @@
         <v>777</v>
       </c>
       <c r="H347" s="112" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="I347" s="111" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="J347" s="111" t="s">
-        <v>898</v>
+        <v>884</v>
       </c>
       <c r="K347" s="111" t="s">
         <v>885</v>
@@ -17454,7 +17477,7 @@
         <v>44968</v>
       </c>
       <c r="M347" s="114" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
     </row>
     <row r="348" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17462,13 +17485,13 @@
         <v>44964</v>
       </c>
       <c r="B348" s="109" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="C348" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D348" s="75">
-        <v>33576136</v>
+        <v>33603750</v>
       </c>
       <c r="E348" s="109" t="s">
         <v>155</v>
@@ -17480,22 +17503,22 @@
         <v>777</v>
       </c>
       <c r="H348" s="112" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="I348" s="111" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="J348" s="111" t="s">
-        <v>884</v>
+        <v>916</v>
       </c>
       <c r="K348" s="111" t="s">
-        <v>885</v>
+        <v>888</v>
       </c>
       <c r="L348" s="113">
         <v>44968</v>
       </c>
       <c r="M348" s="114" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
     </row>
     <row r="349" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17503,13 +17526,13 @@
         <v>44964</v>
       </c>
       <c r="B349" s="109" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="C349" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D349" s="75">
-        <v>33603750</v>
+        <v>33602876</v>
       </c>
       <c r="E349" s="109" t="s">
         <v>155</v>
@@ -17521,22 +17544,22 @@
         <v>777</v>
       </c>
       <c r="H349" s="112" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="I349" s="111" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="J349" s="111" t="s">
-        <v>916</v>
+        <v>892</v>
       </c>
       <c r="K349" s="111" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="L349" s="113">
         <v>44968</v>
       </c>
       <c r="M349" s="114" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
     </row>
     <row r="350" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17544,13 +17567,13 @@
         <v>44964</v>
       </c>
       <c r="B350" s="109" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="C350" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D350" s="75">
-        <v>33602876</v>
+        <v>33598168</v>
       </c>
       <c r="E350" s="109" t="s">
         <v>155</v>
@@ -17562,13 +17585,13 @@
         <v>777</v>
       </c>
       <c r="H350" s="112" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="I350" s="111" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="J350" s="111" t="s">
-        <v>892</v>
+        <v>884</v>
       </c>
       <c r="K350" s="111" t="s">
         <v>885</v>
@@ -17577,7 +17600,7 @@
         <v>44968</v>
       </c>
       <c r="M350" s="114" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
     </row>
     <row r="351" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17585,13 +17608,13 @@
         <v>44964</v>
       </c>
       <c r="B351" s="109" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C351" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D351" s="75">
-        <v>33598168</v>
+        <v>33583060</v>
       </c>
       <c r="E351" s="109" t="s">
         <v>155</v>
@@ -17603,10 +17626,10 @@
         <v>777</v>
       </c>
       <c r="H351" s="112" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="I351" s="111" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="J351" s="111" t="s">
         <v>884</v>
@@ -17618,7 +17641,7 @@
         <v>44968</v>
       </c>
       <c r="M351" s="114" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
     </row>
     <row r="352" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17626,13 +17649,13 @@
         <v>44964</v>
       </c>
       <c r="B352" s="109" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C352" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D352" s="75">
-        <v>33583060</v>
+        <v>33583208</v>
       </c>
       <c r="E352" s="109" t="s">
         <v>155</v>
@@ -17644,22 +17667,22 @@
         <v>777</v>
       </c>
       <c r="H352" s="112" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="I352" s="111" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="J352" s="111" t="s">
-        <v>884</v>
+        <v>890</v>
       </c>
       <c r="K352" s="111" t="s">
-        <v>885</v>
+        <v>641</v>
       </c>
       <c r="L352" s="113">
         <v>44968</v>
       </c>
       <c r="M352" s="114" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
     </row>
     <row r="353" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17667,13 +17690,13 @@
         <v>44964</v>
       </c>
       <c r="B353" s="109" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="C353" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D353" s="75">
-        <v>33583208</v>
+        <v>33596804</v>
       </c>
       <c r="E353" s="109" t="s">
         <v>155</v>
@@ -17685,13 +17708,13 @@
         <v>777</v>
       </c>
       <c r="H353" s="112" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="I353" s="111" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="J353" s="111" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="K353" s="111" t="s">
         <v>641</v>
@@ -17700,7 +17723,7 @@
         <v>44968</v>
       </c>
       <c r="M353" s="114" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
     </row>
     <row r="354" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17708,13 +17731,13 @@
         <v>44964</v>
       </c>
       <c r="B354" s="109" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="C354" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D354" s="75">
-        <v>33596804</v>
+        <v>33585715</v>
       </c>
       <c r="E354" s="109" t="s">
         <v>155</v>
@@ -17726,13 +17749,13 @@
         <v>777</v>
       </c>
       <c r="H354" s="112" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="I354" s="111" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="J354" s="111" t="s">
-        <v>887</v>
+        <v>890</v>
       </c>
       <c r="K354" s="111" t="s">
         <v>641</v>
@@ -17741,7 +17764,7 @@
         <v>44968</v>
       </c>
       <c r="M354" s="114" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
     </row>
     <row r="355" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17749,13 +17772,13 @@
         <v>44964</v>
       </c>
       <c r="B355" s="109" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="C355" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D355" s="75">
-        <v>33585715</v>
+        <v>33583569</v>
       </c>
       <c r="E355" s="109" t="s">
         <v>155</v>
@@ -17767,22 +17790,22 @@
         <v>777</v>
       </c>
       <c r="H355" s="112" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="I355" s="111" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="J355" s="111" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="K355" s="111" t="s">
-        <v>641</v>
+        <v>885</v>
       </c>
       <c r="L355" s="113">
         <v>44968</v>
       </c>
       <c r="M355" s="114" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
     </row>
     <row r="356" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17790,13 +17813,13 @@
         <v>44964</v>
       </c>
       <c r="B356" s="109" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="C356" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D356" s="75">
-        <v>33583569</v>
+        <v>33586015</v>
       </c>
       <c r="E356" s="109" t="s">
         <v>155</v>
@@ -17808,10 +17831,10 @@
         <v>777</v>
       </c>
       <c r="H356" s="112" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="I356" s="111" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="J356" s="111" t="s">
         <v>892</v>
@@ -17823,7 +17846,7 @@
         <v>44968</v>
       </c>
       <c r="M356" s="114" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="357" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17831,13 +17854,13 @@
         <v>44964</v>
       </c>
       <c r="B357" s="109" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="C357" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D357" s="75">
-        <v>33586015</v>
+        <v>33598546</v>
       </c>
       <c r="E357" s="109" t="s">
         <v>155</v>
@@ -17849,22 +17872,22 @@
         <v>777</v>
       </c>
       <c r="H357" s="112" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="I357" s="111" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="J357" s="111" t="s">
-        <v>892</v>
+        <v>926</v>
       </c>
       <c r="K357" s="111" t="s">
-        <v>885</v>
+        <v>641</v>
       </c>
       <c r="L357" s="113">
         <v>44968</v>
       </c>
       <c r="M357" s="114" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="358" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17872,13 +17895,13 @@
         <v>44964</v>
       </c>
       <c r="B358" s="109" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="C358" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D358" s="75">
-        <v>33598546</v>
+        <v>33585194</v>
       </c>
       <c r="E358" s="109" t="s">
         <v>155</v>
@@ -17890,13 +17913,13 @@
         <v>777</v>
       </c>
       <c r="H358" s="112" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="I358" s="111" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="J358" s="111" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="K358" s="111" t="s">
         <v>641</v>
@@ -17905,7 +17928,7 @@
         <v>44968</v>
       </c>
       <c r="M358" s="114" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="359" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17913,13 +17936,13 @@
         <v>44964</v>
       </c>
       <c r="B359" s="109" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="C359" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D359" s="75">
-        <v>33585194</v>
+        <v>33585725</v>
       </c>
       <c r="E359" s="109" t="s">
         <v>155</v>
@@ -17931,13 +17954,13 @@
         <v>777</v>
       </c>
       <c r="H359" s="112" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="I359" s="111" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="J359" s="111" t="s">
-        <v>928</v>
+        <v>890</v>
       </c>
       <c r="K359" s="111" t="s">
         <v>641</v>
@@ -17946,7 +17969,7 @@
         <v>44968</v>
       </c>
       <c r="M359" s="114" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="360" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17954,13 +17977,13 @@
         <v>44964</v>
       </c>
       <c r="B360" s="109" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="C360" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D360" s="75">
-        <v>33585725</v>
+        <v>33602786</v>
       </c>
       <c r="E360" s="109" t="s">
         <v>155</v>
@@ -17972,22 +17995,22 @@
         <v>777</v>
       </c>
       <c r="H360" s="112" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="I360" s="111" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="J360" s="111" t="s">
-        <v>890</v>
+        <v>884</v>
       </c>
       <c r="K360" s="111" t="s">
-        <v>641</v>
+        <v>885</v>
       </c>
       <c r="L360" s="113">
         <v>44968</v>
       </c>
       <c r="M360" s="114" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="361" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17995,13 +18018,13 @@
         <v>44964</v>
       </c>
       <c r="B361" s="109" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="C361" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D361" s="75">
-        <v>33602786</v>
+        <v>33574061</v>
       </c>
       <c r="E361" s="109" t="s">
         <v>155</v>
@@ -18013,13 +18036,13 @@
         <v>777</v>
       </c>
       <c r="H361" s="112" t="s">
-        <v>967</v>
+        <v>1023</v>
       </c>
       <c r="I361" s="111" t="s">
-        <v>930</v>
+        <v>1013</v>
       </c>
       <c r="J361" s="111" t="s">
-        <v>884</v>
+        <v>1021</v>
       </c>
       <c r="K361" s="111" t="s">
         <v>885</v>
@@ -18028,7 +18051,7 @@
         <v>44968</v>
       </c>
       <c r="M361" s="114" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="362" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18036,13 +18059,13 @@
         <v>44964</v>
       </c>
       <c r="B362" s="109" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="C362" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D362" s="75">
-        <v>33574061</v>
+        <v>33603712</v>
       </c>
       <c r="E362" s="109" t="s">
         <v>155</v>
@@ -18054,22 +18077,22 @@
         <v>777</v>
       </c>
       <c r="H362" s="112" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="I362" s="111" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="J362" s="111" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="K362" s="111" t="s">
-        <v>885</v>
+        <v>641</v>
       </c>
       <c r="L362" s="113">
         <v>44968</v>
       </c>
       <c r="M362" s="114" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="363" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18077,13 +18100,13 @@
         <v>44964</v>
       </c>
       <c r="B363" s="109" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="C363" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D363" s="75">
-        <v>33603712</v>
+        <v>33581478</v>
       </c>
       <c r="E363" s="109" t="s">
         <v>155</v>
@@ -18095,22 +18118,22 @@
         <v>777</v>
       </c>
       <c r="H363" s="112" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="I363" s="111" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="J363" s="111" t="s">
-        <v>1022</v>
+        <v>1016</v>
       </c>
       <c r="K363" s="111" t="s">
-        <v>641</v>
+        <v>885</v>
       </c>
       <c r="L363" s="113">
         <v>44968</v>
       </c>
       <c r="M363" s="114" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="364" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18118,13 +18141,13 @@
         <v>44964</v>
       </c>
       <c r="B364" s="109" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="C364" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D364" s="75">
-        <v>33581478</v>
+        <v>33571896</v>
       </c>
       <c r="E364" s="109" t="s">
         <v>155</v>
@@ -18136,13 +18159,13 @@
         <v>777</v>
       </c>
       <c r="H364" s="112" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="I364" s="111" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="J364" s="111" t="s">
-        <v>1016</v>
+        <v>884</v>
       </c>
       <c r="K364" s="111" t="s">
         <v>885</v>
@@ -18151,7 +18174,7 @@
         <v>44968</v>
       </c>
       <c r="M364" s="114" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="365" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18159,13 +18182,13 @@
         <v>44964</v>
       </c>
       <c r="B365" s="109" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="C365" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D365" s="75">
-        <v>33571896</v>
+        <v>33602734</v>
       </c>
       <c r="E365" s="109" t="s">
         <v>155</v>
@@ -18177,13 +18200,13 @@
         <v>777</v>
       </c>
       <c r="H365" s="112" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="I365" s="111" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="J365" s="111" t="s">
-        <v>884</v>
+        <v>892</v>
       </c>
       <c r="K365" s="111" t="s">
         <v>885</v>
@@ -18192,7 +18215,7 @@
         <v>44968</v>
       </c>
       <c r="M365" s="114" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="366" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18200,13 +18223,13 @@
         <v>44964</v>
       </c>
       <c r="B366" s="109" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="C366" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D366" s="75">
-        <v>33602734</v>
+        <v>33575532</v>
       </c>
       <c r="E366" s="109" t="s">
         <v>155</v>
@@ -18218,13 +18241,13 @@
         <v>777</v>
       </c>
       <c r="H366" s="112" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="I366" s="111" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="J366" s="111" t="s">
-        <v>892</v>
+        <v>1020</v>
       </c>
       <c r="K366" s="111" t="s">
         <v>885</v>
@@ -18233,7 +18256,7 @@
         <v>44968</v>
       </c>
       <c r="M366" s="114" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="367" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18241,13 +18264,13 @@
         <v>44964</v>
       </c>
       <c r="B367" s="109" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="C367" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D367" s="75">
-        <v>33575532</v>
+        <v>33585921</v>
       </c>
       <c r="E367" s="109" t="s">
         <v>155</v>
@@ -18259,22 +18282,22 @@
         <v>777</v>
       </c>
       <c r="H367" s="112" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="I367" s="111" t="s">
-        <v>1019</v>
+        <v>1032</v>
       </c>
       <c r="J367" s="111" t="s">
-        <v>1020</v>
+        <v>887</v>
       </c>
       <c r="K367" s="111" t="s">
-        <v>885</v>
+        <v>641</v>
       </c>
       <c r="L367" s="113">
         <v>44968</v>
       </c>
       <c r="M367" s="114" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="368" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18282,13 +18305,13 @@
         <v>44964</v>
       </c>
       <c r="B368" s="109" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="C368" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D368" s="75">
-        <v>33585921</v>
+        <v>33603487</v>
       </c>
       <c r="E368" s="109" t="s">
         <v>155</v>
@@ -18300,13 +18323,13 @@
         <v>777</v>
       </c>
       <c r="H368" s="112" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="I368" s="111" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="J368" s="111" t="s">
-        <v>887</v>
+        <v>1031</v>
       </c>
       <c r="K368" s="111" t="s">
         <v>641</v>
@@ -18315,48 +18338,46 @@
         <v>44968</v>
       </c>
       <c r="M368" s="114" t="s">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="369" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A369" s="108">
-        <v>44964</v>
-      </c>
-      <c r="B369" s="109" t="s">
-        <v>871</v>
-      </c>
-      <c r="C369" s="109" t="s">
-        <v>76</v>
-      </c>
-      <c r="D369" s="75">
-        <v>33603487</v>
-      </c>
-      <c r="E369" s="109" t="s">
-        <v>155</v>
-      </c>
-      <c r="F369" s="110">
-        <v>90</v>
-      </c>
-      <c r="G369" s="111" t="s">
-        <v>777</v>
-      </c>
-      <c r="H369" s="112" t="s">
-        <v>1030</v>
-      </c>
-      <c r="I369" s="111" t="s">
-        <v>1033</v>
-      </c>
-      <c r="J369" s="111" t="s">
-        <v>1031</v>
-      </c>
-      <c r="K369" s="111" t="s">
-        <v>641</v>
-      </c>
-      <c r="L369" s="113">
-        <v>44968</v>
-      </c>
-      <c r="M369" s="114" t="s">
         <v>1012</v>
+      </c>
+    </row>
+    <row r="369" spans="1:13" s="138" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A369" s="129">
+        <v>44993</v>
+      </c>
+      <c r="B369" s="130" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C369" s="130" t="s">
+        <v>76</v>
+      </c>
+      <c r="D369" s="131">
+        <v>55320856</v>
+      </c>
+      <c r="E369" s="130" t="s">
+        <v>86</v>
+      </c>
+      <c r="F369" s="132">
+        <v>110.5</v>
+      </c>
+      <c r="G369" s="133" t="s">
+        <v>821</v>
+      </c>
+      <c r="H369" s="134" t="s">
+        <v>775</v>
+      </c>
+      <c r="I369" s="133" t="s">
+        <v>370</v>
+      </c>
+      <c r="J369" s="133" t="s">
+        <v>822</v>
+      </c>
+      <c r="K369" s="135"/>
+      <c r="L369" s="136" t="s">
+        <v>1036</v>
+      </c>
+      <c r="M369" s="137" t="s">
+        <v>1037</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ooredoo event: request completed
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1372" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1E2594B-E548-46C9-AA09-B73C05BE8D3E}"/>
+  <xr:revisionPtr revIDLastSave="1376" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{339D41A6-D093-45BC-B227-B4626ECFB285}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
+    <workbookView xWindow="32160" yWindow="3360" windowWidth="21600" windowHeight="11235" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="OoredooMasterFile" sheetId="2" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2362" uniqueCount="1038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2361" uniqueCount="1037">
   <si>
     <t>ICC ID</t>
   </si>
@@ -3258,13 +3258,11 @@
     <t>8997401002220201412</t>
   </si>
   <si>
-    <t>R-1</t>
-  </si>
-  <si>
     <t>Upgraded from Plan C to Plan D at November 15, 2022
 02-Feb-2023 @11:47 - FIXING OOREDOO BILLING FOR 11 ACCOUNTS
 08-Feb-2023 @11:31 - Request was Completed with Plan D; 
-08-Mar-2023 @15:42 - Sim Card Replacement</t>
+08-Mar-2023 @15:42 - Sim Card Replacement
+09-Mar-2023 @09:50 - Request was Completed with Plan D; Replacement sim card has been activated</t>
   </si>
 </sst>
 </file>
@@ -3402,7 +3400,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3478,12 +3476,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4021,14 +4013,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -18341,7 +18333,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="369" spans="1:13" s="138" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:13" s="137" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A369" s="129">
         <v>44993</v>
       </c>
@@ -18373,11 +18365,11 @@
         <v>822</v>
       </c>
       <c r="K369" s="135"/>
-      <c r="L369" s="136" t="s">
+      <c r="L369" s="138">
+        <v>44994</v>
+      </c>
+      <c r="M369" s="136" t="s">
         <v>1036</v>
-      </c>
-      <c r="M369" s="137" t="s">
-        <v>1037</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some minor update for Ooredoo Master File
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1376" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{339D41A6-D093-45BC-B227-B4626ECFB285}"/>
+  <xr:revisionPtr revIDLastSave="1413" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F6F6963-A329-4B6C-9483-81993B2A1FD1}"/>
   <bookViews>
-    <workbookView xWindow="32160" yWindow="3360" windowWidth="21600" windowHeight="11235" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="OoredooMasterFile" sheetId="2" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2361" uniqueCount="1037">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2370" uniqueCount="1042">
   <si>
     <t>ICC ID</t>
   </si>
@@ -3263,6 +3263,21 @@
 08-Feb-2023 @11:31 - Request was Completed with Plan D; 
 08-Mar-2023 @15:42 - Sim Card Replacement
 09-Mar-2023 @09:50 - Request was Completed with Plan D; Replacement sim card has been activated</t>
+  </si>
+  <si>
+    <t>8997401002232058057</t>
+  </si>
+  <si>
+    <t>R-1</t>
+  </si>
+  <si>
+    <t>14-Mar-2023 @09:00 - Ooredoo Sim Requested with Plan A; Requested by QHSE Manager to Mr. Hussam - Approved</t>
+  </si>
+  <si>
+    <t>HSET DEPARTMENT</t>
+  </si>
+  <si>
+    <t>HSET</t>
   </si>
 </sst>
 </file>
@@ -3400,7 +3415,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3476,6 +3491,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3626,7 +3647,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4021,6 +4042,12 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="14" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5027,8 +5054,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}" name="OoredooActiveUsers" displayName="OoredooActiveUsers" ref="A2:M369" headerRowDxfId="74" totalsRowDxfId="71" headerRowBorderDxfId="73" tableBorderDxfId="72">
-  <autoFilter ref="A2:M369" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}" name="OoredooActiveUsers" displayName="OoredooActiveUsers" ref="A2:M370" headerRowDxfId="74" totalsRowDxfId="71" headerRowBorderDxfId="73" tableBorderDxfId="72">
+  <autoFilter ref="A2:M370" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:M369">
     <sortCondition ref="A2:A369"/>
   </sortState>
@@ -5359,13 +5386,13 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:W369"/>
+  <dimension ref="A1:W370"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="J359" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E363" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A370" sqref="A370"/>
+      <selection pane="bottomRight" activeCell="F371" sqref="F371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18370,6 +18397,42 @@
       </c>
       <c r="M369" s="136" t="s">
         <v>1036</v>
+      </c>
+    </row>
+    <row r="370" spans="1:13" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A370" s="108">
+        <v>44999</v>
+      </c>
+      <c r="B370" s="109" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C370" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D370" s="139"/>
+      <c r="E370" s="109" t="s">
+        <v>127</v>
+      </c>
+      <c r="F370" s="110">
+        <v>58.5</v>
+      </c>
+      <c r="G370" s="111" t="s">
+        <v>821</v>
+      </c>
+      <c r="H370" s="112" t="s">
+        <v>1041</v>
+      </c>
+      <c r="I370" s="111" t="s">
+        <v>1040</v>
+      </c>
+      <c r="J370" s="111" t="s">
+        <v>1040</v>
+      </c>
+      <c r="L370" s="140" t="s">
+        <v>1038</v>
+      </c>
+      <c r="M370" s="114" t="s">
+        <v>1039</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ooredoo event: added 2 new connection
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1413" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F6F6963-A329-4B6C-9483-81993B2A1FD1}"/>
+  <xr:revisionPtr revIDLastSave="1441" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D4FBBB1-946A-419C-821A-A60F37D26871}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2370" uniqueCount="1042">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2388" uniqueCount="1053">
   <si>
     <t>ICC ID</t>
   </si>
@@ -3278,6 +3278,39 @@
   </si>
   <si>
     <t>HSET</t>
+  </si>
+  <si>
+    <t>8997401002232058065</t>
+  </si>
+  <si>
+    <t>FINANCE DEPARTMENT</t>
+  </si>
+  <si>
+    <t>DEPARTMENT</t>
+  </si>
+  <si>
+    <t>R-2</t>
+  </si>
+  <si>
+    <t>19-Mar-2023 @11:42 - Ooredoo Sim Requested with Plan A; Approved by Mr. Hussam via Email</t>
+  </si>
+  <si>
+    <t>8997401002232058073</t>
+  </si>
+  <si>
+    <t>RISK &amp; QUALITY DEPARTMENT</t>
+  </si>
+  <si>
+    <t>R-3</t>
+  </si>
+  <si>
+    <t>19-Mar-2023 @11:43 - Ooredoo Sim Requested with Plan A; Approved by Mr. Hussam via Email</t>
+  </si>
+  <si>
+    <t>FINANCE</t>
+  </si>
+  <si>
+    <t>RISK &amp; QUALITY</t>
   </si>
 </sst>
 </file>
@@ -5054,8 +5087,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}" name="OoredooActiveUsers" displayName="OoredooActiveUsers" ref="A2:M370" headerRowDxfId="74" totalsRowDxfId="71" headerRowBorderDxfId="73" tableBorderDxfId="72">
-  <autoFilter ref="A2:M370" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}" name="OoredooActiveUsers" displayName="OoredooActiveUsers" ref="A2:M372" headerRowDxfId="74" totalsRowDxfId="71" headerRowBorderDxfId="73" tableBorderDxfId="72">
+  <autoFilter ref="A2:M372" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:M369">
     <sortCondition ref="A2:A369"/>
   </sortState>
@@ -5386,13 +5419,13 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:W370"/>
+  <dimension ref="A1:W372"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E363" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F371" sqref="F371"/>
+      <selection pane="bottomRight" activeCell="B373" sqref="B373"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18433,6 +18466,78 @@
       </c>
       <c r="M370" s="114" t="s">
         <v>1039</v>
+      </c>
+    </row>
+    <row r="371" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A371" s="108">
+        <v>45004</v>
+      </c>
+      <c r="B371" s="109" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C371" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D371" s="139"/>
+      <c r="E371" s="109" t="s">
+        <v>127</v>
+      </c>
+      <c r="F371" s="110">
+        <v>58.5</v>
+      </c>
+      <c r="G371" s="111" t="s">
+        <v>821</v>
+      </c>
+      <c r="H371" s="112" t="s">
+        <v>1051</v>
+      </c>
+      <c r="I371" s="111" t="s">
+        <v>1043</v>
+      </c>
+      <c r="J371" s="111" t="s">
+        <v>1044</v>
+      </c>
+      <c r="L371" s="140" t="s">
+        <v>1045</v>
+      </c>
+      <c r="M371" s="114" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="372" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A372" s="108">
+        <v>45004</v>
+      </c>
+      <c r="B372" s="109" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C372" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D372" s="139"/>
+      <c r="E372" s="109" t="s">
+        <v>127</v>
+      </c>
+      <c r="F372" s="110">
+        <v>58.5</v>
+      </c>
+      <c r="G372" s="111" t="s">
+        <v>821</v>
+      </c>
+      <c r="H372" s="112" t="s">
+        <v>1052</v>
+      </c>
+      <c r="I372" s="111" t="s">
+        <v>1048</v>
+      </c>
+      <c r="J372" s="111" t="s">
+        <v>1044</v>
+      </c>
+      <c r="L372" s="140" t="s">
+        <v>1049</v>
+      </c>
+      <c r="M372" s="114" t="s">
+        <v>1050</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ooredoo event: added 1 new connection
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1441" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D4FBBB1-946A-419C-821A-A60F37D26871}"/>
+  <xr:revisionPtr revIDLastSave="1480" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAB00E2F-C826-433B-9B18-0886695ADE82}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="OoredooMasterFile" sheetId="2" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2388" uniqueCount="1053">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2398" uniqueCount="1057">
   <si>
     <t>ICC ID</t>
   </si>
@@ -2505,10 +2505,6 @@
   </si>
   <si>
     <t>Cancelled (55683664)</t>
-  </si>
-  <si>
-    <t>22-Jan-2023 @10:10 - Requested to be Cancelled by Finance Dept.
-23-Jan-2023 @09:32 - Request was Completed with Plan A; Cancellation of Service Number with its Plan A was Completed (SR: 12521424)</t>
   </si>
   <si>
     <t>8997401002220201016</t>
@@ -3311,6 +3307,22 @@
   </si>
   <si>
     <t>RISK &amp; QUALITY</t>
+  </si>
+  <si>
+    <t>22-Jan-2023 @10:10 - Requested to be Cancelled by Finance Dept. as per HR's Old Ooredoo Master File.
+23-Jan-2023 @09:32 - Request was Completed with Plan A; Cancellation of Service Number with its Plan A was Completed (SR: 12521424)</t>
+  </si>
+  <si>
+    <t>8997401002232058081</t>
+  </si>
+  <si>
+    <t>ARUN SELASTIN PUSHPAM</t>
+  </si>
+  <si>
+    <t>R-4</t>
+  </si>
+  <si>
+    <t>20-Mar-2023 @10:01 - Ooredoo Sim Requested with Plan A; Previous Service Number is 55683664 but was Cancelled due to misunderstanding between Finance and HR Depts. and old Ooredoo Master File Records - New Service Connection was applied with the same Plan details as the old one</t>
   </si>
 </sst>
 </file>
@@ -5087,8 +5099,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}" name="OoredooActiveUsers" displayName="OoredooActiveUsers" ref="A2:M372" headerRowDxfId="74" totalsRowDxfId="71" headerRowBorderDxfId="73" tableBorderDxfId="72">
-  <autoFilter ref="A2:M372" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}" name="OoredooActiveUsers" displayName="OoredooActiveUsers" ref="A2:M373" headerRowDxfId="74" totalsRowDxfId="71" headerRowBorderDxfId="73" tableBorderDxfId="72">
+  <autoFilter ref="A2:M373" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:M369">
     <sortCondition ref="A2:A369"/>
   </sortState>
@@ -5419,13 +5431,13 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:W372"/>
+  <dimension ref="A1:W373"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E363" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E369" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B373" sqref="B373"/>
+      <selection pane="bottomRight" activeCell="B374" sqref="B374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5453,7 +5465,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="95" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="87" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B1" s="87"/>
       <c r="C1" s="88"/>
@@ -15997,7 +16009,7 @@
         <v>44949</v>
       </c>
       <c r="M311" s="99" t="s">
-        <v>807</v>
+        <v>1052</v>
       </c>
       <c r="N311" s="7"/>
       <c r="O311" s="7"/>
@@ -16015,13 +16027,13 @@
         <v>44956</v>
       </c>
       <c r="B312" s="120" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C312" s="120" t="s">
         <v>76</v>
       </c>
       <c r="D312" s="69" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E312" s="120" t="s">
         <v>155</v>
@@ -16030,16 +16042,16 @@
         <v>90</v>
       </c>
       <c r="G312" s="122" t="s">
+        <v>808</v>
+      </c>
+      <c r="H312" s="123" t="s">
         <v>809</v>
       </c>
-      <c r="H312" s="123" t="s">
+      <c r="I312" s="122" t="s">
         <v>810</v>
       </c>
-      <c r="I312" s="122" t="s">
+      <c r="J312" s="122" t="s">
         <v>811</v>
-      </c>
-      <c r="J312" s="122" t="s">
-        <v>812</v>
       </c>
       <c r="K312" s="122" t="s">
         <v>585</v>
@@ -16048,7 +16060,7 @@
         <v>44958</v>
       </c>
       <c r="M312" s="125" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="N312"/>
       <c r="O312"/>
@@ -16099,7 +16111,7 @@
         <v>44965</v>
       </c>
       <c r="M313" s="99" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="314" spans="1:23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -16122,7 +16134,7 @@
         <v>110.5</v>
       </c>
       <c r="G314" s="39" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="H314" s="45" t="s">
         <v>149</v>
@@ -16131,14 +16143,14 @@
         <v>150</v>
       </c>
       <c r="J314" s="39" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="K314" s="16"/>
       <c r="L314" s="48">
         <v>44965</v>
       </c>
       <c r="M314" s="106" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="315" spans="1:23" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -16161,13 +16173,13 @@
         <v>110.5</v>
       </c>
       <c r="G315" s="16" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="H315" s="17" t="s">
         <v>88</v>
       </c>
       <c r="I315" s="16" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="J315" s="16"/>
       <c r="K315" s="16"/>
@@ -16175,7 +16187,7 @@
         <v>44965</v>
       </c>
       <c r="M315" s="99" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="N315"/>
       <c r="O315"/>
@@ -16217,14 +16229,14 @@
         <v>203</v>
       </c>
       <c r="J316" s="16" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="K316" s="16"/>
       <c r="L316" s="48">
         <v>44965</v>
       </c>
       <c r="M316" s="99" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="N316"/>
       <c r="O316"/>
@@ -16263,7 +16275,7 @@
         <v>88</v>
       </c>
       <c r="I317" s="16" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="J317" s="16"/>
       <c r="K317" s="16"/>
@@ -16271,7 +16283,7 @@
         <v>44965</v>
       </c>
       <c r="M317" s="99" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="N317"/>
       <c r="O317"/>
@@ -16318,7 +16330,7 @@
         <v>44965</v>
       </c>
       <c r="M318" s="99" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="N318"/>
       <c r="O318"/>
@@ -16360,16 +16372,16 @@
         <v>532</v>
       </c>
       <c r="J319" s="16" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="K319" s="16" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="L319" s="48">
         <v>44965</v>
       </c>
       <c r="M319" s="99" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="N319"/>
       <c r="O319"/>
@@ -16411,16 +16423,16 @@
         <v>538</v>
       </c>
       <c r="J320" s="16" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="K320" s="16" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="L320" s="48">
         <v>44965</v>
       </c>
       <c r="M320" s="99" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="321" spans="1:23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -16457,7 +16469,7 @@
         <v>44965</v>
       </c>
       <c r="M321" s="107" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="322" spans="1:23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -16496,7 +16508,7 @@
         <v>44965</v>
       </c>
       <c r="M322" s="99" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="323" spans="1:23" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -16510,7 +16522,7 @@
         <v>76</v>
       </c>
       <c r="D323" s="17" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="E323" s="126" t="s">
         <v>77</v>
@@ -16519,7 +16531,7 @@
         <v>195</v>
       </c>
       <c r="G323" s="16" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="H323" s="17" t="s">
         <v>79</v>
@@ -16528,14 +16540,14 @@
         <v>80</v>
       </c>
       <c r="J323" s="16" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="K323" s="16"/>
       <c r="L323" s="119">
         <v>44965</v>
       </c>
       <c r="M323" s="128" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="N323"/>
       <c r="O323"/>
@@ -16553,7 +16565,7 @@
         <v>44964</v>
       </c>
       <c r="B324" s="109" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C324" s="109" t="s">
         <v>76</v>
@@ -16571,22 +16583,22 @@
         <v>777</v>
       </c>
       <c r="H324" s="112" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="I324" s="111" t="s">
+        <v>882</v>
+      </c>
+      <c r="J324" s="111" t="s">
         <v>883</v>
       </c>
-      <c r="J324" s="111" t="s">
+      <c r="K324" s="122" t="s">
         <v>884</v>
-      </c>
-      <c r="K324" s="122" t="s">
-        <v>885</v>
       </c>
       <c r="L324" s="113">
         <v>44968</v>
       </c>
       <c r="M324" s="114" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="325" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16594,7 +16606,7 @@
         <v>44964</v>
       </c>
       <c r="B325" s="109" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C325" s="109" t="s">
         <v>76</v>
@@ -16612,22 +16624,22 @@
         <v>777</v>
       </c>
       <c r="H325" s="112" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="I325" s="111" t="s">
+        <v>885</v>
+      </c>
+      <c r="J325" s="111" t="s">
         <v>886</v>
       </c>
-      <c r="J325" s="111" t="s">
+      <c r="K325" s="111" t="s">
         <v>887</v>
-      </c>
-      <c r="K325" s="111" t="s">
-        <v>888</v>
       </c>
       <c r="L325" s="113">
         <v>44968</v>
       </c>
       <c r="M325" s="114" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="326" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16635,7 +16647,7 @@
         <v>44964</v>
       </c>
       <c r="B326" s="109" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C326" s="109" t="s">
         <v>76</v>
@@ -16653,13 +16665,13 @@
         <v>777</v>
       </c>
       <c r="H326" s="112" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="I326" s="111" t="s">
+        <v>888</v>
+      </c>
+      <c r="J326" s="111" t="s">
         <v>889</v>
-      </c>
-      <c r="J326" s="111" t="s">
-        <v>890</v>
       </c>
       <c r="K326" s="111" t="s">
         <v>641</v>
@@ -16668,7 +16680,7 @@
         <v>44968</v>
       </c>
       <c r="M326" s="114" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="327" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16676,7 +16688,7 @@
         <v>44964</v>
       </c>
       <c r="B327" s="109" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C327" s="109" t="s">
         <v>76</v>
@@ -16694,13 +16706,13 @@
         <v>777</v>
       </c>
       <c r="H327" s="112" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="I327" s="111" t="s">
+        <v>890</v>
+      </c>
+      <c r="J327" s="111" t="s">
         <v>891</v>
-      </c>
-      <c r="J327" s="111" t="s">
-        <v>892</v>
       </c>
       <c r="K327" s="111" t="s">
         <v>641</v>
@@ -16709,7 +16721,7 @@
         <v>44968</v>
       </c>
       <c r="M327" s="114" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="328" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16717,7 +16729,7 @@
         <v>44964</v>
       </c>
       <c r="B328" s="109" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C328" s="109" t="s">
         <v>76</v>
@@ -16735,22 +16747,22 @@
         <v>777</v>
       </c>
       <c r="H328" s="112" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="I328" s="111" t="s">
+        <v>892</v>
+      </c>
+      <c r="J328" s="111" t="s">
         <v>893</v>
       </c>
-      <c r="J328" s="111" t="s">
-        <v>894</v>
-      </c>
       <c r="K328" s="111" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="L328" s="113">
         <v>44968</v>
       </c>
       <c r="M328" s="114" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="329" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16758,7 +16770,7 @@
         <v>44964</v>
       </c>
       <c r="B329" s="109" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C329" s="109" t="s">
         <v>76</v>
@@ -16776,22 +16788,22 @@
         <v>777</v>
       </c>
       <c r="H329" s="112" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="I329" s="111" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="J329" s="111" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="K329" s="111" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="L329" s="113">
         <v>44968</v>
       </c>
       <c r="M329" s="114" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="330" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16799,7 +16811,7 @@
         <v>44964</v>
       </c>
       <c r="B330" s="109" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C330" s="109" t="s">
         <v>76</v>
@@ -16817,13 +16829,13 @@
         <v>777</v>
       </c>
       <c r="H330" s="112" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="I330" s="111" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="J330" s="111" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="K330" s="111" t="s">
         <v>641</v>
@@ -16832,7 +16844,7 @@
         <v>44968</v>
       </c>
       <c r="M330" s="114" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="331" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16840,7 +16852,7 @@
         <v>44964</v>
       </c>
       <c r="B331" s="109" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C331" s="109" t="s">
         <v>76</v>
@@ -16858,22 +16870,22 @@
         <v>777</v>
       </c>
       <c r="H331" s="112" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="I331" s="111" t="s">
+        <v>896</v>
+      </c>
+      <c r="J331" s="111" t="s">
         <v>897</v>
       </c>
-      <c r="J331" s="111" t="s">
-        <v>898</v>
-      </c>
       <c r="K331" s="111" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="L331" s="113">
         <v>44968</v>
       </c>
       <c r="M331" s="114" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="332" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16881,7 +16893,7 @@
         <v>44964</v>
       </c>
       <c r="B332" s="109" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C332" s="109" t="s">
         <v>76</v>
@@ -16899,22 +16911,22 @@
         <v>777</v>
       </c>
       <c r="H332" s="112" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="I332" s="111" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="J332" s="111" t="s">
+        <v>883</v>
+      </c>
+      <c r="K332" s="111" t="s">
         <v>884</v>
-      </c>
-      <c r="K332" s="111" t="s">
-        <v>885</v>
       </c>
       <c r="L332" s="113">
         <v>44968</v>
       </c>
       <c r="M332" s="114" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="333" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16922,7 +16934,7 @@
         <v>44964</v>
       </c>
       <c r="B333" s="109" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C333" s="109" t="s">
         <v>76</v>
@@ -16940,22 +16952,22 @@
         <v>777</v>
       </c>
       <c r="H333" s="112" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="I333" s="111" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="J333" s="111" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="K333" s="111" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="L333" s="113">
         <v>44968</v>
       </c>
       <c r="M333" s="114" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="334" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16963,7 +16975,7 @@
         <v>44964</v>
       </c>
       <c r="B334" s="109" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C334" s="109" t="s">
         <v>76</v>
@@ -16981,22 +16993,22 @@
         <v>777</v>
       </c>
       <c r="H334" s="112" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="I334" s="111" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="J334" s="111" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="K334" s="111" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="L334" s="113">
         <v>44968</v>
       </c>
       <c r="M334" s="114" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="335" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -17004,7 +17016,7 @@
         <v>44964</v>
       </c>
       <c r="B335" s="109" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C335" s="109" t="s">
         <v>76</v>
@@ -17022,13 +17034,13 @@
         <v>777</v>
       </c>
       <c r="H335" s="112" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="I335" s="111" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="J335" s="111" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="K335" s="111" t="s">
         <v>641</v>
@@ -17037,7 +17049,7 @@
         <v>44968</v>
       </c>
       <c r="M335" s="114" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="336" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -17045,7 +17057,7 @@
         <v>44964</v>
       </c>
       <c r="B336" s="109" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C336" s="109" t="s">
         <v>76</v>
@@ -17063,13 +17075,13 @@
         <v>777</v>
       </c>
       <c r="H336" s="112" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="I336" s="111" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="J336" s="111" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="K336" s="111" t="s">
         <v>641</v>
@@ -17078,7 +17090,7 @@
         <v>44968</v>
       </c>
       <c r="M336" s="114" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="337" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17086,7 +17098,7 @@
         <v>44964</v>
       </c>
       <c r="B337" s="109" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C337" s="109" t="s">
         <v>76</v>
@@ -17104,22 +17116,22 @@
         <v>777</v>
       </c>
       <c r="H337" s="112" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="I337" s="111" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="J337" s="111" t="s">
         <v>268</v>
       </c>
       <c r="K337" s="111" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="L337" s="113">
         <v>44968</v>
       </c>
       <c r="M337" s="114" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="338" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17127,7 +17139,7 @@
         <v>44964</v>
       </c>
       <c r="B338" s="109" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C338" s="109" t="s">
         <v>76</v>
@@ -17145,22 +17157,22 @@
         <v>777</v>
       </c>
       <c r="H338" s="112" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="I338" s="111" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="J338" s="111" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="K338" s="111" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="L338" s="113">
         <v>44968</v>
       </c>
       <c r="M338" s="114" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="339" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17168,7 +17180,7 @@
         <v>44964</v>
       </c>
       <c r="B339" s="109" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C339" s="109" t="s">
         <v>76</v>
@@ -17186,13 +17198,13 @@
         <v>777</v>
       </c>
       <c r="H339" s="112" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="I339" s="111" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="J339" s="111" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="K339" s="111" t="s">
         <v>641</v>
@@ -17201,7 +17213,7 @@
         <v>44968</v>
       </c>
       <c r="M339" s="114" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="340" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17209,7 +17221,7 @@
         <v>44964</v>
       </c>
       <c r="B340" s="109" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C340" s="109" t="s">
         <v>76</v>
@@ -17227,22 +17239,22 @@
         <v>777</v>
       </c>
       <c r="H340" s="112" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="I340" s="111" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="J340" s="111" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="K340" s="111" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="L340" s="113">
         <v>44968</v>
       </c>
       <c r="M340" s="114" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="341" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17250,7 +17262,7 @@
         <v>44964</v>
       </c>
       <c r="B341" s="109" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C341" s="109" t="s">
         <v>76</v>
@@ -17268,13 +17280,13 @@
         <v>777</v>
       </c>
       <c r="H341" s="112" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="I341" s="111" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="J341" s="111" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="K341" s="111" t="s">
         <v>641</v>
@@ -17283,7 +17295,7 @@
         <v>44968</v>
       </c>
       <c r="M341" s="114" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="342" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17291,7 +17303,7 @@
         <v>44964</v>
       </c>
       <c r="B342" s="109" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C342" s="109" t="s">
         <v>76</v>
@@ -17309,22 +17321,22 @@
         <v>777</v>
       </c>
       <c r="H342" s="112" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="I342" s="111" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="J342" s="111" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="K342" s="111" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="L342" s="113">
         <v>44968</v>
       </c>
       <c r="M342" s="114" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="343" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17332,7 +17344,7 @@
         <v>44964</v>
       </c>
       <c r="B343" s="109" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="C343" s="109" t="s">
         <v>76</v>
@@ -17350,13 +17362,13 @@
         <v>777</v>
       </c>
       <c r="H343" s="112" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="I343" s="111" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="J343" s="111" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="K343" s="111" t="s">
         <v>641</v>
@@ -17365,7 +17377,7 @@
         <v>44968</v>
       </c>
       <c r="M343" s="114" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="344" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17373,7 +17385,7 @@
         <v>44964</v>
       </c>
       <c r="B344" s="109" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="C344" s="109" t="s">
         <v>76</v>
@@ -17391,13 +17403,13 @@
         <v>777</v>
       </c>
       <c r="H344" s="112" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I344" s="111" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="J344" s="111" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="K344" s="111" t="s">
         <v>641</v>
@@ -17406,7 +17418,7 @@
         <v>44968</v>
       </c>
       <c r="M344" s="114" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="345" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17414,7 +17426,7 @@
         <v>44964</v>
       </c>
       <c r="B345" s="109" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C345" s="109" t="s">
         <v>76</v>
@@ -17432,22 +17444,22 @@
         <v>777</v>
       </c>
       <c r="H345" s="112" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I345" s="111" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="J345" s="111" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="K345" s="111" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="L345" s="113">
         <v>44968</v>
       </c>
       <c r="M345" s="114" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="346" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17455,7 +17467,7 @@
         <v>44964</v>
       </c>
       <c r="B346" s="109" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C346" s="109" t="s">
         <v>76</v>
@@ -17473,22 +17485,22 @@
         <v>777</v>
       </c>
       <c r="H346" s="112" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="I346" s="111" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="J346" s="111" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="K346" s="111" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="L346" s="113">
         <v>44968</v>
       </c>
       <c r="M346" s="114" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="347" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17496,7 +17508,7 @@
         <v>44964</v>
       </c>
       <c r="B347" s="109" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C347" s="109" t="s">
         <v>76</v>
@@ -17514,22 +17526,22 @@
         <v>777</v>
       </c>
       <c r="H347" s="112" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="I347" s="111" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="J347" s="111" t="s">
+        <v>883</v>
+      </c>
+      <c r="K347" s="111" t="s">
         <v>884</v>
-      </c>
-      <c r="K347" s="111" t="s">
-        <v>885</v>
       </c>
       <c r="L347" s="113">
         <v>44968</v>
       </c>
       <c r="M347" s="114" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="348" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17537,7 +17549,7 @@
         <v>44964</v>
       </c>
       <c r="B348" s="109" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C348" s="109" t="s">
         <v>76</v>
@@ -17555,22 +17567,22 @@
         <v>777</v>
       </c>
       <c r="H348" s="112" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="I348" s="111" t="s">
+        <v>914</v>
+      </c>
+      <c r="J348" s="111" t="s">
         <v>915</v>
       </c>
-      <c r="J348" s="111" t="s">
-        <v>916</v>
-      </c>
       <c r="K348" s="111" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="L348" s="113">
         <v>44968</v>
       </c>
       <c r="M348" s="114" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="349" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17578,7 +17590,7 @@
         <v>44964</v>
       </c>
       <c r="B349" s="109" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C349" s="109" t="s">
         <v>76</v>
@@ -17596,22 +17608,22 @@
         <v>777</v>
       </c>
       <c r="H349" s="112" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="I349" s="111" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="J349" s="111" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="K349" s="111" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="L349" s="113">
         <v>44968</v>
       </c>
       <c r="M349" s="114" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="350" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17619,7 +17631,7 @@
         <v>44964</v>
       </c>
       <c r="B350" s="109" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C350" s="109" t="s">
         <v>76</v>
@@ -17637,22 +17649,22 @@
         <v>777</v>
       </c>
       <c r="H350" s="112" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="I350" s="111" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="J350" s="111" t="s">
+        <v>883</v>
+      </c>
+      <c r="K350" s="111" t="s">
         <v>884</v>
-      </c>
-      <c r="K350" s="111" t="s">
-        <v>885</v>
       </c>
       <c r="L350" s="113">
         <v>44968</v>
       </c>
       <c r="M350" s="114" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="351" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17660,7 +17672,7 @@
         <v>44964</v>
       </c>
       <c r="B351" s="109" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C351" s="109" t="s">
         <v>76</v>
@@ -17678,22 +17690,22 @@
         <v>777</v>
       </c>
       <c r="H351" s="112" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="I351" s="111" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="J351" s="111" t="s">
+        <v>883</v>
+      </c>
+      <c r="K351" s="111" t="s">
         <v>884</v>
-      </c>
-      <c r="K351" s="111" t="s">
-        <v>885</v>
       </c>
       <c r="L351" s="113">
         <v>44968</v>
       </c>
       <c r="M351" s="114" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="352" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17701,7 +17713,7 @@
         <v>44964</v>
       </c>
       <c r="B352" s="109" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C352" s="109" t="s">
         <v>76</v>
@@ -17719,13 +17731,13 @@
         <v>777</v>
       </c>
       <c r="H352" s="112" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="I352" s="111" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="J352" s="111" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="K352" s="111" t="s">
         <v>641</v>
@@ -17734,7 +17746,7 @@
         <v>44968</v>
       </c>
       <c r="M352" s="114" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="353" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17742,7 +17754,7 @@
         <v>44964</v>
       </c>
       <c r="B353" s="109" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C353" s="109" t="s">
         <v>76</v>
@@ -17760,13 +17772,13 @@
         <v>777</v>
       </c>
       <c r="H353" s="112" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="I353" s="111" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="J353" s="111" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="K353" s="111" t="s">
         <v>641</v>
@@ -17775,7 +17787,7 @@
         <v>44968</v>
       </c>
       <c r="M353" s="114" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="354" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17783,7 +17795,7 @@
         <v>44964</v>
       </c>
       <c r="B354" s="109" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C354" s="109" t="s">
         <v>76</v>
@@ -17801,13 +17813,13 @@
         <v>777</v>
       </c>
       <c r="H354" s="112" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="I354" s="111" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="J354" s="111" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="K354" s="111" t="s">
         <v>641</v>
@@ -17816,7 +17828,7 @@
         <v>44968</v>
       </c>
       <c r="M354" s="114" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="355" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17824,7 +17836,7 @@
         <v>44964</v>
       </c>
       <c r="B355" s="109" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C355" s="109" t="s">
         <v>76</v>
@@ -17842,22 +17854,22 @@
         <v>777</v>
       </c>
       <c r="H355" s="112" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="I355" s="111" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="J355" s="111" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="K355" s="111" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="L355" s="113">
         <v>44968</v>
       </c>
       <c r="M355" s="114" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="356" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17865,7 +17877,7 @@
         <v>44964</v>
       </c>
       <c r="B356" s="109" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C356" s="109" t="s">
         <v>76</v>
@@ -17883,22 +17895,22 @@
         <v>777</v>
       </c>
       <c r="H356" s="112" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="I356" s="111" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="J356" s="111" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="K356" s="111" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="L356" s="113">
         <v>44968</v>
       </c>
       <c r="M356" s="114" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="357" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17906,7 +17918,7 @@
         <v>44964</v>
       </c>
       <c r="B357" s="109" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C357" s="109" t="s">
         <v>76</v>
@@ -17924,13 +17936,13 @@
         <v>777</v>
       </c>
       <c r="H357" s="112" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="I357" s="111" t="s">
+        <v>924</v>
+      </c>
+      <c r="J357" s="111" t="s">
         <v>925</v>
-      </c>
-      <c r="J357" s="111" t="s">
-        <v>926</v>
       </c>
       <c r="K357" s="111" t="s">
         <v>641</v>
@@ -17939,7 +17951,7 @@
         <v>44968</v>
       </c>
       <c r="M357" s="114" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="358" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17947,7 +17959,7 @@
         <v>44964</v>
       </c>
       <c r="B358" s="109" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C358" s="109" t="s">
         <v>76</v>
@@ -17965,13 +17977,13 @@
         <v>777</v>
       </c>
       <c r="H358" s="112" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="I358" s="111" t="s">
+        <v>926</v>
+      </c>
+      <c r="J358" s="111" t="s">
         <v>927</v>
-      </c>
-      <c r="J358" s="111" t="s">
-        <v>928</v>
       </c>
       <c r="K358" s="111" t="s">
         <v>641</v>
@@ -17980,7 +17992,7 @@
         <v>44968</v>
       </c>
       <c r="M358" s="114" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="359" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17988,7 +18000,7 @@
         <v>44964</v>
       </c>
       <c r="B359" s="109" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C359" s="109" t="s">
         <v>76</v>
@@ -18006,13 +18018,13 @@
         <v>777</v>
       </c>
       <c r="H359" s="112" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="I359" s="111" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="J359" s="111" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="K359" s="111" t="s">
         <v>641</v>
@@ -18021,7 +18033,7 @@
         <v>44968</v>
       </c>
       <c r="M359" s="114" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="360" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18029,7 +18041,7 @@
         <v>44964</v>
       </c>
       <c r="B360" s="109" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C360" s="109" t="s">
         <v>76</v>
@@ -18047,22 +18059,22 @@
         <v>777</v>
       </c>
       <c r="H360" s="112" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="I360" s="111" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="J360" s="111" t="s">
+        <v>883</v>
+      </c>
+      <c r="K360" s="111" t="s">
         <v>884</v>
-      </c>
-      <c r="K360" s="111" t="s">
-        <v>885</v>
       </c>
       <c r="L360" s="113">
         <v>44968</v>
       </c>
       <c r="M360" s="114" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="361" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18070,7 +18082,7 @@
         <v>44964</v>
       </c>
       <c r="B361" s="109" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C361" s="109" t="s">
         <v>76</v>
@@ -18088,22 +18100,22 @@
         <v>777</v>
       </c>
       <c r="H361" s="112" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="I361" s="111" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="J361" s="111" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="K361" s="111" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="L361" s="113">
         <v>44968</v>
       </c>
       <c r="M361" s="114" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="362" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18111,7 +18123,7 @@
         <v>44964</v>
       </c>
       <c r="B362" s="109" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="C362" s="109" t="s">
         <v>76</v>
@@ -18129,13 +18141,13 @@
         <v>777</v>
       </c>
       <c r="H362" s="112" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="I362" s="111" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="J362" s="111" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="K362" s="111" t="s">
         <v>641</v>
@@ -18144,7 +18156,7 @@
         <v>44968</v>
       </c>
       <c r="M362" s="114" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="363" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18152,7 +18164,7 @@
         <v>44964</v>
       </c>
       <c r="B363" s="109" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C363" s="109" t="s">
         <v>76</v>
@@ -18170,22 +18182,22 @@
         <v>777</v>
       </c>
       <c r="H363" s="112" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I363" s="111" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J363" s="111" t="s">
         <v>1015</v>
       </c>
-      <c r="J363" s="111" t="s">
-        <v>1016</v>
-      </c>
       <c r="K363" s="111" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="L363" s="113">
         <v>44968</v>
       </c>
       <c r="M363" s="114" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="364" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18193,7 +18205,7 @@
         <v>44964</v>
       </c>
       <c r="B364" s="109" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C364" s="109" t="s">
         <v>76</v>
@@ -18211,22 +18223,22 @@
         <v>777</v>
       </c>
       <c r="H364" s="112" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="I364" s="111" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="J364" s="111" t="s">
+        <v>883</v>
+      </c>
+      <c r="K364" s="111" t="s">
         <v>884</v>
-      </c>
-      <c r="K364" s="111" t="s">
-        <v>885</v>
       </c>
       <c r="L364" s="113">
         <v>44968</v>
       </c>
       <c r="M364" s="114" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="365" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18234,7 +18246,7 @@
         <v>44964</v>
       </c>
       <c r="B365" s="109" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C365" s="109" t="s">
         <v>76</v>
@@ -18252,22 +18264,22 @@
         <v>777</v>
       </c>
       <c r="H365" s="112" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="I365" s="111" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="J365" s="111" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="K365" s="111" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="L365" s="113">
         <v>44968</v>
       </c>
       <c r="M365" s="114" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="366" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18275,7 +18287,7 @@
         <v>44964</v>
       </c>
       <c r="B366" s="109" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C366" s="109" t="s">
         <v>76</v>
@@ -18293,22 +18305,22 @@
         <v>777</v>
       </c>
       <c r="H366" s="112" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="I366" s="111" t="s">
+        <v>1018</v>
+      </c>
+      <c r="J366" s="111" t="s">
         <v>1019</v>
       </c>
-      <c r="J366" s="111" t="s">
-        <v>1020</v>
-      </c>
       <c r="K366" s="111" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="L366" s="113">
         <v>44968</v>
       </c>
       <c r="M366" s="114" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="367" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18316,7 +18328,7 @@
         <v>44964</v>
       </c>
       <c r="B367" s="109" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="C367" s="109" t="s">
         <v>76</v>
@@ -18334,13 +18346,13 @@
         <v>777</v>
       </c>
       <c r="H367" s="112" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="I367" s="111" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="J367" s="111" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="K367" s="111" t="s">
         <v>641</v>
@@ -18349,7 +18361,7 @@
         <v>44968</v>
       </c>
       <c r="M367" s="114" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="368" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18357,7 +18369,7 @@
         <v>44964</v>
       </c>
       <c r="B368" s="109" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="C368" s="109" t="s">
         <v>76</v>
@@ -18375,13 +18387,13 @@
         <v>777</v>
       </c>
       <c r="H368" s="112" t="s">
+        <v>1029</v>
+      </c>
+      <c r="I368" s="111" t="s">
+        <v>1032</v>
+      </c>
+      <c r="J368" s="111" t="s">
         <v>1030</v>
-      </c>
-      <c r="I368" s="111" t="s">
-        <v>1033</v>
-      </c>
-      <c r="J368" s="111" t="s">
-        <v>1031</v>
       </c>
       <c r="K368" s="111" t="s">
         <v>641</v>
@@ -18390,7 +18402,7 @@
         <v>44968</v>
       </c>
       <c r="M368" s="114" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="369" spans="1:13" s="137" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -18398,7 +18410,7 @@
         <v>44993</v>
       </c>
       <c r="B369" s="130" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="C369" s="130" t="s">
         <v>76</v>
@@ -18413,7 +18425,7 @@
         <v>110.5</v>
       </c>
       <c r="G369" s="133" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="H369" s="134" t="s">
         <v>775</v>
@@ -18422,14 +18434,14 @@
         <v>370</v>
       </c>
       <c r="J369" s="133" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="K369" s="135"/>
       <c r="L369" s="138">
         <v>44994</v>
       </c>
       <c r="M369" s="136" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="370" spans="1:13" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18437,7 +18449,7 @@
         <v>44999</v>
       </c>
       <c r="B370" s="109" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="C370" s="109" t="s">
         <v>76</v>
@@ -18450,22 +18462,22 @@
         <v>58.5</v>
       </c>
       <c r="G370" s="111" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="H370" s="112" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="I370" s="111" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="J370" s="111" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="L370" s="140" t="s">
+        <v>1037</v>
+      </c>
+      <c r="M370" s="114" t="s">
         <v>1038</v>
-      </c>
-      <c r="M370" s="114" t="s">
-        <v>1039</v>
       </c>
     </row>
     <row r="371" spans="1:13" x14ac:dyDescent="0.3">
@@ -18473,7 +18485,7 @@
         <v>45004</v>
       </c>
       <c r="B371" s="109" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="C371" s="109" t="s">
         <v>76</v>
@@ -18486,22 +18498,22 @@
         <v>58.5</v>
       </c>
       <c r="G371" s="111" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="H371" s="112" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="I371" s="111" t="s">
+        <v>1042</v>
+      </c>
+      <c r="J371" s="111" t="s">
         <v>1043</v>
       </c>
-      <c r="J371" s="111" t="s">
+      <c r="L371" s="140" t="s">
         <v>1044</v>
       </c>
-      <c r="L371" s="140" t="s">
+      <c r="M371" s="114" t="s">
         <v>1045</v>
-      </c>
-      <c r="M371" s="114" t="s">
-        <v>1046</v>
       </c>
     </row>
     <row r="372" spans="1:13" x14ac:dyDescent="0.3">
@@ -18509,7 +18521,7 @@
         <v>45004</v>
       </c>
       <c r="B372" s="109" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="C372" s="109" t="s">
         <v>76</v>
@@ -18522,22 +18534,61 @@
         <v>58.5</v>
       </c>
       <c r="G372" s="111" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="H372" s="112" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="I372" s="111" t="s">
+        <v>1047</v>
+      </c>
+      <c r="J372" s="111" t="s">
+        <v>1043</v>
+      </c>
+      <c r="L372" s="140" t="s">
         <v>1048</v>
       </c>
-      <c r="J372" s="111" t="s">
-        <v>1044</v>
-      </c>
-      <c r="L372" s="140" t="s">
+      <c r="M372" s="114" t="s">
         <v>1049</v>
       </c>
-      <c r="M372" s="114" t="s">
-        <v>1050</v>
+    </row>
+    <row r="373" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A373" s="108">
+        <v>45005</v>
+      </c>
+      <c r="B373" s="109" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C373" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D373" s="139"/>
+      <c r="E373" s="109" t="s">
+        <v>127</v>
+      </c>
+      <c r="F373" s="110">
+        <v>58.5</v>
+      </c>
+      <c r="G373" s="111" t="s">
+        <v>777</v>
+      </c>
+      <c r="H373" s="112" t="s">
+        <v>592</v>
+      </c>
+      <c r="I373" s="111" t="s">
+        <v>1054</v>
+      </c>
+      <c r="J373" s="111" t="s">
+        <v>590</v>
+      </c>
+      <c r="K373" s="111" t="s">
+        <v>585</v>
+      </c>
+      <c r="L373" s="140" t="s">
+        <v>1055</v>
+      </c>
+      <c r="M373" s="114" t="s">
+        <v>1056</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ooredoo event: completed 3 requests
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1480" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAB00E2F-C826-433B-9B18-0886695ADE82}"/>
+  <xr:revisionPtr revIDLastSave="1498" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A6D7674-FC7B-42E3-A1F9-E9109D545631}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
+    <workbookView xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="8880" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="OoredooMasterFile" sheetId="2" r:id="rId1"/>
@@ -3264,12 +3264,6 @@
     <t>8997401002232058057</t>
   </si>
   <si>
-    <t>R-1</t>
-  </si>
-  <si>
-    <t>14-Mar-2023 @09:00 - Ooredoo Sim Requested with Plan A; Requested by QHSE Manager to Mr. Hussam - Approved</t>
-  </si>
-  <si>
     <t>HSET DEPARTMENT</t>
   </si>
   <si>
@@ -3285,22 +3279,10 @@
     <t>DEPARTMENT</t>
   </si>
   <si>
-    <t>R-2</t>
-  </si>
-  <si>
-    <t>19-Mar-2023 @11:42 - Ooredoo Sim Requested with Plan A; Approved by Mr. Hussam via Email</t>
-  </si>
-  <si>
     <t>8997401002232058073</t>
   </si>
   <si>
     <t>RISK &amp; QUALITY DEPARTMENT</t>
-  </si>
-  <si>
-    <t>R-3</t>
-  </si>
-  <si>
-    <t>19-Mar-2023 @11:43 - Ooredoo Sim Requested with Plan A; Approved by Mr. Hussam via Email</t>
   </si>
   <si>
     <t>FINANCE</t>
@@ -3323,6 +3305,27 @@
   </si>
   <si>
     <t>20-Mar-2023 @10:01 - Ooredoo Sim Requested with Plan A; Previous Service Number is 55683664 but was Cancelled due to misunderstanding between Finance and HR Depts. and old Ooredoo Master File Records - New Service Connection was applied with the same Plan details as the old one</t>
+  </si>
+  <si>
+    <t>66169486</t>
+  </si>
+  <si>
+    <t>14-Mar-2023 @09:00 - Ooredoo Sim Requested with Plan A; Requested by QHSE Manager to Mr. Hussam - Approved
+21-Mar-2023 @08:33 - Request was Completed; Service Number is 66169486 with Plan A; Request Completed</t>
+  </si>
+  <si>
+    <t>55952391</t>
+  </si>
+  <si>
+    <t>19-Mar-2023 @11:42 - Ooredoo Sim Requested with Plan A; Approved by Mr. Hussam via Email
+21-Mar-2023 @08:34 - Request was Completed; Service Number is 55952391 with Plan A; Request Completed</t>
+  </si>
+  <si>
+    <t>33108762</t>
+  </si>
+  <si>
+    <t>19-Mar-2023 @11:43 - Ooredoo Sim Requested with Plan A; Approved by Mr. Hussam via Email
+21-Mar-2023 @08:34 - Request was Completed; Service Number is 33108762 with Plan A; Request Completed</t>
   </si>
 </sst>
 </file>
@@ -3692,7 +3695,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4092,6 +4095,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="14" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -16009,7 +16015,7 @@
         <v>44949</v>
       </c>
       <c r="M311" s="99" t="s">
-        <v>1052</v>
+        <v>1046</v>
       </c>
       <c r="N311" s="7"/>
       <c r="O311" s="7"/>
@@ -18454,7 +18460,9 @@
       <c r="C370" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D370" s="139"/>
+      <c r="D370" s="75" t="s">
+        <v>1051</v>
+      </c>
       <c r="E370" s="109" t="s">
         <v>127</v>
       </c>
@@ -18465,32 +18473,34 @@
         <v>820</v>
       </c>
       <c r="H370" s="112" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="I370" s="111" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="J370" s="111" t="s">
-        <v>1039</v>
-      </c>
-      <c r="L370" s="140" t="s">
         <v>1037</v>
       </c>
+      <c r="L370" s="113">
+        <v>45006</v>
+      </c>
       <c r="M370" s="114" t="s">
-        <v>1038</v>
-      </c>
-    </row>
-    <row r="371" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="371" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A371" s="108">
         <v>45004</v>
       </c>
       <c r="B371" s="109" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="C371" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D371" s="139"/>
+      <c r="D371" s="75" t="s">
+        <v>1053</v>
+      </c>
       <c r="E371" s="109" t="s">
         <v>127</v>
       </c>
@@ -18501,32 +18511,34 @@
         <v>820</v>
       </c>
       <c r="H371" s="112" t="s">
-        <v>1050</v>
+        <v>1044</v>
       </c>
       <c r="I371" s="111" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="J371" s="111" t="s">
-        <v>1043</v>
-      </c>
-      <c r="L371" s="140" t="s">
-        <v>1044</v>
+        <v>1041</v>
+      </c>
+      <c r="L371" s="113">
+        <v>45006</v>
       </c>
       <c r="M371" s="114" t="s">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="372" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="372" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A372" s="108">
         <v>45004</v>
       </c>
       <c r="B372" s="109" t="s">
-        <v>1046</v>
+        <v>1042</v>
       </c>
       <c r="C372" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D372" s="139"/>
+      <c r="D372" s="141" t="s">
+        <v>1055</v>
+      </c>
       <c r="E372" s="109" t="s">
         <v>127</v>
       </c>
@@ -18537,19 +18549,19 @@
         <v>820</v>
       </c>
       <c r="H372" s="112" t="s">
-        <v>1051</v>
+        <v>1045</v>
       </c>
       <c r="I372" s="111" t="s">
-        <v>1047</v>
+        <v>1043</v>
       </c>
       <c r="J372" s="111" t="s">
-        <v>1043</v>
-      </c>
-      <c r="L372" s="140" t="s">
-        <v>1048</v>
+        <v>1041</v>
+      </c>
+      <c r="L372" s="113">
+        <v>45006</v>
       </c>
       <c r="M372" s="114" t="s">
-        <v>1049</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="373" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18557,7 +18569,7 @@
         <v>45005</v>
       </c>
       <c r="B373" s="109" t="s">
-        <v>1053</v>
+        <v>1047</v>
       </c>
       <c r="C373" s="109" t="s">
         <v>76</v>
@@ -18576,7 +18588,7 @@
         <v>592</v>
       </c>
       <c r="I373" s="111" t="s">
-        <v>1054</v>
+        <v>1048</v>
       </c>
       <c r="J373" s="111" t="s">
         <v>590</v>
@@ -18585,10 +18597,10 @@
         <v>585</v>
       </c>
       <c r="L373" s="140" t="s">
-        <v>1055</v>
+        <v>1049</v>
       </c>
       <c r="M373" s="114" t="s">
-        <v>1056</v>
+        <v>1050</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
slight modification on ooredoo master file
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1513" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4175605-75A7-46B5-B981-6F4265992DD8}"/>
+  <xr:revisionPtr revIDLastSave="1532" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05AB56AC-7259-4C39-ACF9-44959388DED0}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
@@ -2774,9 +2774,6 @@
     <t>MECHANICAL TECHNICIAN</t>
   </si>
   <si>
-    <t>MUHAMMAD MOHSIN HUSSAIN</t>
-  </si>
-  <si>
     <t>SENIOR ELECTRICAL TECHNICIAN</t>
   </si>
   <si>
@@ -2786,9 +2783,6 @@
     <t>ASSISTANT ELECTRICAL TECHNICIAN</t>
   </si>
   <si>
-    <t>UZAIR KHAN ANWAR KHAN</t>
-  </si>
-  <si>
     <t>SHOBASH KANDEL</t>
   </si>
   <si>
@@ -2903,13 +2897,7 @@
     <t>000758 - MECHANICAL/HVAC</t>
   </si>
   <si>
-    <t>001815 - ELECTRICAL</t>
-  </si>
-  <si>
     <t>001761 - ELECTRICAL</t>
-  </si>
-  <si>
-    <t>001764 - ELECTRICAL</t>
   </si>
   <si>
     <t>001814 - MECHANICAL/HVAC</t>
@@ -3347,6 +3335,18 @@
   </si>
   <si>
     <t>ECS SUPERVISOR</t>
+  </si>
+  <si>
+    <t>GILBERT NUWAHEREZA</t>
+  </si>
+  <si>
+    <t>BISMARK GYAMFI</t>
+  </si>
+  <si>
+    <t>000721 - MECHANICAL/HVAC</t>
+  </si>
+  <si>
+    <t>001847 - ELECTRICAL</t>
   </si>
 </sst>
 </file>
@@ -5458,10 +5458,10 @@
   <dimension ref="A1:W374"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="J366" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E366" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L375" sqref="L375"/>
+      <selection pane="bottomRight" activeCell="D374" sqref="D374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5489,7 +5489,7 @@
   <sheetData>
     <row r="1" spans="1:23" s="95" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="87" t="s">
-        <v>1033</v>
+        <v>1029</v>
       </c>
       <c r="B1" s="87"/>
       <c r="C1" s="88"/>
@@ -16033,7 +16033,7 @@
         <v>44949</v>
       </c>
       <c r="M311" s="99" t="s">
-        <v>1046</v>
+        <v>1042</v>
       </c>
       <c r="N311" s="7"/>
       <c r="O311" s="7"/>
@@ -16607,7 +16607,7 @@
         <v>777</v>
       </c>
       <c r="H324" s="112" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="I324" s="111" t="s">
         <v>882</v>
@@ -16622,7 +16622,7 @@
         <v>44968</v>
       </c>
       <c r="M324" s="114" t="s">
-        <v>967</v>
+        <v>963</v>
       </c>
     </row>
     <row r="325" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16648,7 +16648,7 @@
         <v>777</v>
       </c>
       <c r="H325" s="112" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="I325" s="111" t="s">
         <v>885</v>
@@ -16663,7 +16663,7 @@
         <v>44968</v>
       </c>
       <c r="M325" s="114" t="s">
-        <v>968</v>
+        <v>964</v>
       </c>
     </row>
     <row r="326" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16689,7 +16689,7 @@
         <v>777</v>
       </c>
       <c r="H326" s="112" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="I326" s="111" t="s">
         <v>888</v>
@@ -16704,7 +16704,7 @@
         <v>44968</v>
       </c>
       <c r="M326" s="114" t="s">
-        <v>969</v>
+        <v>965</v>
       </c>
     </row>
     <row r="327" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16730,22 +16730,22 @@
         <v>777</v>
       </c>
       <c r="H327" s="112" t="s">
-        <v>933</v>
+        <v>1063</v>
       </c>
       <c r="I327" s="111" t="s">
-        <v>890</v>
+        <v>1061</v>
       </c>
       <c r="J327" s="111" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="K327" s="111" t="s">
-        <v>641</v>
+        <v>887</v>
       </c>
       <c r="L327" s="113">
         <v>44968</v>
       </c>
       <c r="M327" s="114" t="s">
-        <v>970</v>
+        <v>966</v>
       </c>
     </row>
     <row r="328" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16771,13 +16771,13 @@
         <v>777</v>
       </c>
       <c r="H328" s="112" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="I328" s="111" t="s">
+        <v>891</v>
+      </c>
+      <c r="J328" s="111" t="s">
         <v>892</v>
-      </c>
-      <c r="J328" s="111" t="s">
-        <v>893</v>
       </c>
       <c r="K328" s="111" t="s">
         <v>887</v>
@@ -16786,7 +16786,7 @@
         <v>44968</v>
       </c>
       <c r="M328" s="114" t="s">
-        <v>971</v>
+        <v>967</v>
       </c>
     </row>
     <row r="329" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16812,22 +16812,22 @@
         <v>777</v>
       </c>
       <c r="H329" s="112" t="s">
-        <v>935</v>
+        <v>1062</v>
       </c>
       <c r="I329" s="111" t="s">
-        <v>894</v>
+        <v>1060</v>
       </c>
       <c r="J329" s="111" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
       <c r="K329" s="111" t="s">
-        <v>887</v>
+        <v>641</v>
       </c>
       <c r="L329" s="113">
         <v>44968</v>
       </c>
       <c r="M329" s="114" t="s">
-        <v>972</v>
+        <v>968</v>
       </c>
     </row>
     <row r="330" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16853,10 +16853,10 @@
         <v>777</v>
       </c>
       <c r="H330" s="112" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
       <c r="I330" s="111" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="J330" s="111" t="s">
         <v>889</v>
@@ -16868,7 +16868,7 @@
         <v>44968</v>
       </c>
       <c r="M330" s="114" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
     </row>
     <row r="331" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16894,13 +16894,13 @@
         <v>777</v>
       </c>
       <c r="H331" s="112" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="I331" s="111" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="J331" s="111" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="K331" s="111" t="s">
         <v>884</v>
@@ -16909,7 +16909,7 @@
         <v>44968</v>
       </c>
       <c r="M331" s="114" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
     </row>
     <row r="332" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16935,10 +16935,10 @@
         <v>777</v>
       </c>
       <c r="H332" s="112" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
       <c r="I332" s="111" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="J332" s="111" t="s">
         <v>883</v>
@@ -16950,7 +16950,7 @@
         <v>44968</v>
       </c>
       <c r="M332" s="114" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
     </row>
     <row r="333" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -16976,13 +16976,13 @@
         <v>777</v>
       </c>
       <c r="H333" s="112" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="I333" s="111" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="J333" s="111" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="K333" s="111" t="s">
         <v>884</v>
@@ -16991,7 +16991,7 @@
         <v>44968</v>
       </c>
       <c r="M333" s="114" t="s">
-        <v>976</v>
+        <v>972</v>
       </c>
     </row>
     <row r="334" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -17017,13 +17017,13 @@
         <v>777</v>
       </c>
       <c r="H334" s="112" t="s">
-        <v>940</v>
+        <v>936</v>
       </c>
       <c r="I334" s="111" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="J334" s="111" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="K334" s="111" t="s">
         <v>887</v>
@@ -17032,7 +17032,7 @@
         <v>44968</v>
       </c>
       <c r="M334" s="114" t="s">
-        <v>977</v>
+        <v>973</v>
       </c>
     </row>
     <row r="335" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -17058,13 +17058,13 @@
         <v>777</v>
       </c>
       <c r="H335" s="112" t="s">
-        <v>941</v>
+        <v>937</v>
       </c>
       <c r="I335" s="111" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="J335" s="111" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="K335" s="111" t="s">
         <v>641</v>
@@ -17073,7 +17073,7 @@
         <v>44968</v>
       </c>
       <c r="M335" s="114" t="s">
-        <v>978</v>
+        <v>974</v>
       </c>
     </row>
     <row r="336" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
@@ -17099,10 +17099,10 @@
         <v>777</v>
       </c>
       <c r="H336" s="112" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
       <c r="I336" s="111" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="J336" s="111" t="s">
         <v>889</v>
@@ -17114,7 +17114,7 @@
         <v>44968</v>
       </c>
       <c r="M336" s="114" t="s">
-        <v>979</v>
+        <v>975</v>
       </c>
     </row>
     <row r="337" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17140,10 +17140,10 @@
         <v>777</v>
       </c>
       <c r="H337" s="112" t="s">
-        <v>943</v>
+        <v>939</v>
       </c>
       <c r="I337" s="111" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="J337" s="111" t="s">
         <v>268</v>
@@ -17155,7 +17155,7 @@
         <v>44968</v>
       </c>
       <c r="M337" s="114" t="s">
-        <v>980</v>
+        <v>976</v>
       </c>
     </row>
     <row r="338" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17181,13 +17181,13 @@
         <v>777</v>
       </c>
       <c r="H338" s="112" t="s">
-        <v>944</v>
+        <v>940</v>
       </c>
       <c r="I338" s="111" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="J338" s="111" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="K338" s="111" t="s">
         <v>884</v>
@@ -17196,7 +17196,7 @@
         <v>44968</v>
       </c>
       <c r="M338" s="114" t="s">
-        <v>981</v>
+        <v>977</v>
       </c>
     </row>
     <row r="339" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17222,10 +17222,10 @@
         <v>777</v>
       </c>
       <c r="H339" s="112" t="s">
-        <v>945</v>
+        <v>941</v>
       </c>
       <c r="I339" s="111" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="J339" s="111" t="s">
         <v>886</v>
@@ -17237,7 +17237,7 @@
         <v>44968</v>
       </c>
       <c r="M339" s="114" t="s">
-        <v>982</v>
+        <v>978</v>
       </c>
     </row>
     <row r="340" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17263,13 +17263,13 @@
         <v>777</v>
       </c>
       <c r="H340" s="112" t="s">
-        <v>946</v>
+        <v>942</v>
       </c>
       <c r="I340" s="111" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="J340" s="111" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="K340" s="111" t="s">
         <v>884</v>
@@ -17278,7 +17278,7 @@
         <v>44968</v>
       </c>
       <c r="M340" s="114" t="s">
-        <v>983</v>
+        <v>979</v>
       </c>
     </row>
     <row r="341" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17304,10 +17304,10 @@
         <v>777</v>
       </c>
       <c r="H341" s="112" t="s">
-        <v>947</v>
+        <v>943</v>
       </c>
       <c r="I341" s="111" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="J341" s="111" t="s">
         <v>889</v>
@@ -17319,7 +17319,7 @@
         <v>44968</v>
       </c>
       <c r="M341" s="114" t="s">
-        <v>984</v>
+        <v>980</v>
       </c>
     </row>
     <row r="342" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17345,13 +17345,13 @@
         <v>777</v>
       </c>
       <c r="H342" s="112" t="s">
-        <v>948</v>
+        <v>944</v>
       </c>
       <c r="I342" s="111" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="J342" s="111" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="K342" s="111" t="s">
         <v>884</v>
@@ -17360,7 +17360,7 @@
         <v>44968</v>
       </c>
       <c r="M342" s="114" t="s">
-        <v>985</v>
+        <v>981</v>
       </c>
     </row>
     <row r="343" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17386,10 +17386,10 @@
         <v>777</v>
       </c>
       <c r="H343" s="112" t="s">
-        <v>949</v>
+        <v>945</v>
       </c>
       <c r="I343" s="111" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="J343" s="111" t="s">
         <v>886</v>
@@ -17401,7 +17401,7 @@
         <v>44968</v>
       </c>
       <c r="M343" s="114" t="s">
-        <v>986</v>
+        <v>982</v>
       </c>
     </row>
     <row r="344" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17427,10 +17427,10 @@
         <v>777</v>
       </c>
       <c r="H344" s="112" t="s">
-        <v>950</v>
+        <v>946</v>
       </c>
       <c r="I344" s="111" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="J344" s="111" t="s">
         <v>889</v>
@@ -17442,7 +17442,7 @@
         <v>44968</v>
       </c>
       <c r="M344" s="114" t="s">
-        <v>987</v>
+        <v>983</v>
       </c>
     </row>
     <row r="345" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17468,13 +17468,13 @@
         <v>777</v>
       </c>
       <c r="H345" s="112" t="s">
-        <v>951</v>
+        <v>947</v>
       </c>
       <c r="I345" s="111" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="J345" s="111" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="K345" s="111" t="s">
         <v>884</v>
@@ -17483,7 +17483,7 @@
         <v>44968</v>
       </c>
       <c r="M345" s="114" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
     </row>
     <row r="346" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17509,13 +17509,13 @@
         <v>777</v>
       </c>
       <c r="H346" s="112" t="s">
-        <v>952</v>
+        <v>948</v>
       </c>
       <c r="I346" s="111" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="J346" s="111" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="K346" s="111" t="s">
         <v>884</v>
@@ -17524,7 +17524,7 @@
         <v>44968</v>
       </c>
       <c r="M346" s="114" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
     </row>
     <row r="347" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17550,10 +17550,10 @@
         <v>777</v>
       </c>
       <c r="H347" s="112" t="s">
-        <v>953</v>
+        <v>949</v>
       </c>
       <c r="I347" s="111" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="J347" s="111" t="s">
         <v>883</v>
@@ -17565,7 +17565,7 @@
         <v>44968</v>
       </c>
       <c r="M347" s="114" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
     </row>
     <row r="348" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17591,13 +17591,13 @@
         <v>777</v>
       </c>
       <c r="H348" s="112" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
       <c r="I348" s="111" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="J348" s="111" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="K348" s="111" t="s">
         <v>887</v>
@@ -17606,7 +17606,7 @@
         <v>44968</v>
       </c>
       <c r="M348" s="114" t="s">
-        <v>991</v>
+        <v>987</v>
       </c>
     </row>
     <row r="349" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17632,13 +17632,13 @@
         <v>777</v>
       </c>
       <c r="H349" s="112" t="s">
-        <v>955</v>
+        <v>951</v>
       </c>
       <c r="I349" s="111" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="J349" s="111" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="K349" s="111" t="s">
         <v>884</v>
@@ -17647,7 +17647,7 @@
         <v>44968</v>
       </c>
       <c r="M349" s="114" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
     </row>
     <row r="350" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17673,10 +17673,10 @@
         <v>777</v>
       </c>
       <c r="H350" s="112" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="I350" s="111" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="J350" s="111" t="s">
         <v>883</v>
@@ -17688,7 +17688,7 @@
         <v>44968</v>
       </c>
       <c r="M350" s="114" t="s">
-        <v>993</v>
+        <v>989</v>
       </c>
     </row>
     <row r="351" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17714,10 +17714,10 @@
         <v>777</v>
       </c>
       <c r="H351" s="112" t="s">
-        <v>957</v>
+        <v>953</v>
       </c>
       <c r="I351" s="111" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="J351" s="111" t="s">
         <v>883</v>
@@ -17729,7 +17729,7 @@
         <v>44968</v>
       </c>
       <c r="M351" s="114" t="s">
-        <v>994</v>
+        <v>990</v>
       </c>
     </row>
     <row r="352" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17755,10 +17755,10 @@
         <v>777</v>
       </c>
       <c r="H352" s="112" t="s">
-        <v>958</v>
+        <v>954</v>
       </c>
       <c r="I352" s="111" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="J352" s="111" t="s">
         <v>889</v>
@@ -17770,7 +17770,7 @@
         <v>44968</v>
       </c>
       <c r="M352" s="114" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
     </row>
     <row r="353" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17796,10 +17796,10 @@
         <v>777</v>
       </c>
       <c r="H353" s="112" t="s">
-        <v>959</v>
+        <v>955</v>
       </c>
       <c r="I353" s="111" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="J353" s="111" t="s">
         <v>886</v>
@@ -17811,7 +17811,7 @@
         <v>44968</v>
       </c>
       <c r="M353" s="114" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
     </row>
     <row r="354" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17837,10 +17837,10 @@
         <v>777</v>
       </c>
       <c r="H354" s="112" t="s">
-        <v>960</v>
+        <v>956</v>
       </c>
       <c r="I354" s="111" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="J354" s="111" t="s">
         <v>889</v>
@@ -17852,7 +17852,7 @@
         <v>44968</v>
       </c>
       <c r="M354" s="114" t="s">
-        <v>997</v>
+        <v>993</v>
       </c>
     </row>
     <row r="355" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17878,13 +17878,13 @@
         <v>777</v>
       </c>
       <c r="H355" s="112" t="s">
-        <v>961</v>
+        <v>957</v>
       </c>
       <c r="I355" s="111" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="J355" s="111" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="K355" s="111" t="s">
         <v>884</v>
@@ -17893,7 +17893,7 @@
         <v>44968</v>
       </c>
       <c r="M355" s="114" t="s">
-        <v>998</v>
+        <v>994</v>
       </c>
     </row>
     <row r="356" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17919,13 +17919,13 @@
         <v>777</v>
       </c>
       <c r="H356" s="112" t="s">
-        <v>962</v>
+        <v>958</v>
       </c>
       <c r="I356" s="111" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="J356" s="111" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="K356" s="111" t="s">
         <v>884</v>
@@ -17934,7 +17934,7 @@
         <v>44968</v>
       </c>
       <c r="M356" s="114" t="s">
-        <v>999</v>
+        <v>995</v>
       </c>
     </row>
     <row r="357" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -17960,13 +17960,13 @@
         <v>777</v>
       </c>
       <c r="H357" s="112" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="I357" s="111" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="J357" s="111" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="K357" s="111" t="s">
         <v>641</v>
@@ -17975,7 +17975,7 @@
         <v>44968</v>
       </c>
       <c r="M357" s="114" t="s">
-        <v>1000</v>
+        <v>996</v>
       </c>
     </row>
     <row r="358" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18001,13 +18001,13 @@
         <v>777</v>
       </c>
       <c r="H358" s="112" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
       <c r="I358" s="111" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="J358" s="111" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="K358" s="111" t="s">
         <v>641</v>
@@ -18016,7 +18016,7 @@
         <v>44968</v>
       </c>
       <c r="M358" s="114" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
     </row>
     <row r="359" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18042,10 +18042,10 @@
         <v>777</v>
       </c>
       <c r="H359" s="112" t="s">
-        <v>965</v>
+        <v>961</v>
       </c>
       <c r="I359" s="111" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="J359" s="111" t="s">
         <v>889</v>
@@ -18057,7 +18057,7 @@
         <v>44968</v>
       </c>
       <c r="M359" s="114" t="s">
-        <v>1002</v>
+        <v>998</v>
       </c>
     </row>
     <row r="360" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18083,10 +18083,10 @@
         <v>777</v>
       </c>
       <c r="H360" s="112" t="s">
-        <v>966</v>
+        <v>962</v>
       </c>
       <c r="I360" s="111" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="J360" s="111" t="s">
         <v>883</v>
@@ -18098,7 +18098,7 @@
         <v>44968</v>
       </c>
       <c r="M360" s="114" t="s">
-        <v>1003</v>
+        <v>999</v>
       </c>
     </row>
     <row r="361" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18124,13 +18124,13 @@
         <v>777</v>
       </c>
       <c r="H361" s="112" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="I361" s="111" t="s">
-        <v>1012</v>
+        <v>1008</v>
       </c>
       <c r="J361" s="111" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
       <c r="K361" s="111" t="s">
         <v>884</v>
@@ -18139,7 +18139,7 @@
         <v>44968</v>
       </c>
       <c r="M361" s="114" t="s">
-        <v>1004</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="362" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18165,13 +18165,13 @@
         <v>777</v>
       </c>
       <c r="H362" s="112" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="I362" s="111" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="J362" s="111" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
       <c r="K362" s="111" t="s">
         <v>641</v>
@@ -18180,7 +18180,7 @@
         <v>44968</v>
       </c>
       <c r="M362" s="114" t="s">
-        <v>1005</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="363" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18206,13 +18206,13 @@
         <v>777</v>
       </c>
       <c r="H363" s="112" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
       <c r="I363" s="111" t="s">
-        <v>1014</v>
+        <v>1010</v>
       </c>
       <c r="J363" s="111" t="s">
-        <v>1015</v>
+        <v>1011</v>
       </c>
       <c r="K363" s="111" t="s">
         <v>884</v>
@@ -18221,7 +18221,7 @@
         <v>44968</v>
       </c>
       <c r="M363" s="114" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="364" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18247,10 +18247,10 @@
         <v>777</v>
       </c>
       <c r="H364" s="112" t="s">
-        <v>1025</v>
+        <v>1021</v>
       </c>
       <c r="I364" s="111" t="s">
-        <v>1016</v>
+        <v>1012</v>
       </c>
       <c r="J364" s="111" t="s">
         <v>883</v>
@@ -18262,7 +18262,7 @@
         <v>44968</v>
       </c>
       <c r="M364" s="114" t="s">
-        <v>1007</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="365" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18288,13 +18288,13 @@
         <v>777</v>
       </c>
       <c r="H365" s="112" t="s">
-        <v>1026</v>
+        <v>1022</v>
       </c>
       <c r="I365" s="111" t="s">
-        <v>1017</v>
+        <v>1013</v>
       </c>
       <c r="J365" s="111" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="K365" s="111" t="s">
         <v>884</v>
@@ -18303,7 +18303,7 @@
         <v>44968</v>
       </c>
       <c r="M365" s="114" t="s">
-        <v>1008</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="366" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18329,13 +18329,13 @@
         <v>777</v>
       </c>
       <c r="H366" s="112" t="s">
-        <v>1027</v>
+        <v>1023</v>
       </c>
       <c r="I366" s="111" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="J366" s="111" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="K366" s="111" t="s">
         <v>884</v>
@@ -18344,7 +18344,7 @@
         <v>44968</v>
       </c>
       <c r="M366" s="114" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="367" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18370,10 +18370,10 @@
         <v>777</v>
       </c>
       <c r="H367" s="112" t="s">
-        <v>1028</v>
+        <v>1024</v>
       </c>
       <c r="I367" s="111" t="s">
-        <v>1031</v>
+        <v>1027</v>
       </c>
       <c r="J367" s="111" t="s">
         <v>886</v>
@@ -18385,7 +18385,7 @@
         <v>44968</v>
       </c>
       <c r="M367" s="114" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="368" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18411,13 +18411,13 @@
         <v>777</v>
       </c>
       <c r="H368" s="112" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="I368" s="111" t="s">
-        <v>1032</v>
+        <v>1028</v>
       </c>
       <c r="J368" s="111" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
       <c r="K368" s="111" t="s">
         <v>641</v>
@@ -18426,7 +18426,7 @@
         <v>44968</v>
       </c>
       <c r="M368" s="114" t="s">
-        <v>1011</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="369" spans="1:13" s="137" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -18434,7 +18434,7 @@
         <v>44993</v>
       </c>
       <c r="B369" s="130" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
       <c r="C369" s="130" t="s">
         <v>76</v>
@@ -18465,7 +18465,7 @@
         <v>44994</v>
       </c>
       <c r="M369" s="136" t="s">
-        <v>1035</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="370" spans="1:13" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -18473,13 +18473,13 @@
         <v>44999</v>
       </c>
       <c r="B370" s="109" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
       <c r="C370" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D370" s="75" t="s">
-        <v>1051</v>
+        <v>1047</v>
       </c>
       <c r="E370" s="109" t="s">
         <v>127</v>
@@ -18491,19 +18491,19 @@
         <v>820</v>
       </c>
       <c r="H370" s="112" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="I370" s="111" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
       <c r="J370" s="111" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
       <c r="L370" s="113">
         <v>45006</v>
       </c>
       <c r="M370" s="114" t="s">
-        <v>1052</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="371" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18511,13 +18511,13 @@
         <v>45004</v>
       </c>
       <c r="B371" s="109" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
       <c r="C371" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D371" s="75" t="s">
-        <v>1053</v>
+        <v>1049</v>
       </c>
       <c r="E371" s="109" t="s">
         <v>127</v>
@@ -18529,19 +18529,19 @@
         <v>820</v>
       </c>
       <c r="H371" s="112" t="s">
-        <v>1044</v>
+        <v>1040</v>
       </c>
       <c r="I371" s="111" t="s">
-        <v>1040</v>
+        <v>1036</v>
       </c>
       <c r="J371" s="111" t="s">
-        <v>1041</v>
+        <v>1037</v>
       </c>
       <c r="L371" s="113">
         <v>45006</v>
       </c>
       <c r="M371" s="114" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="372" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18549,13 +18549,13 @@
         <v>45004</v>
       </c>
       <c r="B372" s="109" t="s">
-        <v>1042</v>
+        <v>1038</v>
       </c>
       <c r="C372" s="109" t="s">
         <v>76</v>
       </c>
       <c r="D372" s="75" t="s">
-        <v>1055</v>
+        <v>1051</v>
       </c>
       <c r="E372" s="109" t="s">
         <v>127</v>
@@ -18567,19 +18567,19 @@
         <v>820</v>
       </c>
       <c r="H372" s="112" t="s">
-        <v>1045</v>
+        <v>1041</v>
       </c>
       <c r="I372" s="111" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
       <c r="J372" s="111" t="s">
-        <v>1041</v>
+        <v>1037</v>
       </c>
       <c r="L372" s="113">
         <v>45006</v>
       </c>
       <c r="M372" s="114" t="s">
-        <v>1056</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="373" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18587,7 +18587,7 @@
         <v>45005</v>
       </c>
       <c r="B373" s="109" t="s">
-        <v>1047</v>
+        <v>1043</v>
       </c>
       <c r="C373" s="109" t="s">
         <v>76</v>
@@ -18606,7 +18606,7 @@
         <v>592</v>
       </c>
       <c r="I373" s="111" t="s">
-        <v>1048</v>
+        <v>1044</v>
       </c>
       <c r="J373" s="111" t="s">
         <v>590</v>
@@ -18615,10 +18615,10 @@
         <v>585</v>
       </c>
       <c r="L373" s="140" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
       <c r="M373" s="114" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="374" spans="1:13" x14ac:dyDescent="0.3">
@@ -18626,7 +18626,7 @@
         <v>45026</v>
       </c>
       <c r="B374" s="109" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
       <c r="C374" s="109" t="s">
         <v>76</v>
@@ -18639,25 +18639,25 @@
         <v>110.5</v>
       </c>
       <c r="G374" s="111" t="s">
-        <v>1058</v>
+        <v>1054</v>
       </c>
       <c r="H374" s="112" t="s">
+        <v>1055</v>
+      </c>
+      <c r="I374" s="111" t="s">
+        <v>1056</v>
+      </c>
+      <c r="J374" s="111" t="s">
         <v>1059</v>
-      </c>
-      <c r="I374" s="111" t="s">
-        <v>1060</v>
-      </c>
-      <c r="J374" s="111" t="s">
-        <v>1063</v>
       </c>
       <c r="K374" s="111" t="s">
         <v>608</v>
       </c>
       <c r="L374" s="140" t="s">
-        <v>1061</v>
+        <v>1057</v>
       </c>
       <c r="M374" s="114" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ooredoo event: completed 2 request
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1532" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05AB56AC-7259-4C39-ACF9-44959388DED0}"/>
+  <xr:revisionPtr revIDLastSave="1544" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B3A7CAC-C954-4365-95AF-36317E43A65E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
+    <workbookView xWindow="30135" yWindow="945" windowWidth="17280" windowHeight="8880" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="OoredooMasterFile" sheetId="2" r:id="rId1"/>
@@ -3289,12 +3289,6 @@
     <t>ARUN SELASTIN PUSHPAM</t>
   </si>
   <si>
-    <t>R-4</t>
-  </si>
-  <si>
-    <t>20-Mar-2023 @10:01 - Ooredoo Sim Requested with Plan A; Previous Service Number is 55683664 but was Cancelled due to misunderstanding between Finance and HR Depts. and old Ooredoo Master File Records - New Service Connection was applied with the same Plan details as the old one</t>
-  </si>
-  <si>
     <t>66169486</t>
   </si>
   <si>
@@ -3328,12 +3322,6 @@
     <t>KANNATHASAN K</t>
   </si>
   <si>
-    <t>R-1</t>
-  </si>
-  <si>
-    <t>10-Apr-2023 @12:08 - Ooredoo Sim Requested with Plan D; Request from MEP Team - Approved by HRM</t>
-  </si>
-  <si>
     <t>ECS SUPERVISOR</t>
   </si>
   <si>
@@ -3347,6 +3335,20 @@
   </si>
   <si>
     <t>001847 - ELECTRICAL</t>
+  </si>
+  <si>
+    <t>50766278</t>
+  </si>
+  <si>
+    <t>20-Mar-2023 @10:01 - Ooredoo Sim Requested with Plan A; Previous Service Number is 55683664 but was Cancelled due to misunderstanding between Finance and HR Depts. and old Ooredoo Master File Records - New Service Connection was applied with the same Plan details as the old one
+10-Apr-2023 @14:28 - Request was Completed; Service Number is 50766278 with Plan A; Request Completed</t>
+  </si>
+  <si>
+    <t>33632251</t>
+  </si>
+  <si>
+    <t>10-Apr-2023 @12:08 - Ooredoo Sim Requested with Plan D; Request from MEP Team - Approved by HRM
+10-Apr-2023 @14:28 - Request was Completed; Service Number is 33632251 with Plan D; Request Completed</t>
   </si>
 </sst>
 </file>
@@ -3484,7 +3486,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3560,12 +3562,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3716,7 +3712,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4112,10 +4108,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="14" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -16730,10 +16723,10 @@
         <v>777</v>
       </c>
       <c r="H327" s="112" t="s">
-        <v>1063</v>
+        <v>1059</v>
       </c>
       <c r="I327" s="111" t="s">
-        <v>1061</v>
+        <v>1057</v>
       </c>
       <c r="J327" s="111" t="s">
         <v>892</v>
@@ -16812,10 +16805,10 @@
         <v>777</v>
       </c>
       <c r="H329" s="112" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="I329" s="111" t="s">
-        <v>1060</v>
+        <v>1056</v>
       </c>
       <c r="J329" s="111" t="s">
         <v>889</v>
@@ -18479,7 +18472,7 @@
         <v>76</v>
       </c>
       <c r="D370" s="75" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="E370" s="109" t="s">
         <v>127</v>
@@ -18503,7 +18496,7 @@
         <v>45006</v>
       </c>
       <c r="M370" s="114" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="371" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18517,7 +18510,7 @@
         <v>76</v>
       </c>
       <c r="D371" s="75" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="E371" s="109" t="s">
         <v>127</v>
@@ -18541,7 +18534,7 @@
         <v>45006</v>
       </c>
       <c r="M371" s="114" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="372" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -18555,7 +18548,7 @@
         <v>76</v>
       </c>
       <c r="D372" s="75" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="E372" s="109" t="s">
         <v>127</v>
@@ -18579,10 +18572,10 @@
         <v>45006</v>
       </c>
       <c r="M372" s="114" t="s">
-        <v>1052</v>
-      </c>
-    </row>
-    <row r="373" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="373" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A373" s="108">
         <v>45005</v>
       </c>
@@ -18592,7 +18585,9 @@
       <c r="C373" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D373" s="139"/>
+      <c r="D373" s="75" t="s">
+        <v>1060</v>
+      </c>
       <c r="E373" s="109" t="s">
         <v>127</v>
       </c>
@@ -18614,24 +18609,26 @@
       <c r="K373" s="111" t="s">
         <v>585</v>
       </c>
-      <c r="L373" s="140" t="s">
-        <v>1045</v>
+      <c r="L373" s="113">
+        <v>45026</v>
       </c>
       <c r="M373" s="114" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="374" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="374" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A374" s="108">
         <v>45026</v>
       </c>
       <c r="B374" s="109" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="C374" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D374" s="139"/>
+      <c r="D374" s="139" t="s">
+        <v>1062</v>
+      </c>
       <c r="E374" s="109" t="s">
         <v>86</v>
       </c>
@@ -18639,25 +18636,25 @@
         <v>110.5</v>
       </c>
       <c r="G374" s="111" t="s">
+        <v>1052</v>
+      </c>
+      <c r="H374" s="112" t="s">
+        <v>1053</v>
+      </c>
+      <c r="I374" s="111" t="s">
         <v>1054</v>
       </c>
-      <c r="H374" s="112" t="s">
+      <c r="J374" s="111" t="s">
         <v>1055</v>
-      </c>
-      <c r="I374" s="111" t="s">
-        <v>1056</v>
-      </c>
-      <c r="J374" s="111" t="s">
-        <v>1059</v>
       </c>
       <c r="K374" s="111" t="s">
         <v>608</v>
       </c>
-      <c r="L374" s="140" t="s">
-        <v>1057</v>
+      <c r="L374" s="113">
+        <v>45026</v>
       </c>
       <c r="M374" s="114" t="s">
-        <v>1058</v>
+        <v>1063</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ooredoo event: requested 1 new sim connection
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1578" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0909D45-ADAF-442D-8B0B-BBC56B6F7FC6}"/>
+  <xr:revisionPtr revIDLastSave="1592" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B765E6AB-732B-4B2A-8316-922091C953FF}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
+    <workbookView xWindow="34485" yWindow="0" windowWidth="17250" windowHeight="8865" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="OoredooMasterFile" sheetId="2" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2413" uniqueCount="1067">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2423" uniqueCount="1074">
   <si>
     <t>ICC ID</t>
   </si>
@@ -3361,6 +3361,27 @@
   <si>
     <t>06-Jun-2023 @10:33 - Old User: 000304 - SHADAB ALAM BADRUDDIN; This number was handed over on June 2022
 06-Jun-2023 @10:37 - Request was Completed with Plan D; New Details Updated</t>
+  </si>
+  <si>
+    <t>8997401002232058511</t>
+  </si>
+  <si>
+    <t>Warehouse Staff</t>
+  </si>
+  <si>
+    <t>001874</t>
+  </si>
+  <si>
+    <t>ALAGARSAMY MARIMUTHU MARIMUTHU</t>
+  </si>
+  <si>
+    <t>EQUIPMENT TECHNICIAN</t>
+  </si>
+  <si>
+    <t>R-1</t>
+  </si>
+  <si>
+    <t>08-Jun-2023 @15:26 - Ooredoo Sim Requested with Plan A; Approved by Mr. Beshoy (DGM) for Plan A</t>
   </si>
 </sst>
 </file>
@@ -3498,7 +3519,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3574,6 +3595,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3724,7 +3751,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4148,6 +4175,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="14" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5155,8 +5188,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}" name="OoredooActiveUsers" displayName="OoredooActiveUsers" ref="A2:M374" headerRowDxfId="74" totalsRowDxfId="71" headerRowBorderDxfId="73" tableBorderDxfId="72">
-  <autoFilter ref="A2:M374" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}" name="OoredooActiveUsers" displayName="OoredooActiveUsers" ref="A2:M375" headerRowDxfId="74" totalsRowDxfId="71" headerRowBorderDxfId="73" tableBorderDxfId="72">
+  <autoFilter ref="A2:M375" xr:uid="{4AD2AC7E-012B-4F07-A206-33AFC7B8FBCF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:M374">
     <sortCondition ref="A2:A374"/>
   </sortState>
@@ -5487,7 +5520,7 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:W374"/>
+  <dimension ref="A1:W375"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="H361" activePane="bottomRight" state="frozen"/>
@@ -18707,6 +18740,45 @@
       </c>
       <c r="M374" s="143" t="s">
         <v>1066</v>
+      </c>
+    </row>
+    <row r="375" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A375" s="108">
+        <v>45085</v>
+      </c>
+      <c r="B375" s="109" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C375" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="D375" s="149"/>
+      <c r="E375" s="109" t="s">
+        <v>127</v>
+      </c>
+      <c r="F375" s="110">
+        <v>58.5</v>
+      </c>
+      <c r="G375" s="111" t="s">
+        <v>1068</v>
+      </c>
+      <c r="H375" s="112" t="s">
+        <v>1069</v>
+      </c>
+      <c r="I375" s="111" t="s">
+        <v>1070</v>
+      </c>
+      <c r="J375" s="111" t="s">
+        <v>1071</v>
+      </c>
+      <c r="K375" s="111" t="s">
+        <v>638</v>
+      </c>
+      <c r="L375" s="150" t="s">
+        <v>1072</v>
+      </c>
+      <c r="M375" s="114" t="s">
+        <v>1073</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ooredoo event: completed 1 request
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1592" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B765E6AB-732B-4B2A-8316-922091C953FF}"/>
+  <xr:revisionPtr revIDLastSave="1598" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66CC543C-AAFA-4EF4-8F4E-A6A2FD1263ED}"/>
   <bookViews>
-    <workbookView xWindow="34485" yWindow="0" windowWidth="17250" windowHeight="8865" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
+    <workbookView xWindow="30195" yWindow="1365" windowWidth="21600" windowHeight="11235" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="OoredooMasterFile" sheetId="2" r:id="rId1"/>
@@ -3378,10 +3378,11 @@
     <t>EQUIPMENT TECHNICIAN</t>
   </si>
   <si>
-    <t>R-1</t>
-  </si>
-  <si>
-    <t>08-Jun-2023 @15:26 - Ooredoo Sim Requested with Plan A; Approved by Mr. Beshoy (DGM) for Plan A</t>
+    <t>51159461</t>
+  </si>
+  <si>
+    <t>08-Jun-2023 @15:26 - Ooredoo Sim Requested with Plan A; Approved by Mr. Beshoy (DGM) for Plan A
+04-Jul-2023 @08:29 - Request was Completed; Service Number is 51159461 with Plan A; Completed Request on 15-June-23</t>
   </si>
 </sst>
 </file>
@@ -3519,7 +3520,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3595,12 +3596,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3751,7 +3746,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4177,10 +4172,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="14" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -18742,7 +18734,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="375" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A375" s="108">
         <v>45085</v>
       </c>
@@ -18752,7 +18744,9 @@
       <c r="C375" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D375" s="149"/>
+      <c r="D375" s="149" t="s">
+        <v>1072</v>
+      </c>
       <c r="E375" s="109" t="s">
         <v>127</v>
       </c>
@@ -18774,8 +18768,8 @@
       <c r="K375" s="111" t="s">
         <v>638</v>
       </c>
-      <c r="L375" s="150" t="s">
-        <v>1072</v>
+      <c r="L375" s="113">
+        <v>45111</v>
       </c>
       <c r="M375" s="114" t="s">
         <v>1073</v>

</xml_diff>

<commit_message>
ooredoo event: sim card replacement
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1598" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66CC543C-AAFA-4EF4-8F4E-A6A2FD1263ED}"/>
+  <xr:revisionPtr revIDLastSave="1605" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3986C511-D172-49C7-A1B2-F34BF752C1AC}"/>
   <bookViews>
     <workbookView xWindow="30195" yWindow="1365" windowWidth="21600" windowHeight="11235" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2423" uniqueCount="1074">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2424" uniqueCount="1075">
   <si>
     <t>ICC ID</t>
   </si>
@@ -3363,9 +3363,6 @@
 06-Jun-2023 @10:37 - Request was Completed with Plan D; New Details Updated</t>
   </si>
   <si>
-    <t>8997401002232058511</t>
-  </si>
-  <si>
     <t>Warehouse Staff</t>
   </si>
   <si>
@@ -3381,8 +3378,15 @@
     <t>51159461</t>
   </si>
   <si>
+    <t>8997401002232058107</t>
+  </si>
+  <si>
+    <t>R-1</t>
+  </si>
+  <si>
     <t>08-Jun-2023 @15:26 - Ooredoo Sim Requested with Plan A; Approved by Mr. Beshoy (DGM) for Plan A
-04-Jul-2023 @08:29 - Request was Completed; Service Number is 51159461 with Plan A; Completed Request on 15-June-23</t>
+04-Jul-2023 @08:29 - Request was Completed; Service Number is 51159461 with Plan A; Completed Request on 15-June-23
+04-Jul-2023 @16:14 - Request to Replace Sim Card with same details as before</t>
   </si>
 </sst>
 </file>
@@ -3520,7 +3524,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3596,6 +3600,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4172,7 +4182,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="14" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -18734,18 +18744,18 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="375" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A375" s="108">
-        <v>45085</v>
+        <v>45111</v>
       </c>
       <c r="B375" s="109" t="s">
-        <v>1067</v>
+        <v>1072</v>
       </c>
       <c r="C375" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="D375" s="149" t="s">
-        <v>1072</v>
+      <c r="D375" s="75" t="s">
+        <v>1071</v>
       </c>
       <c r="E375" s="109" t="s">
         <v>127</v>
@@ -18754,25 +18764,25 @@
         <v>58.5</v>
       </c>
       <c r="G375" s="111" t="s">
+        <v>1067</v>
+      </c>
+      <c r="H375" s="112" t="s">
         <v>1068</v>
       </c>
-      <c r="H375" s="112" t="s">
+      <c r="I375" s="111" t="s">
         <v>1069</v>
       </c>
-      <c r="I375" s="111" t="s">
+      <c r="J375" s="111" t="s">
         <v>1070</v>
-      </c>
-      <c r="J375" s="111" t="s">
-        <v>1071</v>
       </c>
       <c r="K375" s="111" t="s">
         <v>638</v>
       </c>
-      <c r="L375" s="113">
-        <v>45111</v>
+      <c r="L375" s="149" t="s">
+        <v>1073</v>
       </c>
       <c r="M375" s="114" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ooredoo event: 2 sim for cancellation
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1626" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D2304C1-9BC7-4812-834E-74F6E757418A}"/>
+  <xr:revisionPtr revIDLastSave="1638" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BDF60CC-DDD2-40F9-BDDF-A036F2FDE469}"/>
   <bookViews>
-    <workbookView xWindow="30210" yWindow="1395" windowWidth="17250" windowHeight="8865" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
+    <workbookView xWindow="30645" yWindow="1830" windowWidth="17250" windowHeight="8865" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="OoredooMasterFile" sheetId="2" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2423" uniqueCount="1075">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2427" uniqueCount="1079">
   <si>
     <t>ICC ID</t>
   </si>
@@ -3388,6 +3388,18 @@
 04-Jul-2023 @08:29 - Request was Completed; Service Number is 51159461 with Plan A; Completed Request on 15-June-23
 04-Jul-2023 @16:14 - Request to Replace Sim Card with same details as before
 23-Jul-2023 @12:20 - Request was Completed with Plan A; Completed request on last week of June 2023</t>
+  </si>
+  <si>
+    <t>R-1</t>
+  </si>
+  <si>
+    <t>24-Jul-2023 @10:18 - DEACTIVATED on 24-July-2023 as per Mr. Iraklis Request via Email</t>
+  </si>
+  <si>
+    <t>R-2</t>
+  </si>
+  <si>
+    <t>24-Jul-2023 @10:19 - DEACTIVATED on 24-July-2023 as per Mr. Iraklis request via Email</t>
   </si>
 </sst>
 </file>
@@ -3525,7 +3537,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3601,6 +3613,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3751,7 +3769,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4175,6 +4193,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7984,9 +8005,9 @@
       <c r="L73" s="48"/>
       <c r="M73" s="99"/>
     </row>
-    <row r="74" spans="1:13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="15">
-        <v>43831</v>
+        <v>45131</v>
       </c>
       <c r="B74" s="41" t="s">
         <v>418</v>
@@ -8014,8 +8035,12 @@
       </c>
       <c r="J74" s="16"/>
       <c r="K74" s="16"/>
-      <c r="L74" s="48"/>
-      <c r="M74" s="99"/>
+      <c r="L74" s="149" t="s">
+        <v>1075</v>
+      </c>
+      <c r="M74" s="99" t="s">
+        <v>1076</v>
+      </c>
     </row>
     <row r="75" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="15">
@@ -13393,7 +13418,7 @@
     </row>
     <row r="243" spans="1:23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A243" s="15">
-        <v>43831</v>
+        <v>45131</v>
       </c>
       <c r="B243" s="41" t="s">
         <v>6</v>
@@ -13419,8 +13444,12 @@
       </c>
       <c r="J243" s="16"/>
       <c r="K243" s="16"/>
-      <c r="L243" s="48"/>
-      <c r="M243" s="99"/>
+      <c r="L243" s="149" t="s">
+        <v>1077</v>
+      </c>
+      <c r="M243" s="99" t="s">
+        <v>1078</v>
+      </c>
     </row>
     <row r="244" spans="1:23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A244" s="15">

</xml_diff>

<commit_message>
ooredoo event: cancellation request completed
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1638" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BDF60CC-DDD2-40F9-BDDF-A036F2FDE469}"/>
+  <xr:revisionPtr revIDLastSave="1646" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{822F043E-9B9B-45F5-8ACC-CB9DBDE012DE}"/>
   <bookViews>
-    <workbookView xWindow="30645" yWindow="1830" windowWidth="17250" windowHeight="8865" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
+    <workbookView xWindow="33045" yWindow="4230" windowWidth="17250" windowHeight="8865" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="OoredooMasterFile" sheetId="2" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2427" uniqueCount="1079">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2425" uniqueCount="1077">
   <si>
     <t>ICC ID</t>
   </si>
@@ -3390,16 +3390,12 @@
 23-Jul-2023 @12:20 - Request was Completed with Plan A; Completed request on last week of June 2023</t>
   </si>
   <si>
-    <t>R-1</t>
-  </si>
-  <si>
-    <t>24-Jul-2023 @10:18 - DEACTIVATED on 24-July-2023 as per Mr. Iraklis Request via Email</t>
-  </si>
-  <si>
-    <t>R-2</t>
-  </si>
-  <si>
-    <t>24-Jul-2023 @10:19 - DEACTIVATED on 24-July-2023 as per Mr. Iraklis request via Email</t>
+    <t>24-Jul-2023 @10:18 - DEACTIVATED on 24-July-2023 as per Mr. Iraklis Request via Email
+27-Jul-2023 @16:05 - Request was Completed with Plan D; Request Completed</t>
+  </si>
+  <si>
+    <t>24-Jul-2023 @10:19 - DEACTIVATED on 24-July-2023 as per Mr. Iraklis request via Email
+27-Jul-2023 @16:05 - Request was Completed with Plan 500; Request Completed</t>
   </si>
 </sst>
 </file>
@@ -3537,7 +3533,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3613,12 +3609,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3769,7 +3759,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4193,9 +4183,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5535,10 +5522,10 @@
   <dimension ref="A1:W375"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E367" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E370" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I375" sqref="I375"/>
+      <selection pane="bottomRight" activeCell="D375" sqref="D375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8005,7 +7992,7 @@
       <c r="L73" s="48"/>
       <c r="M73" s="99"/>
     </row>
-    <row r="74" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="15">
         <v>45131</v>
       </c>
@@ -8035,11 +8022,11 @@
       </c>
       <c r="J74" s="16"/>
       <c r="K74" s="16"/>
-      <c r="L74" s="149" t="s">
+      <c r="L74" s="48">
+        <v>45134</v>
+      </c>
+      <c r="M74" s="99" t="s">
         <v>1075</v>
-      </c>
-      <c r="M74" s="99" t="s">
-        <v>1076</v>
       </c>
     </row>
     <row r="75" spans="1:13" customFormat="1" x14ac:dyDescent="0.3">
@@ -13416,7 +13403,7 @@
       <c r="L242" s="48"/>
       <c r="M242" s="99"/>
     </row>
-    <row r="243" spans="1:23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A243" s="15">
         <v>45131</v>
       </c>
@@ -13444,11 +13431,11 @@
       </c>
       <c r="J243" s="16"/>
       <c r="K243" s="16"/>
-      <c r="L243" s="149" t="s">
-        <v>1077</v>
+      <c r="L243" s="48">
+        <v>45134</v>
       </c>
       <c r="M243" s="99" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="244" spans="1:23" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ooredoo event: finished one request
</commit_message>
<xml_diff>
--- a/Commands/Database/OoredooMasterFile.xlsx
+++ b/Commands/Database/OoredooMasterFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acintercityfm-my.sharepoint.com/personal/jesimiel_saroza_acintercityfm_com/Documents/ACIFM Workspace/Ooredoo/#Work Automation - Ooredoo/Commands/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1658" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C31C8BF1-AB0D-4134-8579-1FAC35976F7E}"/>
+  <xr:revisionPtr revIDLastSave="1662" documentId="13_ncr:1_{246DA109-2828-4575-BD11-6E355FEF06BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87F7330E-389C-4967-A002-EF4A016F6A97}"/>
   <bookViews>
-    <workbookView xWindow="31425" yWindow="4035" windowWidth="17250" windowHeight="8865" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
+    <workbookView xWindow="31560" yWindow="2745" windowWidth="17250" windowHeight="8865" xr2:uid="{19AA8B23-C0AD-45A4-BDC8-EC244BF91A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="OoredooMasterFile" sheetId="2" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2426" uniqueCount="1078">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2425" uniqueCount="1077">
   <si>
     <t>ICC ID</t>
   </si>
@@ -3395,11 +3395,9 @@
     <t>ZAIN UL ABEDIN</t>
   </si>
   <si>
-    <t>R-1</t>
-  </si>
-  <si>
     <t>PRF # 2813
-31-Jul-2023 @11:48 - Requested to Replacement of Sim Card and Update the new details of new Sim Holder</t>
+31-Jul-2023 @11:48 - Requested to Replacement of Sim Card and Update the new details of new Sim Holder
+16-Aug-2023 @11:25 - Request was Completed with Plan A; Request Completed</t>
   </si>
 </sst>
 </file>
@@ -3537,7 +3535,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3613,12 +3611,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3769,7 +3761,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4193,9 +4185,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5228,9 +5217,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5268,7 +5257,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5374,7 +5363,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5516,7 +5505,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -13524,7 +13513,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="246" spans="1:23" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:23" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A246" s="15">
         <v>45138</v>
       </c>
@@ -13558,11 +13547,11 @@
       <c r="K246" s="16" t="s">
         <v>582</v>
       </c>
-      <c r="L246" s="149" t="s">
+      <c r="L246" s="48">
+        <v>45154</v>
+      </c>
+      <c r="M246" s="99" t="s">
         <v>1076</v>
-      </c>
-      <c r="M246" s="99" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="247" spans="1:23" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>